<commit_message>
Actualización Guion, Escaleta, y mapa conceptual CN_06_03_CO
Actualización Guion, Escaleta, y mapa conceptual CN_06_03_CO
</commit_message>
<xml_diff>
--- a/fuentes/contenidos/grado06/guion03/Escaleta CN_06_03_CO.xlsx
+++ b/fuentes/contenidos/grado06/guion03/Escaleta CN_06_03_CO.xlsx
@@ -16,50 +16,14 @@
     <sheet name="DATOS" sheetId="1" state="hidden" r:id="rId2"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Hoja2!$A$1:$U$2</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Hoja2!$A$2:$U$36</definedName>
   </definedNames>
   <calcPr calcId="152511"/>
 </workbook>
 </file>
 
-<file path=xl/comments1.xml><?xml version="1.0" encoding="utf-8"?>
-<comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <authors>
-    <author>diego m.</author>
-  </authors>
-  <commentList>
-    <comment ref="G19" authorId="0" shapeId="0">
-      <text>
-        <r>
-          <rPr>
-            <b/>
-            <sz val="9"/>
-            <color indexed="81"/>
-            <rFont val="Tahoma"/>
-            <family val="2"/>
-          </rPr>
-          <t>diego m.:</t>
-        </r>
-        <r>
-          <rPr>
-            <sz val="9"/>
-            <color indexed="81"/>
-            <rFont val="Tahoma"/>
-            <family val="2"/>
-          </rPr>
-          <t xml:space="preserve">
-La vida en la tierra, 3 - pg 90
-Bio. Solomon - pg 576
-</t>
-        </r>
-      </text>
-    </comment>
-  </commentList>
-</comments>
-</file>
-
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="665" uniqueCount="246">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="652" uniqueCount="244">
   <si>
     <t>Asignatura</t>
   </si>
@@ -443,9 +407,6 @@
     <t>m101a</t>
   </si>
   <si>
-    <t>Evaluación sobre la composición de los seres vivos</t>
-  </si>
-  <si>
     <t>La función de relación</t>
   </si>
   <si>
@@ -458,9 +419,6 @@
     <t>Refuerza tu aprendizaje: Las funciones de los seres vivos</t>
   </si>
   <si>
-    <t>Evaluación sobre las funciones de los seres vivos</t>
-  </si>
-  <si>
     <t xml:space="preserve">Características de las arqueas </t>
   </si>
   <si>
@@ -497,9 +455,6 @@
     <t>Refuerza tu aprendizaje: La clasificación de los seres vivos</t>
   </si>
   <si>
-    <t>Evaluación sobre la clasificación de los seres vivos</t>
-  </si>
-  <si>
     <t>El dominio Eucaria</t>
   </si>
   <si>
@@ -530,9 +485,6 @@
     <t>Interactivo que permite entender la importancia del agua para la vida</t>
   </si>
   <si>
-    <t>Actividad para seleccionar los elementos básicos que forman parte de un ser vivo</t>
-  </si>
-  <si>
     <t>RM</t>
   </si>
   <si>
@@ -608,9 +560,6 @@
     <t>Recurso M5A-01</t>
   </si>
   <si>
-    <t>Actividad que permite evaluar los conocimientos aprendidos acerca de las funciones de los seres vivos</t>
-  </si>
-  <si>
     <t>Recurso M4A-03</t>
   </si>
   <si>
@@ -713,9 +662,6 @@
     <t>Actividad para identificar y clasificar los seres vivos del dominio Eucaria</t>
   </si>
   <si>
-    <t>Actividad que permite evaluar los conocimientos aprendidos acerca de la clasificación de los seres vivos</t>
-  </si>
-  <si>
     <t>Recurso M101A-02</t>
   </si>
   <si>
@@ -779,18 +725,6 @@
     <t>Evalúa tus conocimientos sobre el tema Los seres vivos</t>
   </si>
   <si>
-    <t>Recursos adicionales 01</t>
-  </si>
-  <si>
-    <t>Recurso M4A-06</t>
-  </si>
-  <si>
-    <t>RF_01_02_CO</t>
-  </si>
-  <si>
-    <t>Banco de actividades: Los seres vivos</t>
-  </si>
-  <si>
     <t>Recurso M101AP-01</t>
   </si>
   <si>
@@ -798,13 +732,37 @@
   </si>
   <si>
     <t>Ver cambios del texto en la ficha en el cuadro del guion</t>
+  </si>
+  <si>
+    <t>Actividad de preguntas sobre la célula</t>
+  </si>
+  <si>
+    <t>Actividad para identificar los elementos básicos que forman parte de un ser vivo</t>
+  </si>
+  <si>
+    <t>Refuerza tu aprendizaje: El dominio Eucaria</t>
+  </si>
+  <si>
+    <t>Actividad sobre la clasificación de los seres vivos</t>
+  </si>
+  <si>
+    <t>Actividad de preguntas que permite evaluar los conocimientos aprendidos acerca de la clasificación de los seres vivos</t>
+  </si>
+  <si>
+    <t>Motor que incluye preguntas de respuesta abierta del tema Los seres vivos</t>
+  </si>
+  <si>
+    <t>Banco de actividades</t>
+  </si>
+  <si>
+    <t>Cambiar en la ficha “Tarea”  la palabra “Cúter” por “bisturí”.</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="6" x14ac:knownFonts="1">
+  <fonts count="5" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -836,17 +794,12 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <sz val="9"/>
-      <color indexed="81"/>
-      <name val="Tahoma"/>
+      <b/>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
       <family val="2"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="9"/>
-      <color indexed="81"/>
-      <name val="Tahoma"/>
-      <family val="2"/>
+      <scheme val="minor"/>
     </font>
   </fonts>
   <fills count="13">
@@ -991,7 +944,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="57">
+  <cellXfs count="58">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
@@ -1063,6 +1016,18 @@
     <xf numFmtId="0" fontId="0" fillId="10" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="12" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="12" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="3" fillId="12" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
@@ -1131,15 +1096,6 @@
     </xf>
     <xf numFmtId="0" fontId="2" fillId="4" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="12" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -1444,12 +1400,12 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:U284"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:U283"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
-      <pane ySplit="2" topLeftCell="A3" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" sqref="A1:A2"/>
+      <pane ySplit="2" topLeftCell="A29" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="A38" sqref="A38"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1477,110 +1433,110 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:21" s="15" customFormat="1" ht="33.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="43" t="s">
+      <c r="A1" s="47" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="41" t="s">
+      <c r="B1" s="45" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="52" t="s">
+      <c r="C1" s="56" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="43" t="s">
+      <c r="D1" s="47" t="s">
         <v>110</v>
       </c>
-      <c r="E1" s="41" t="s">
+      <c r="E1" s="45" t="s">
         <v>111</v>
       </c>
-      <c r="F1" s="39" t="s">
+      <c r="F1" s="43" t="s">
         <v>112</v>
       </c>
-      <c r="G1" s="45" t="s">
+      <c r="G1" s="49" t="s">
         <v>3</v>
       </c>
-      <c r="H1" s="39" t="s">
+      <c r="H1" s="43" t="s">
         <v>113</v>
       </c>
-      <c r="I1" s="39" t="s">
+      <c r="I1" s="43" t="s">
         <v>107</v>
       </c>
-      <c r="J1" s="49" t="s">
+      <c r="J1" s="53" t="s">
         <v>4</v>
       </c>
-      <c r="K1" s="47" t="s">
+      <c r="K1" s="51" t="s">
         <v>108</v>
       </c>
-      <c r="L1" s="45" t="s">
+      <c r="L1" s="49" t="s">
         <v>14</v>
       </c>
-      <c r="M1" s="51" t="s">
+      <c r="M1" s="55" t="s">
         <v>21</v>
       </c>
-      <c r="N1" s="51"/>
-      <c r="O1" s="31" t="s">
+      <c r="N1" s="55"/>
+      <c r="O1" s="35" t="s">
         <v>109</v>
       </c>
-      <c r="P1" s="31" t="s">
+      <c r="P1" s="35" t="s">
         <v>114</v>
       </c>
-      <c r="Q1" s="33" t="s">
+      <c r="Q1" s="37" t="s">
         <v>85</v>
       </c>
-      <c r="R1" s="37" t="s">
+      <c r="R1" s="41" t="s">
         <v>86</v>
       </c>
-      <c r="S1" s="33" t="s">
+      <c r="S1" s="37" t="s">
         <v>87</v>
       </c>
-      <c r="T1" s="35" t="s">
+      <c r="T1" s="39" t="s">
         <v>88</v>
       </c>
-      <c r="U1" s="33" t="s">
+      <c r="U1" s="37" t="s">
         <v>89</v>
       </c>
     </row>
     <row r="2" spans="1:21" s="15" customFormat="1" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A2" s="44"/>
-      <c r="B2" s="42"/>
-      <c r="C2" s="53"/>
-      <c r="D2" s="44"/>
-      <c r="E2" s="42"/>
-      <c r="F2" s="40"/>
-      <c r="G2" s="46"/>
-      <c r="H2" s="40"/>
-      <c r="I2" s="40"/>
-      <c r="J2" s="50"/>
-      <c r="K2" s="48"/>
-      <c r="L2" s="46"/>
+      <c r="A2" s="48"/>
+      <c r="B2" s="46"/>
+      <c r="C2" s="57"/>
+      <c r="D2" s="48"/>
+      <c r="E2" s="46"/>
+      <c r="F2" s="44"/>
+      <c r="G2" s="50"/>
+      <c r="H2" s="44"/>
+      <c r="I2" s="44"/>
+      <c r="J2" s="54"/>
+      <c r="K2" s="52"/>
+      <c r="L2" s="50"/>
       <c r="M2" s="16" t="s">
         <v>90</v>
       </c>
       <c r="N2" s="16" t="s">
         <v>91</v>
       </c>
-      <c r="O2" s="32"/>
-      <c r="P2" s="32"/>
-      <c r="Q2" s="34"/>
-      <c r="R2" s="38"/>
-      <c r="S2" s="34"/>
-      <c r="T2" s="36"/>
-      <c r="U2" s="34"/>
+      <c r="O2" s="36"/>
+      <c r="P2" s="36"/>
+      <c r="Q2" s="38"/>
+      <c r="R2" s="42"/>
+      <c r="S2" s="38"/>
+      <c r="T2" s="40"/>
+      <c r="U2" s="38"/>
     </row>
     <row r="3" spans="1:21" ht="30.75" thickTop="1" x14ac:dyDescent="0.25">
       <c r="A3" s="4" t="s">
         <v>17</v>
       </c>
       <c r="B3" s="12" t="s">
+        <v>148</v>
+      </c>
+      <c r="C3" s="13" t="s">
+        <v>149</v>
+      </c>
+      <c r="D3" s="14" t="s">
+        <v>150</v>
+      </c>
+      <c r="E3" s="12" t="s">
         <v>151</v>
-      </c>
-      <c r="C3" s="13" t="s">
-        <v>152</v>
-      </c>
-      <c r="D3" s="14" t="s">
-        <v>153</v>
-      </c>
-      <c r="E3" s="12" t="s">
-        <v>154</v>
       </c>
       <c r="F3" s="9"/>
       <c r="G3" s="17" t="s">
@@ -1593,7 +1549,7 @@
         <v>19</v>
       </c>
       <c r="J3" s="27" t="s">
-        <v>155</v>
+        <v>152</v>
       </c>
       <c r="K3" s="7" t="s">
         <v>20</v>
@@ -1613,16 +1569,16 @@
         <v>6</v>
       </c>
       <c r="R3" s="11" t="s">
-        <v>157</v>
+        <v>153</v>
       </c>
       <c r="S3" s="30" t="s">
-        <v>158</v>
+        <v>154</v>
       </c>
       <c r="T3" s="29" t="s">
-        <v>159</v>
+        <v>155</v>
       </c>
       <c r="U3" s="10" t="s">
-        <v>160</v>
+        <v>156</v>
       </c>
     </row>
     <row r="4" spans="1:21" ht="30" x14ac:dyDescent="0.25">
@@ -1630,16 +1586,16 @@
         <v>17</v>
       </c>
       <c r="B4" s="12" t="s">
+        <v>148</v>
+      </c>
+      <c r="C4" s="13" t="s">
+        <v>149</v>
+      </c>
+      <c r="D4" s="14" t="s">
+        <v>150</v>
+      </c>
+      <c r="E4" s="12" t="s">
         <v>151</v>
-      </c>
-      <c r="C4" s="13" t="s">
-        <v>152</v>
-      </c>
-      <c r="D4" s="14" t="s">
-        <v>153</v>
-      </c>
-      <c r="E4" s="12" t="s">
-        <v>154</v>
       </c>
       <c r="F4" s="9"/>
       <c r="G4" s="17" t="s">
@@ -1652,7 +1608,7 @@
         <v>20</v>
       </c>
       <c r="J4" s="27" t="s">
-        <v>156</v>
+        <v>237</v>
       </c>
       <c r="K4" s="7" t="s">
         <v>20</v>
@@ -1672,16 +1628,16 @@
         <v>6</v>
       </c>
       <c r="R4" s="11" t="s">
+        <v>153</v>
+      </c>
+      <c r="S4" s="10" t="s">
         <v>157</v>
       </c>
-      <c r="S4" s="10" t="s">
-        <v>161</v>
-      </c>
       <c r="T4" s="29" t="s">
-        <v>162</v>
+        <v>158</v>
       </c>
       <c r="U4" s="10" t="s">
-        <v>163</v>
+        <v>159</v>
       </c>
     </row>
     <row r="5" spans="1:21" ht="30" x14ac:dyDescent="0.25">
@@ -1689,16 +1645,16 @@
         <v>17</v>
       </c>
       <c r="B5" s="12" t="s">
-        <v>151</v>
+        <v>148</v>
       </c>
       <c r="C5" s="13" t="s">
-        <v>152</v>
+        <v>149</v>
       </c>
       <c r="D5" s="14" t="s">
-        <v>153</v>
+        <v>150</v>
       </c>
       <c r="E5" s="12" t="s">
-        <v>164</v>
+        <v>160</v>
       </c>
       <c r="F5" s="9"/>
       <c r="G5" s="17" t="s">
@@ -1711,7 +1667,7 @@
         <v>19</v>
       </c>
       <c r="J5" s="27" t="s">
-        <v>165</v>
+        <v>161</v>
       </c>
       <c r="K5" s="7" t="s">
         <v>19</v>
@@ -1728,40 +1684,40 @@
         <v>19</v>
       </c>
       <c r="Q5" s="10" t="s">
-        <v>170</v>
+        <v>166</v>
       </c>
       <c r="R5" s="11" t="s">
-        <v>171</v>
+        <v>167</v>
       </c>
       <c r="S5" s="10" t="s">
-        <v>152</v>
+        <v>149</v>
       </c>
       <c r="T5" s="29" t="s">
         <v>124</v>
       </c>
       <c r="U5" s="10" t="s">
-        <v>172</v>
-      </c>
-    </row>
-    <row r="6" spans="1:21" ht="30" x14ac:dyDescent="0.25">
+        <v>168</v>
+      </c>
+    </row>
+    <row r="6" spans="1:21" ht="45" x14ac:dyDescent="0.25">
       <c r="A6" s="4" t="s">
         <v>17</v>
       </c>
       <c r="B6" s="12" t="s">
-        <v>151</v>
+        <v>148</v>
       </c>
       <c r="C6" s="13" t="s">
-        <v>152</v>
+        <v>149</v>
       </c>
       <c r="D6" s="14" t="s">
-        <v>153</v>
+        <v>150</v>
       </c>
       <c r="E6" s="12" t="s">
-        <v>166</v>
+        <v>160</v>
       </c>
       <c r="F6" s="9"/>
       <c r="G6" s="17" t="s">
-        <v>125</v>
+        <v>236</v>
       </c>
       <c r="H6" s="18">
         <v>4</v>
@@ -1770,7 +1726,7 @@
         <v>20</v>
       </c>
       <c r="J6" s="27" t="s">
-        <v>167</v>
+        <v>169</v>
       </c>
       <c r="K6" s="7" t="s">
         <v>20</v>
@@ -1780,47 +1736,47 @@
       </c>
       <c r="M6" s="8"/>
       <c r="N6" s="8" t="s">
-        <v>126</v>
+        <v>32</v>
       </c>
       <c r="O6" s="9"/>
-      <c r="P6" s="18" t="s">
-        <v>19</v>
+      <c r="P6" s="34" t="s">
+        <v>20</v>
       </c>
       <c r="Q6" s="10">
         <v>6</v>
       </c>
       <c r="R6" s="11" t="s">
+        <v>153</v>
+      </c>
+      <c r="S6" s="10" t="s">
         <v>157</v>
       </c>
-      <c r="S6" s="10" t="s">
-        <v>161</v>
-      </c>
       <c r="T6" s="29" t="s">
-        <v>168</v>
+        <v>165</v>
       </c>
       <c r="U6" s="10" t="s">
-        <v>163</v>
-      </c>
-    </row>
-    <row r="7" spans="1:21" ht="45" x14ac:dyDescent="0.25">
+        <v>159</v>
+      </c>
+    </row>
+    <row r="7" spans="1:21" ht="30" x14ac:dyDescent="0.25">
       <c r="A7" s="4" t="s">
         <v>17</v>
       </c>
       <c r="B7" s="12" t="s">
-        <v>151</v>
+        <v>148</v>
       </c>
       <c r="C7" s="13" t="s">
-        <v>152</v>
+        <v>149</v>
       </c>
       <c r="D7" s="14" t="s">
-        <v>153</v>
+        <v>150</v>
       </c>
       <c r="E7" s="12" t="s">
-        <v>166</v>
+        <v>162</v>
       </c>
       <c r="F7" s="9"/>
       <c r="G7" s="17" t="s">
-        <v>127</v>
+        <v>125</v>
       </c>
       <c r="H7" s="18">
         <v>5</v>
@@ -1829,7 +1785,7 @@
         <v>20</v>
       </c>
       <c r="J7" s="27" t="s">
-        <v>173</v>
+        <v>163</v>
       </c>
       <c r="K7" s="7" t="s">
         <v>20</v>
@@ -1839,26 +1795,26 @@
       </c>
       <c r="M7" s="8"/>
       <c r="N7" s="8" t="s">
-        <v>32</v>
+        <v>126</v>
       </c>
       <c r="O7" s="9"/>
       <c r="P7" s="18" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="Q7" s="10">
         <v>6</v>
       </c>
       <c r="R7" s="11" t="s">
+        <v>153</v>
+      </c>
+      <c r="S7" s="10" t="s">
         <v>157</v>
       </c>
-      <c r="S7" s="10" t="s">
-        <v>161</v>
-      </c>
       <c r="T7" s="29" t="s">
-        <v>169</v>
+        <v>164</v>
       </c>
       <c r="U7" s="10" t="s">
-        <v>163</v>
+        <v>159</v>
       </c>
     </row>
     <row r="8" spans="1:21" ht="15.75" x14ac:dyDescent="0.25">
@@ -1866,16 +1822,16 @@
         <v>17</v>
       </c>
       <c r="B8" s="12" t="s">
-        <v>151</v>
+        <v>148</v>
       </c>
       <c r="C8" s="13" t="s">
-        <v>152</v>
+        <v>149</v>
       </c>
       <c r="D8" s="14" t="s">
-        <v>174</v>
+        <v>170</v>
       </c>
       <c r="E8" s="12" t="s">
-        <v>175</v>
+        <v>171</v>
       </c>
       <c r="F8" s="9"/>
       <c r="G8" s="20"/>
@@ -1899,16 +1855,16 @@
         <v>17</v>
       </c>
       <c r="B9" s="12" t="s">
-        <v>151</v>
+        <v>148</v>
       </c>
       <c r="C9" s="13" t="s">
-        <v>152</v>
+        <v>149</v>
       </c>
       <c r="D9" s="14" t="s">
-        <v>174</v>
+        <v>170</v>
       </c>
       <c r="E9" s="12" t="s">
-        <v>176</v>
+        <v>172</v>
       </c>
       <c r="F9" s="9"/>
       <c r="G9" s="17"/>
@@ -1932,20 +1888,20 @@
         <v>17</v>
       </c>
       <c r="B10" s="12" t="s">
-        <v>151</v>
+        <v>148</v>
       </c>
       <c r="C10" s="13" t="s">
-        <v>152</v>
+        <v>149</v>
       </c>
       <c r="D10" s="14" t="s">
-        <v>174</v>
+        <v>170</v>
       </c>
       <c r="E10" s="12" t="s">
-        <v>177</v>
+        <v>173</v>
       </c>
       <c r="F10" s="9"/>
       <c r="G10" s="20" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
       <c r="H10" s="21">
         <v>6</v>
@@ -1954,7 +1910,7 @@
         <v>19</v>
       </c>
       <c r="J10" s="28" t="s">
-        <v>178</v>
+        <v>174</v>
       </c>
       <c r="K10" s="23" t="s">
         <v>19</v>
@@ -1966,26 +1922,26 @@
         <v>62</v>
       </c>
       <c r="N10" s="25"/>
-      <c r="O10" s="56" t="s">
-        <v>245</v>
+      <c r="O10" s="33" t="s">
+        <v>235</v>
       </c>
       <c r="P10" s="21" t="s">
         <v>19</v>
       </c>
       <c r="Q10" s="10" t="s">
-        <v>170</v>
+        <v>166</v>
       </c>
       <c r="R10" s="11" t="s">
-        <v>171</v>
+        <v>167</v>
       </c>
       <c r="S10" s="10" t="s">
-        <v>152</v>
+        <v>149</v>
       </c>
       <c r="T10" s="29" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
       <c r="U10" s="10" t="s">
-        <v>172</v>
+        <v>168</v>
       </c>
     </row>
     <row r="11" spans="1:21" ht="30" x14ac:dyDescent="0.25">
@@ -1993,20 +1949,20 @@
         <v>17</v>
       </c>
       <c r="B11" s="12" t="s">
-        <v>151</v>
+        <v>148</v>
       </c>
       <c r="C11" s="13" t="s">
-        <v>152</v>
+        <v>149</v>
       </c>
       <c r="D11" s="14" t="s">
-        <v>174</v>
+        <v>170</v>
       </c>
       <c r="E11" s="12" t="s">
-        <v>177</v>
+        <v>173</v>
       </c>
       <c r="F11" s="9"/>
       <c r="G11" s="17" t="s">
-        <v>129</v>
+        <v>128</v>
       </c>
       <c r="H11" s="18">
         <v>7</v>
@@ -2015,7 +1971,7 @@
         <v>20</v>
       </c>
       <c r="J11" s="27" t="s">
-        <v>179</v>
+        <v>175</v>
       </c>
       <c r="K11" s="7" t="s">
         <v>19</v>
@@ -2032,19 +1988,19 @@
         <v>19</v>
       </c>
       <c r="Q11" s="10" t="s">
-        <v>170</v>
+        <v>166</v>
       </c>
       <c r="R11" s="11" t="s">
-        <v>171</v>
+        <v>167</v>
       </c>
       <c r="S11" s="10" t="s">
-        <v>152</v>
+        <v>149</v>
       </c>
       <c r="T11" s="29" t="s">
-        <v>129</v>
+        <v>128</v>
       </c>
       <c r="U11" s="10" t="s">
-        <v>172</v>
+        <v>168</v>
       </c>
     </row>
     <row r="12" spans="1:21" ht="30" x14ac:dyDescent="0.25">
@@ -2052,20 +2008,20 @@
         <v>17</v>
       </c>
       <c r="B12" s="12" t="s">
-        <v>151</v>
+        <v>148</v>
       </c>
       <c r="C12" s="13" t="s">
-        <v>152</v>
+        <v>149</v>
       </c>
       <c r="D12" s="14" t="s">
-        <v>174</v>
+        <v>170</v>
       </c>
       <c r="E12" s="12" t="s">
-        <v>177</v>
+        <v>173</v>
       </c>
       <c r="F12" s="9"/>
       <c r="G12" s="17" t="s">
-        <v>130</v>
+        <v>129</v>
       </c>
       <c r="H12" s="18">
         <v>8</v>
@@ -2074,7 +2030,7 @@
         <v>20</v>
       </c>
       <c r="J12" s="27" t="s">
-        <v>180</v>
+        <v>176</v>
       </c>
       <c r="K12" s="7" t="s">
         <v>20</v>
@@ -2094,16 +2050,16 @@
         <v>6</v>
       </c>
       <c r="R12" s="11" t="s">
+        <v>153</v>
+      </c>
+      <c r="S12" s="10" t="s">
         <v>157</v>
       </c>
-      <c r="S12" s="10" t="s">
-        <v>161</v>
-      </c>
       <c r="T12" s="29" t="s">
-        <v>181</v>
+        <v>177</v>
       </c>
       <c r="U12" s="10" t="s">
-        <v>163</v>
+        <v>159</v>
       </c>
     </row>
     <row r="13" spans="1:21" ht="30" x14ac:dyDescent="0.25">
@@ -2111,20 +2067,20 @@
         <v>17</v>
       </c>
       <c r="B13" s="12" t="s">
-        <v>151</v>
+        <v>148</v>
       </c>
       <c r="C13" s="13" t="s">
-        <v>152</v>
+        <v>149</v>
       </c>
       <c r="D13" s="14" t="s">
-        <v>174</v>
+        <v>170</v>
       </c>
       <c r="E13" s="12" t="s">
-        <v>166</v>
+        <v>162</v>
       </c>
       <c r="F13" s="9"/>
       <c r="G13" s="17" t="s">
-        <v>131</v>
+        <v>130</v>
       </c>
       <c r="H13" s="18">
         <v>9</v>
@@ -2133,7 +2089,7 @@
         <v>20</v>
       </c>
       <c r="J13" s="27" t="s">
-        <v>179</v>
+        <v>175</v>
       </c>
       <c r="K13" s="7" t="s">
         <v>19</v>
@@ -2150,78 +2106,78 @@
         <v>19</v>
       </c>
       <c r="Q13" s="10" t="s">
-        <v>170</v>
+        <v>166</v>
       </c>
       <c r="R13" s="11" t="s">
-        <v>171</v>
+        <v>167</v>
       </c>
       <c r="S13" s="10" t="s">
-        <v>152</v>
+        <v>149</v>
       </c>
       <c r="T13" s="29" t="s">
-        <v>131</v>
+        <v>130</v>
       </c>
       <c r="U13" s="10" t="s">
-        <v>172</v>
-      </c>
-    </row>
-    <row r="14" spans="1:21" ht="45" x14ac:dyDescent="0.25">
+        <v>168</v>
+      </c>
+    </row>
+    <row r="14" spans="1:21" ht="30" x14ac:dyDescent="0.25">
       <c r="A14" s="4" t="s">
         <v>17</v>
       </c>
       <c r="B14" s="12" t="s">
-        <v>151</v>
+        <v>148</v>
       </c>
       <c r="C14" s="13" t="s">
-        <v>152</v>
+        <v>149</v>
       </c>
       <c r="D14" s="14" t="s">
-        <v>174</v>
+        <v>179</v>
       </c>
       <c r="E14" s="12" t="s">
-        <v>166</v>
+        <v>180</v>
       </c>
       <c r="F14" s="9"/>
-      <c r="G14" s="17" t="s">
-        <v>132</v>
-      </c>
-      <c r="H14" s="18">
+      <c r="G14" s="20" t="s">
+        <v>131</v>
+      </c>
+      <c r="H14" s="21">
         <v>10</v>
       </c>
-      <c r="I14" s="5" t="s">
+      <c r="I14" s="22" t="s">
         <v>20</v>
       </c>
-      <c r="J14" s="27" t="s">
-        <v>182</v>
-      </c>
-      <c r="K14" s="7" t="s">
+      <c r="J14" s="28" t="s">
+        <v>181</v>
+      </c>
+      <c r="K14" s="23" t="s">
         <v>20</v>
       </c>
-      <c r="L14" s="6" t="s">
+      <c r="L14" s="24" t="s">
         <v>8</v>
       </c>
-      <c r="M14" s="8"/>
-      <c r="N14" s="8" t="s">
-        <v>32</v>
-      </c>
-      <c r="O14" s="9"/>
-      <c r="P14" s="18" t="s">
-        <v>20</v>
+      <c r="M14" s="25"/>
+      <c r="N14" s="25" t="s">
+        <v>28</v>
+      </c>
+      <c r="O14" s="26"/>
+      <c r="P14" s="21" t="s">
+        <v>19</v>
       </c>
       <c r="Q14" s="10">
         <v>6</v>
       </c>
       <c r="R14" s="11" t="s">
+        <v>153</v>
+      </c>
+      <c r="S14" s="10" t="s">
         <v>157</v>
       </c>
-      <c r="S14" s="10" t="s">
-        <v>161</v>
-      </c>
       <c r="T14" s="29" t="s">
-        <v>183</v>
+        <v>182</v>
       </c>
       <c r="U14" s="10" t="s">
-        <v>163</v>
+        <v>159</v>
       </c>
     </row>
     <row r="15" spans="1:21" ht="30" x14ac:dyDescent="0.25">
@@ -2229,58 +2185,58 @@
         <v>17</v>
       </c>
       <c r="B15" s="12" t="s">
-        <v>151</v>
+        <v>148</v>
       </c>
       <c r="C15" s="13" t="s">
-        <v>152</v>
+        <v>149</v>
       </c>
       <c r="D15" s="14" t="s">
+        <v>179</v>
+      </c>
+      <c r="E15" s="12" t="s">
+        <v>183</v>
+      </c>
+      <c r="F15" s="9"/>
+      <c r="G15" s="17" t="s">
+        <v>132</v>
+      </c>
+      <c r="H15" s="18">
+        <v>11</v>
+      </c>
+      <c r="I15" s="5" t="s">
+        <v>19</v>
+      </c>
+      <c r="J15" s="27" t="s">
         <v>184</v>
       </c>
-      <c r="E15" s="12" t="s">
-        <v>185</v>
-      </c>
-      <c r="F15" s="9"/>
-      <c r="G15" s="20" t="s">
-        <v>133</v>
-      </c>
-      <c r="H15" s="21">
-        <v>11</v>
-      </c>
-      <c r="I15" s="22" t="s">
+      <c r="K15" s="7" t="s">
         <v>20</v>
       </c>
-      <c r="J15" s="28" t="s">
-        <v>186</v>
-      </c>
-      <c r="K15" s="23" t="s">
-        <v>20</v>
-      </c>
-      <c r="L15" s="24" t="s">
-        <v>8</v>
-      </c>
-      <c r="M15" s="25"/>
-      <c r="N15" s="25" t="s">
-        <v>28</v>
-      </c>
-      <c r="O15" s="26"/>
-      <c r="P15" s="21" t="s">
+      <c r="L15" s="6" t="s">
+        <v>5</v>
+      </c>
+      <c r="M15" s="8" t="s">
+        <v>58</v>
+      </c>
+      <c r="N15" s="8"/>
+      <c r="O15" s="9"/>
+      <c r="P15" s="18" t="s">
         <v>19</v>
       </c>
       <c r="Q15" s="10">
         <v>6</v>
       </c>
       <c r="R15" s="11" t="s">
-        <v>157</v>
+        <v>185</v>
       </c>
       <c r="S15" s="10" t="s">
-        <v>161</v>
+        <v>186</v>
       </c>
       <c r="T15" s="29" t="s">
         <v>187</v>
       </c>
       <c r="U15" s="10" t="s">
-        <v>163</v>
+        <v>188</v>
       </c>
     </row>
     <row r="16" spans="1:21" ht="30" x14ac:dyDescent="0.25">
@@ -2288,26 +2244,26 @@
         <v>17</v>
       </c>
       <c r="B16" s="12" t="s">
-        <v>151</v>
+        <v>148</v>
       </c>
       <c r="C16" s="13" t="s">
-        <v>152</v>
+        <v>149</v>
       </c>
       <c r="D16" s="14" t="s">
-        <v>184</v>
+        <v>179</v>
       </c>
       <c r="E16" s="12" t="s">
-        <v>188</v>
+        <v>183</v>
       </c>
       <c r="F16" s="9"/>
       <c r="G16" s="17" t="s">
-        <v>134</v>
+        <v>133</v>
       </c>
       <c r="H16" s="18">
         <v>12</v>
       </c>
       <c r="I16" s="5" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="J16" s="27" t="s">
         <v>189</v>
@@ -2316,12 +2272,12 @@
         <v>20</v>
       </c>
       <c r="L16" s="6" t="s">
-        <v>5</v>
-      </c>
-      <c r="M16" s="8" t="s">
-        <v>58</v>
-      </c>
-      <c r="N16" s="8"/>
+        <v>8</v>
+      </c>
+      <c r="M16" s="8"/>
+      <c r="N16" s="8" t="s">
+        <v>27</v>
+      </c>
       <c r="O16" s="9"/>
       <c r="P16" s="18" t="s">
         <v>19</v>
@@ -2330,16 +2286,16 @@
         <v>6</v>
       </c>
       <c r="R16" s="11" t="s">
+        <v>153</v>
+      </c>
+      <c r="S16" s="10" t="s">
+        <v>157</v>
+      </c>
+      <c r="T16" s="29" t="s">
         <v>190</v>
       </c>
-      <c r="S16" s="10" t="s">
-        <v>191</v>
-      </c>
-      <c r="T16" s="29" t="s">
-        <v>192</v>
-      </c>
       <c r="U16" s="10" t="s">
-        <v>193</v>
+        <v>159</v>
       </c>
     </row>
     <row r="17" spans="1:21" ht="30" x14ac:dyDescent="0.25">
@@ -2347,20 +2303,20 @@
         <v>17</v>
       </c>
       <c r="B17" s="12" t="s">
-        <v>151</v>
+        <v>148</v>
       </c>
       <c r="C17" s="13" t="s">
-        <v>152</v>
+        <v>149</v>
       </c>
       <c r="D17" s="14" t="s">
-        <v>184</v>
+        <v>179</v>
       </c>
       <c r="E17" s="12" t="s">
-        <v>188</v>
+        <v>183</v>
       </c>
       <c r="F17" s="9"/>
       <c r="G17" s="17" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
       <c r="H17" s="18">
         <v>13</v>
@@ -2369,7 +2325,7 @@
         <v>20</v>
       </c>
       <c r="J17" s="27" t="s">
-        <v>194</v>
+        <v>191</v>
       </c>
       <c r="K17" s="7" t="s">
         <v>20</v>
@@ -2379,7 +2335,7 @@
       </c>
       <c r="M17" s="8"/>
       <c r="N17" s="8" t="s">
-        <v>27</v>
+        <v>119</v>
       </c>
       <c r="O17" s="9"/>
       <c r="P17" s="18" t="s">
@@ -2389,16 +2345,16 @@
         <v>6</v>
       </c>
       <c r="R17" s="11" t="s">
+        <v>153</v>
+      </c>
+      <c r="S17" s="10" t="s">
         <v>157</v>
       </c>
-      <c r="S17" s="10" t="s">
-        <v>161</v>
-      </c>
       <c r="T17" s="29" t="s">
-        <v>195</v>
+        <v>192</v>
       </c>
       <c r="U17" s="10" t="s">
-        <v>163</v>
+        <v>159</v>
       </c>
     </row>
     <row r="18" spans="1:21" ht="30" x14ac:dyDescent="0.25">
@@ -2406,40 +2362,42 @@
         <v>17</v>
       </c>
       <c r="B18" s="12" t="s">
-        <v>151</v>
+        <v>148</v>
       </c>
       <c r="C18" s="13" t="s">
-        <v>152</v>
+        <v>149</v>
       </c>
       <c r="D18" s="14" t="s">
-        <v>184</v>
+        <v>179</v>
       </c>
       <c r="E18" s="12" t="s">
-        <v>188</v>
-      </c>
-      <c r="F18" s="9"/>
+        <v>143</v>
+      </c>
+      <c r="F18" s="9" t="s">
+        <v>193</v>
+      </c>
       <c r="G18" s="17" t="s">
-        <v>136</v>
+        <v>135</v>
       </c>
       <c r="H18" s="18">
         <v>14</v>
       </c>
       <c r="I18" s="5" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="J18" s="27" t="s">
-        <v>196</v>
+        <v>194</v>
       </c>
       <c r="K18" s="7" t="s">
         <v>20</v>
       </c>
       <c r="L18" s="6" t="s">
-        <v>8</v>
-      </c>
-      <c r="M18" s="8"/>
-      <c r="N18" s="8" t="s">
-        <v>119</v>
-      </c>
+        <v>5</v>
+      </c>
+      <c r="M18" s="8" t="s">
+        <v>54</v>
+      </c>
+      <c r="N18" s="8"/>
       <c r="O18" s="9"/>
       <c r="P18" s="18" t="s">
         <v>19</v>
@@ -2448,16 +2406,16 @@
         <v>6</v>
       </c>
       <c r="R18" s="11" t="s">
-        <v>157</v>
+        <v>185</v>
       </c>
       <c r="S18" s="10" t="s">
-        <v>161</v>
+        <v>186</v>
       </c>
       <c r="T18" s="29" t="s">
-        <v>197</v>
+        <v>195</v>
       </c>
       <c r="U18" s="10" t="s">
-        <v>163</v>
+        <v>188</v>
       </c>
     </row>
     <row r="19" spans="1:21" ht="30" x14ac:dyDescent="0.25">
@@ -2465,42 +2423,42 @@
         <v>17</v>
       </c>
       <c r="B19" s="12" t="s">
-        <v>151</v>
+        <v>148</v>
       </c>
       <c r="C19" s="13" t="s">
-        <v>152</v>
+        <v>149</v>
       </c>
       <c r="D19" s="14" t="s">
-        <v>184</v>
+        <v>179</v>
       </c>
       <c r="E19" s="12" t="s">
-        <v>146</v>
+        <v>143</v>
       </c>
       <c r="F19" s="9" t="s">
-        <v>198</v>
+        <v>193</v>
       </c>
       <c r="G19" s="17" t="s">
-        <v>137</v>
+        <v>136</v>
       </c>
       <c r="H19" s="18">
         <v>15</v>
       </c>
       <c r="I19" s="5" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="J19" s="27" t="s">
-        <v>199</v>
+        <v>196</v>
       </c>
       <c r="K19" s="7" t="s">
         <v>20</v>
       </c>
       <c r="L19" s="6" t="s">
-        <v>5</v>
-      </c>
-      <c r="M19" s="8" t="s">
-        <v>54</v>
-      </c>
-      <c r="N19" s="8"/>
+        <v>8</v>
+      </c>
+      <c r="M19" s="8"/>
+      <c r="N19" s="8" t="s">
+        <v>27</v>
+      </c>
       <c r="O19" s="9"/>
       <c r="P19" s="18" t="s">
         <v>19</v>
@@ -2509,16 +2467,16 @@
         <v>6</v>
       </c>
       <c r="R19" s="11" t="s">
-        <v>190</v>
+        <v>153</v>
       </c>
       <c r="S19" s="10" t="s">
-        <v>191</v>
+        <v>157</v>
       </c>
       <c r="T19" s="29" t="s">
-        <v>200</v>
+        <v>197</v>
       </c>
       <c r="U19" s="10" t="s">
-        <v>193</v>
+        <v>159</v>
       </c>
     </row>
     <row r="20" spans="1:21" ht="30" x14ac:dyDescent="0.25">
@@ -2526,22 +2484,22 @@
         <v>17</v>
       </c>
       <c r="B20" s="12" t="s">
-        <v>151</v>
+        <v>148</v>
       </c>
       <c r="C20" s="13" t="s">
-        <v>152</v>
+        <v>149</v>
       </c>
       <c r="D20" s="14" t="s">
-        <v>184</v>
+        <v>179</v>
       </c>
       <c r="E20" s="12" t="s">
-        <v>146</v>
+        <v>143</v>
       </c>
       <c r="F20" s="9" t="s">
-        <v>198</v>
+        <v>201</v>
       </c>
       <c r="G20" s="17" t="s">
-        <v>138</v>
+        <v>137</v>
       </c>
       <c r="H20" s="18">
         <v>16</v>
@@ -2550,7 +2508,7 @@
         <v>20</v>
       </c>
       <c r="J20" s="27" t="s">
-        <v>201</v>
+        <v>198</v>
       </c>
       <c r="K20" s="7" t="s">
         <v>20</v>
@@ -2560,7 +2518,7 @@
       </c>
       <c r="M20" s="8"/>
       <c r="N20" s="8" t="s">
-        <v>27</v>
+        <v>119</v>
       </c>
       <c r="O20" s="9"/>
       <c r="P20" s="18" t="s">
@@ -2570,16 +2528,16 @@
         <v>6</v>
       </c>
       <c r="R20" s="11" t="s">
+        <v>153</v>
+      </c>
+      <c r="S20" s="10" t="s">
         <v>157</v>
       </c>
-      <c r="S20" s="10" t="s">
-        <v>161</v>
-      </c>
       <c r="T20" s="29" t="s">
-        <v>202</v>
+        <v>199</v>
       </c>
       <c r="U20" s="10" t="s">
-        <v>163</v>
+        <v>159</v>
       </c>
     </row>
     <row r="21" spans="1:21" ht="30" x14ac:dyDescent="0.25">
@@ -2587,22 +2545,22 @@
         <v>17</v>
       </c>
       <c r="B21" s="12" t="s">
-        <v>151</v>
+        <v>148</v>
       </c>
       <c r="C21" s="13" t="s">
-        <v>152</v>
+        <v>149</v>
       </c>
       <c r="D21" s="14" t="s">
-        <v>184</v>
+        <v>179</v>
       </c>
       <c r="E21" s="12" t="s">
-        <v>146</v>
+        <v>143</v>
       </c>
       <c r="F21" s="9" t="s">
-        <v>206</v>
+        <v>200</v>
       </c>
       <c r="G21" s="17" t="s">
-        <v>139</v>
+        <v>138</v>
       </c>
       <c r="H21" s="18">
         <v>17</v>
@@ -2611,7 +2569,7 @@
         <v>20</v>
       </c>
       <c r="J21" s="27" t="s">
-        <v>203</v>
+        <v>202</v>
       </c>
       <c r="K21" s="7" t="s">
         <v>20</v>
@@ -2621,7 +2579,7 @@
       </c>
       <c r="M21" s="8"/>
       <c r="N21" s="8" t="s">
-        <v>119</v>
+        <v>32</v>
       </c>
       <c r="O21" s="9"/>
       <c r="P21" s="18" t="s">
@@ -2631,16 +2589,16 @@
         <v>6</v>
       </c>
       <c r="R21" s="11" t="s">
+        <v>153</v>
+      </c>
+      <c r="S21" s="10" t="s">
         <v>157</v>
       </c>
-      <c r="S21" s="10" t="s">
-        <v>161</v>
-      </c>
       <c r="T21" s="29" t="s">
-        <v>204</v>
+        <v>178</v>
       </c>
       <c r="U21" s="10" t="s">
-        <v>163</v>
+        <v>159</v>
       </c>
     </row>
     <row r="22" spans="1:21" ht="30" x14ac:dyDescent="0.25">
@@ -2648,22 +2606,22 @@
         <v>17</v>
       </c>
       <c r="B22" s="12" t="s">
-        <v>151</v>
+        <v>148</v>
       </c>
       <c r="C22" s="13" t="s">
-        <v>152</v>
+        <v>149</v>
       </c>
       <c r="D22" s="14" t="s">
-        <v>184</v>
+        <v>179</v>
       </c>
       <c r="E22" s="12" t="s">
-        <v>146</v>
+        <v>143</v>
       </c>
       <c r="F22" s="9" t="s">
-        <v>205</v>
+        <v>200</v>
       </c>
       <c r="G22" s="17" t="s">
-        <v>140</v>
+        <v>139</v>
       </c>
       <c r="H22" s="18">
         <v>18</v>
@@ -2672,7 +2630,7 @@
         <v>20</v>
       </c>
       <c r="J22" s="27" t="s">
-        <v>207</v>
+        <v>203</v>
       </c>
       <c r="K22" s="7" t="s">
         <v>20</v>
@@ -2682,7 +2640,7 @@
       </c>
       <c r="M22" s="8"/>
       <c r="N22" s="8" t="s">
-        <v>32</v>
+        <v>118</v>
       </c>
       <c r="O22" s="9"/>
       <c r="P22" s="18" t="s">
@@ -2692,161 +2650,161 @@
         <v>6</v>
       </c>
       <c r="R22" s="11" t="s">
+        <v>153</v>
+      </c>
+      <c r="S22" s="10" t="s">
         <v>157</v>
       </c>
-      <c r="S22" s="10" t="s">
-        <v>161</v>
-      </c>
       <c r="T22" s="29" t="s">
-        <v>209</v>
+        <v>205</v>
       </c>
       <c r="U22" s="10" t="s">
-        <v>163</v>
-      </c>
-    </row>
-    <row r="23" spans="1:21" ht="30" x14ac:dyDescent="0.25">
+        <v>159</v>
+      </c>
+    </row>
+    <row r="23" spans="1:21" ht="45" x14ac:dyDescent="0.25">
       <c r="A23" s="4" t="s">
         <v>17</v>
       </c>
       <c r="B23" s="12" t="s">
-        <v>151</v>
+        <v>148</v>
       </c>
       <c r="C23" s="13" t="s">
-        <v>152</v>
+        <v>149</v>
       </c>
       <c r="D23" s="14" t="s">
-        <v>184</v>
+        <v>179</v>
       </c>
       <c r="E23" s="12" t="s">
-        <v>146</v>
+        <v>143</v>
       </c>
       <c r="F23" s="9" t="s">
-        <v>205</v>
+        <v>206</v>
       </c>
       <c r="G23" s="17" t="s">
-        <v>141</v>
+        <v>140</v>
       </c>
       <c r="H23" s="18">
         <v>19</v>
       </c>
       <c r="I23" s="5" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="J23" s="27" t="s">
-        <v>208</v>
+        <v>207</v>
       </c>
       <c r="K23" s="7" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="L23" s="6" t="s">
-        <v>8</v>
-      </c>
-      <c r="M23" s="8"/>
-      <c r="N23" s="8" t="s">
-        <v>118</v>
-      </c>
+        <v>5</v>
+      </c>
+      <c r="M23" s="8" t="s">
+        <v>62</v>
+      </c>
+      <c r="N23" s="8"/>
       <c r="O23" s="9"/>
       <c r="P23" s="18" t="s">
         <v>19</v>
       </c>
-      <c r="Q23" s="10">
-        <v>6</v>
+      <c r="Q23" s="10" t="s">
+        <v>166</v>
       </c>
       <c r="R23" s="11" t="s">
-        <v>157</v>
+        <v>167</v>
       </c>
       <c r="S23" s="10" t="s">
-        <v>161</v>
+        <v>149</v>
       </c>
       <c r="T23" s="29" t="s">
-        <v>210</v>
+        <v>140</v>
       </c>
       <c r="U23" s="10" t="s">
-        <v>163</v>
-      </c>
-    </row>
-    <row r="24" spans="1:21" ht="45" x14ac:dyDescent="0.25">
+        <v>168</v>
+      </c>
+    </row>
+    <row r="24" spans="1:21" ht="30" x14ac:dyDescent="0.25">
       <c r="A24" s="4" t="s">
         <v>17</v>
       </c>
       <c r="B24" s="12" t="s">
-        <v>151</v>
+        <v>148</v>
       </c>
       <c r="C24" s="13" t="s">
-        <v>152</v>
+        <v>149</v>
       </c>
       <c r="D24" s="14" t="s">
-        <v>184</v>
+        <v>179</v>
       </c>
       <c r="E24" s="12" t="s">
-        <v>146</v>
+        <v>143</v>
       </c>
       <c r="F24" s="9" t="s">
-        <v>211</v>
+        <v>206</v>
       </c>
       <c r="G24" s="17" t="s">
-        <v>142</v>
+        <v>141</v>
       </c>
       <c r="H24" s="18">
         <v>20</v>
       </c>
       <c r="I24" s="5" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="J24" s="27" t="s">
-        <v>212</v>
+        <v>208</v>
       </c>
       <c r="K24" s="7" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="L24" s="6" t="s">
-        <v>5</v>
-      </c>
-      <c r="M24" s="8" t="s">
-        <v>62</v>
-      </c>
-      <c r="N24" s="8"/>
+        <v>8</v>
+      </c>
+      <c r="M24" s="8"/>
+      <c r="N24" s="8" t="s">
+        <v>33</v>
+      </c>
       <c r="O24" s="9"/>
       <c r="P24" s="18" t="s">
         <v>19</v>
       </c>
-      <c r="Q24" s="10" t="s">
-        <v>170</v>
+      <c r="Q24" s="10">
+        <v>6</v>
       </c>
       <c r="R24" s="11" t="s">
-        <v>171</v>
+        <v>153</v>
       </c>
       <c r="S24" s="10" t="s">
-        <v>152</v>
+        <v>157</v>
       </c>
       <c r="T24" s="29" t="s">
-        <v>142</v>
+        <v>209</v>
       </c>
       <c r="U24" s="10" t="s">
-        <v>172</v>
-      </c>
-    </row>
-    <row r="25" spans="1:21" ht="30" x14ac:dyDescent="0.25">
+        <v>159</v>
+      </c>
+    </row>
+    <row r="25" spans="1:21" ht="45" x14ac:dyDescent="0.25">
       <c r="A25" s="4" t="s">
         <v>17</v>
       </c>
       <c r="B25" s="12" t="s">
-        <v>151</v>
+        <v>148</v>
       </c>
       <c r="C25" s="13" t="s">
-        <v>152</v>
+        <v>149</v>
       </c>
       <c r="D25" s="14" t="s">
-        <v>184</v>
+        <v>179</v>
       </c>
       <c r="E25" s="12" t="s">
-        <v>146</v>
+        <v>143</v>
       </c>
       <c r="F25" s="9" t="s">
-        <v>211</v>
+        <v>206</v>
       </c>
       <c r="G25" s="17" t="s">
-        <v>143</v>
+        <v>239</v>
       </c>
       <c r="H25" s="18">
         <v>21</v>
@@ -2855,7 +2813,7 @@
         <v>20</v>
       </c>
       <c r="J25" s="27" t="s">
-        <v>213</v>
+        <v>240</v>
       </c>
       <c r="K25" s="7" t="s">
         <v>20</v>
@@ -2865,26 +2823,26 @@
       </c>
       <c r="M25" s="8"/>
       <c r="N25" s="8" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="O25" s="9"/>
-      <c r="P25" s="18" t="s">
-        <v>19</v>
+      <c r="P25" s="34" t="s">
+        <v>20</v>
       </c>
       <c r="Q25" s="10">
         <v>6</v>
       </c>
       <c r="R25" s="11" t="s">
+        <v>153</v>
+      </c>
+      <c r="S25" s="10" t="s">
         <v>157</v>
       </c>
-      <c r="S25" s="10" t="s">
-        <v>161</v>
-      </c>
       <c r="T25" s="29" t="s">
-        <v>214</v>
+        <v>204</v>
       </c>
       <c r="U25" s="10" t="s">
-        <v>163</v>
+        <v>159</v>
       </c>
     </row>
     <row r="26" spans="1:21" ht="30" x14ac:dyDescent="0.25">
@@ -2892,20 +2850,20 @@
         <v>17</v>
       </c>
       <c r="B26" s="12" t="s">
-        <v>151</v>
+        <v>148</v>
       </c>
       <c r="C26" s="13" t="s">
-        <v>152</v>
+        <v>149</v>
       </c>
       <c r="D26" s="14" t="s">
-        <v>184</v>
+        <v>179</v>
       </c>
       <c r="E26" s="12" t="s">
-        <v>166</v>
+        <v>162</v>
       </c>
       <c r="F26" s="9"/>
       <c r="G26" s="17" t="s">
-        <v>144</v>
+        <v>142</v>
       </c>
       <c r="H26" s="18">
         <v>22</v>
@@ -2914,7 +2872,7 @@
         <v>20</v>
       </c>
       <c r="J26" s="27" t="s">
-        <v>215</v>
+        <v>210</v>
       </c>
       <c r="K26" s="7" t="s">
         <v>20</v>
@@ -2934,16 +2892,16 @@
         <v>6</v>
       </c>
       <c r="R26" s="11" t="s">
+        <v>153</v>
+      </c>
+      <c r="S26" s="10" t="s">
         <v>157</v>
       </c>
-      <c r="S26" s="10" t="s">
-        <v>161</v>
-      </c>
       <c r="T26" s="29" t="s">
-        <v>218</v>
+        <v>212</v>
       </c>
       <c r="U26" s="10" t="s">
-        <v>163</v>
+        <v>159</v>
       </c>
     </row>
     <row r="27" spans="1:21" ht="30" x14ac:dyDescent="0.25">
@@ -2951,20 +2909,20 @@
         <v>17</v>
       </c>
       <c r="B27" s="12" t="s">
-        <v>151</v>
+        <v>148</v>
       </c>
       <c r="C27" s="13" t="s">
-        <v>152</v>
+        <v>149</v>
       </c>
       <c r="D27" s="14" t="s">
-        <v>184</v>
+        <v>179</v>
       </c>
       <c r="E27" s="12" t="s">
-        <v>166</v>
+        <v>162</v>
       </c>
       <c r="F27" s="9"/>
       <c r="G27" s="17" t="s">
-        <v>146</v>
+        <v>238</v>
       </c>
       <c r="H27" s="18">
         <v>23</v>
@@ -2973,7 +2931,7 @@
         <v>20</v>
       </c>
       <c r="J27" s="27" t="s">
-        <v>216</v>
+        <v>211</v>
       </c>
       <c r="K27" s="7" t="s">
         <v>20</v>
@@ -2993,37 +2951,37 @@
         <v>6</v>
       </c>
       <c r="R27" s="11" t="s">
+        <v>153</v>
+      </c>
+      <c r="S27" s="10" t="s">
         <v>157</v>
       </c>
-      <c r="S27" s="10" t="s">
-        <v>161</v>
-      </c>
       <c r="T27" s="29" t="s">
-        <v>219</v>
+        <v>213</v>
       </c>
       <c r="U27" s="10" t="s">
-        <v>163</v>
-      </c>
-    </row>
-    <row r="28" spans="1:21" ht="45" x14ac:dyDescent="0.25">
+        <v>159</v>
+      </c>
+    </row>
+    <row r="28" spans="1:21" ht="30" x14ac:dyDescent="0.25">
       <c r="A28" s="4" t="s">
         <v>17</v>
       </c>
       <c r="B28" s="12" t="s">
-        <v>151</v>
+        <v>148</v>
       </c>
       <c r="C28" s="13" t="s">
-        <v>152</v>
+        <v>149</v>
       </c>
       <c r="D28" s="14" t="s">
-        <v>184</v>
+        <v>214</v>
       </c>
       <c r="E28" s="12" t="s">
-        <v>166</v>
+        <v>162</v>
       </c>
       <c r="F28" s="9"/>
       <c r="G28" s="17" t="s">
-        <v>145</v>
+        <v>144</v>
       </c>
       <c r="H28" s="18">
         <v>24</v>
@@ -3032,7 +2990,7 @@
         <v>20</v>
       </c>
       <c r="J28" s="27" t="s">
-        <v>217</v>
+        <v>215</v>
       </c>
       <c r="K28" s="7" t="s">
         <v>20</v>
@@ -3042,85 +3000,85 @@
       </c>
       <c r="M28" s="8"/>
       <c r="N28" s="8" t="s">
-        <v>32</v>
+        <v>126</v>
       </c>
       <c r="O28" s="9"/>
       <c r="P28" s="18" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="Q28" s="10">
         <v>6</v>
       </c>
       <c r="R28" s="11" t="s">
+        <v>153</v>
+      </c>
+      <c r="S28" s="10" t="s">
         <v>157</v>
       </c>
-      <c r="S28" s="10" t="s">
-        <v>161</v>
-      </c>
       <c r="T28" s="29" t="s">
-        <v>222</v>
+        <v>217</v>
       </c>
       <c r="U28" s="10" t="s">
-        <v>163</v>
-      </c>
-    </row>
-    <row r="29" spans="1:21" ht="30" x14ac:dyDescent="0.25">
+        <v>159</v>
+      </c>
+    </row>
+    <row r="29" spans="1:21" ht="45" x14ac:dyDescent="0.25">
       <c r="A29" s="4" t="s">
         <v>17</v>
       </c>
       <c r="B29" s="12" t="s">
-        <v>151</v>
+        <v>148</v>
       </c>
       <c r="C29" s="13" t="s">
-        <v>152</v>
+        <v>149</v>
       </c>
       <c r="D29" s="14" t="s">
-        <v>220</v>
-      </c>
-      <c r="E29" s="12" t="s">
-        <v>166</v>
-      </c>
+        <v>218</v>
+      </c>
+      <c r="E29" s="12"/>
       <c r="F29" s="9"/>
-      <c r="G29" s="17" t="s">
-        <v>147</v>
-      </c>
-      <c r="H29" s="18">
+      <c r="G29" s="20" t="s">
+        <v>145</v>
+      </c>
+      <c r="H29" s="21">
         <v>25</v>
       </c>
-      <c r="I29" s="5" t="s">
+      <c r="I29" s="22" t="s">
         <v>20</v>
       </c>
-      <c r="J29" s="27" t="s">
-        <v>221</v>
-      </c>
-      <c r="K29" s="7" t="s">
-        <v>20</v>
-      </c>
-      <c r="L29" s="6" t="s">
+      <c r="J29" s="28" t="s">
+        <v>219</v>
+      </c>
+      <c r="K29" s="23" t="s">
+        <v>19</v>
+      </c>
+      <c r="L29" s="24" t="s">
         <v>8</v>
       </c>
-      <c r="M29" s="8"/>
-      <c r="N29" s="8" t="s">
-        <v>126</v>
-      </c>
-      <c r="O29" s="9"/>
-      <c r="P29" s="18" t="s">
+      <c r="M29" s="25"/>
+      <c r="N29" s="25" t="s">
+        <v>120</v>
+      </c>
+      <c r="O29" s="9" t="s">
+        <v>234</v>
+      </c>
+      <c r="P29" s="21" t="s">
         <v>19</v>
       </c>
-      <c r="Q29" s="10">
-        <v>6</v>
+      <c r="Q29" s="10" t="s">
+        <v>222</v>
       </c>
       <c r="R29" s="11" t="s">
-        <v>157</v>
+        <v>223</v>
       </c>
       <c r="S29" s="10" t="s">
-        <v>161</v>
+        <v>149</v>
       </c>
       <c r="T29" s="29" t="s">
-        <v>223</v>
+        <v>145</v>
       </c>
       <c r="U29" s="10" t="s">
-        <v>163</v>
+        <v>224</v>
       </c>
     </row>
     <row r="30" spans="1:21" ht="45" x14ac:dyDescent="0.25">
@@ -3128,18 +3086,18 @@
         <v>17</v>
       </c>
       <c r="B30" s="12" t="s">
-        <v>151</v>
+        <v>148</v>
       </c>
       <c r="C30" s="13" t="s">
-        <v>152</v>
+        <v>149</v>
       </c>
       <c r="D30" s="14" t="s">
-        <v>224</v>
+        <v>218</v>
       </c>
       <c r="E30" s="12"/>
       <c r="F30" s="9"/>
-      <c r="G30" s="20" t="s">
-        <v>148</v>
+      <c r="G30" s="17" t="s">
+        <v>146</v>
       </c>
       <c r="H30" s="21">
         <v>26</v>
@@ -3148,7 +3106,7 @@
         <v>20</v>
       </c>
       <c r="J30" s="28" t="s">
-        <v>225</v>
+        <v>220</v>
       </c>
       <c r="K30" s="23" t="s">
         <v>19</v>
@@ -3160,54 +3118,52 @@
       <c r="N30" s="25" t="s">
         <v>120</v>
       </c>
-      <c r="O30" s="9" t="s">
-        <v>244</v>
-      </c>
+      <c r="O30" s="26"/>
       <c r="P30" s="21" t="s">
         <v>19</v>
       </c>
       <c r="Q30" s="10" t="s">
-        <v>228</v>
+        <v>222</v>
       </c>
       <c r="R30" s="11" t="s">
-        <v>229</v>
+        <v>223</v>
       </c>
       <c r="S30" s="10" t="s">
-        <v>152</v>
+        <v>149</v>
       </c>
       <c r="T30" s="29" t="s">
-        <v>148</v>
+        <v>146</v>
       </c>
       <c r="U30" s="10" t="s">
-        <v>230</v>
-      </c>
-    </row>
-    <row r="31" spans="1:21" ht="45" x14ac:dyDescent="0.25">
+        <v>224</v>
+      </c>
+    </row>
+    <row r="31" spans="1:21" ht="30" x14ac:dyDescent="0.25">
       <c r="A31" s="4" t="s">
         <v>17</v>
       </c>
       <c r="B31" s="12" t="s">
-        <v>151</v>
+        <v>148</v>
       </c>
       <c r="C31" s="13" t="s">
-        <v>152</v>
+        <v>149</v>
       </c>
       <c r="D31" s="14" t="s">
-        <v>224</v>
+        <v>218</v>
       </c>
       <c r="E31" s="12"/>
       <c r="F31" s="9"/>
       <c r="G31" s="17" t="s">
-        <v>149</v>
-      </c>
-      <c r="H31" s="21">
+        <v>147</v>
+      </c>
+      <c r="H31" s="18">
         <v>27</v>
       </c>
-      <c r="I31" s="22" t="s">
+      <c r="I31" s="5" t="s">
         <v>20</v>
       </c>
-      <c r="J31" s="28" t="s">
-        <v>226</v>
+      <c r="J31" s="27" t="s">
+        <v>221</v>
       </c>
       <c r="K31" s="23" t="s">
         <v>19</v>
@@ -3224,38 +3180,38 @@
         <v>19</v>
       </c>
       <c r="Q31" s="10" t="s">
-        <v>228</v>
+        <v>166</v>
       </c>
       <c r="R31" s="11" t="s">
-        <v>229</v>
+        <v>167</v>
       </c>
       <c r="S31" s="10" t="s">
-        <v>152</v>
+        <v>149</v>
       </c>
       <c r="T31" s="29" t="s">
-        <v>149</v>
+        <v>147</v>
       </c>
       <c r="U31" s="10" t="s">
-        <v>230</v>
-      </c>
-    </row>
-    <row r="32" spans="1:21" ht="30" x14ac:dyDescent="0.25">
+        <v>168</v>
+      </c>
+    </row>
+    <row r="32" spans="1:21" ht="60" x14ac:dyDescent="0.25">
       <c r="A32" s="4" t="s">
         <v>17</v>
       </c>
       <c r="B32" s="12" t="s">
-        <v>151</v>
+        <v>148</v>
       </c>
       <c r="C32" s="13" t="s">
-        <v>152</v>
+        <v>149</v>
       </c>
       <c r="D32" s="14" t="s">
-        <v>224</v>
+        <v>218</v>
       </c>
       <c r="E32" s="12"/>
       <c r="F32" s="9"/>
       <c r="G32" s="17" t="s">
-        <v>150</v>
+        <v>225</v>
       </c>
       <c r="H32" s="18">
         <v>28</v>
@@ -3264,55 +3220,57 @@
         <v>20</v>
       </c>
       <c r="J32" s="27" t="s">
-        <v>227</v>
-      </c>
-      <c r="K32" s="23" t="s">
+        <v>228</v>
+      </c>
+      <c r="K32" s="7" t="s">
         <v>19</v>
       </c>
-      <c r="L32" s="24" t="s">
+      <c r="L32" s="6" t="s">
         <v>8</v>
       </c>
-      <c r="M32" s="25"/>
+      <c r="M32" s="8"/>
       <c r="N32" s="25" t="s">
         <v>120</v>
       </c>
-      <c r="O32" s="26"/>
-      <c r="P32" s="21" t="s">
+      <c r="O32" s="9" t="s">
+        <v>243</v>
+      </c>
+      <c r="P32" s="18" t="s">
         <v>19</v>
       </c>
       <c r="Q32" s="10" t="s">
-        <v>170</v>
+        <v>166</v>
       </c>
       <c r="R32" s="11" t="s">
-        <v>171</v>
+        <v>167</v>
       </c>
       <c r="S32" s="10" t="s">
-        <v>152</v>
+        <v>149</v>
       </c>
       <c r="T32" s="29" t="s">
-        <v>150</v>
+        <v>225</v>
       </c>
       <c r="U32" s="10" t="s">
-        <v>172</v>
-      </c>
-    </row>
-    <row r="33" spans="1:21" ht="60" x14ac:dyDescent="0.25">
+        <v>168</v>
+      </c>
+    </row>
+    <row r="33" spans="1:21" ht="45" x14ac:dyDescent="0.25">
       <c r="A33" s="4" t="s">
         <v>17</v>
       </c>
       <c r="B33" s="12" t="s">
-        <v>151</v>
+        <v>148</v>
       </c>
       <c r="C33" s="13" t="s">
-        <v>152</v>
+        <v>149</v>
       </c>
       <c r="D33" s="14" t="s">
-        <v>224</v>
+        <v>218</v>
       </c>
       <c r="E33" s="12"/>
       <c r="F33" s="9"/>
       <c r="G33" s="17" t="s">
-        <v>231</v>
+        <v>226</v>
       </c>
       <c r="H33" s="18">
         <v>29</v>
@@ -3321,7 +3279,7 @@
         <v>20</v>
       </c>
       <c r="J33" s="27" t="s">
-        <v>234</v>
+        <v>227</v>
       </c>
       <c r="K33" s="7" t="s">
         <v>19</v>
@@ -3333,45 +3291,43 @@
       <c r="N33" s="25" t="s">
         <v>120</v>
       </c>
-      <c r="O33" s="9" t="s">
-        <v>244</v>
-      </c>
+      <c r="O33" s="9"/>
       <c r="P33" s="18" t="s">
         <v>19</v>
       </c>
       <c r="Q33" s="10" t="s">
-        <v>170</v>
+        <v>166</v>
       </c>
       <c r="R33" s="11" t="s">
-        <v>171</v>
+        <v>167</v>
       </c>
       <c r="S33" s="10" t="s">
-        <v>152</v>
+        <v>149</v>
       </c>
       <c r="T33" s="29" t="s">
-        <v>231</v>
+        <v>226</v>
       </c>
       <c r="U33" s="10" t="s">
-        <v>172</v>
-      </c>
-    </row>
-    <row r="34" spans="1:21" ht="45" x14ac:dyDescent="0.25">
+        <v>168</v>
+      </c>
+    </row>
+    <row r="34" spans="1:21" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A34" s="4" t="s">
         <v>17</v>
       </c>
       <c r="B34" s="12" t="s">
-        <v>151</v>
+        <v>148</v>
       </c>
       <c r="C34" s="13" t="s">
-        <v>152</v>
-      </c>
-      <c r="D34" s="14" t="s">
-        <v>224</v>
+        <v>149</v>
+      </c>
+      <c r="D34" s="32" t="s">
+        <v>229</v>
       </c>
       <c r="E34" s="12"/>
       <c r="F34" s="9"/>
       <c r="G34" s="17" t="s">
-        <v>232</v>
+        <v>10</v>
       </c>
       <c r="H34" s="18">
         <v>30</v>
@@ -3380,57 +3336,43 @@
         <v>20</v>
       </c>
       <c r="J34" s="27" t="s">
-        <v>233</v>
+        <v>231</v>
       </c>
       <c r="K34" s="7" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="L34" s="6" t="s">
-        <v>8</v>
+        <v>10</v>
       </c>
       <c r="M34" s="8"/>
-      <c r="N34" s="25" t="s">
-        <v>120</v>
-      </c>
+      <c r="N34" s="8"/>
       <c r="O34" s="9"/>
       <c r="P34" s="18" t="s">
         <v>19</v>
       </c>
-      <c r="Q34" s="10" t="s">
-        <v>170</v>
-      </c>
-      <c r="R34" s="11" t="s">
-        <v>171</v>
-      </c>
-      <c r="S34" s="10" t="s">
-        <v>152</v>
-      </c>
-      <c r="T34" s="29" t="s">
-        <v>232</v>
-      </c>
-      <c r="U34" s="10" t="s">
-        <v>172</v>
-      </c>
+      <c r="Q34" s="10"/>
+      <c r="R34" s="11"/>
+      <c r="S34" s="10"/>
+      <c r="T34" s="29"/>
+      <c r="U34" s="10"/>
     </row>
     <row r="35" spans="1:21" ht="30" x14ac:dyDescent="0.25">
       <c r="A35" s="4" t="s">
         <v>17</v>
       </c>
       <c r="B35" s="12" t="s">
-        <v>151</v>
+        <v>148</v>
       </c>
       <c r="C35" s="13" t="s">
-        <v>152</v>
-      </c>
-      <c r="D35" s="55" t="s">
-        <v>235</v>
-      </c>
-      <c r="E35" s="12" t="s">
-        <v>10</v>
-      </c>
+        <v>149</v>
+      </c>
+      <c r="D35" s="31" t="s">
+        <v>229</v>
+      </c>
+      <c r="E35" s="12"/>
       <c r="F35" s="9"/>
       <c r="G35" s="17" t="s">
-        <v>237</v>
+        <v>230</v>
       </c>
       <c r="H35" s="18">
         <v>31</v>
@@ -3438,44 +3380,56 @@
       <c r="I35" s="5" t="s">
         <v>20</v>
       </c>
-      <c r="J35" s="27"/>
+      <c r="J35" s="27" t="s">
+        <v>232</v>
+      </c>
       <c r="K35" s="7" t="s">
         <v>20</v>
       </c>
       <c r="L35" s="6" t="s">
-        <v>10</v>
+        <v>8</v>
       </c>
       <c r="M35" s="8"/>
-      <c r="N35" s="8"/>
+      <c r="N35" s="8" t="s">
+        <v>32</v>
+      </c>
       <c r="O35" s="9"/>
       <c r="P35" s="18" t="s">
         <v>19</v>
       </c>
-      <c r="Q35" s="10"/>
-      <c r="R35" s="11"/>
-      <c r="S35" s="10"/>
-      <c r="T35" s="29"/>
-      <c r="U35" s="10"/>
+      <c r="Q35" s="10">
+        <v>6</v>
+      </c>
+      <c r="R35" s="11" t="s">
+        <v>153</v>
+      </c>
+      <c r="S35" s="10" t="s">
+        <v>157</v>
+      </c>
+      <c r="T35" s="29" t="s">
+        <v>216</v>
+      </c>
+      <c r="U35" s="10" t="s">
+        <v>159</v>
+      </c>
     </row>
     <row r="36" spans="1:21" ht="30" x14ac:dyDescent="0.25">
       <c r="A36" s="4" t="s">
         <v>17</v>
       </c>
       <c r="B36" s="12" t="s">
-        <v>151</v>
+        <v>148</v>
       </c>
       <c r="C36" s="13" t="s">
-        <v>152</v>
-      </c>
-      <c r="D36" s="54" t="s">
-        <v>235</v>
-      </c>
-      <c r="E36" s="12" t="s">
-        <v>236</v>
-      </c>
+        <v>149</v>
+      </c>
+      <c r="D36" s="31" t="s">
+        <v>229</v>
+      </c>
+      <c r="E36" s="12"/>
       <c r="F36" s="9"/>
       <c r="G36" s="17" t="s">
-        <v>238</v>
+        <v>242</v>
       </c>
       <c r="H36" s="18">
         <v>32</v>
@@ -3483,7 +3437,9 @@
       <c r="I36" s="5" t="s">
         <v>20</v>
       </c>
-      <c r="J36" s="27"/>
+      <c r="J36" s="27" t="s">
+        <v>241</v>
+      </c>
       <c r="K36" s="7" t="s">
         <v>20</v>
       </c>
@@ -3492,80 +3448,50 @@
       </c>
       <c r="M36" s="8"/>
       <c r="N36" s="8" t="s">
-        <v>32</v>
+        <v>52</v>
       </c>
       <c r="O36" s="9"/>
       <c r="P36" s="18" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="Q36" s="10">
         <v>6</v>
       </c>
       <c r="R36" s="11" t="s">
-        <v>190</v>
+        <v>153</v>
       </c>
       <c r="S36" s="10" t="s">
-        <v>239</v>
+        <v>157</v>
       </c>
       <c r="T36" s="29" t="s">
-        <v>240</v>
+        <v>233</v>
       </c>
       <c r="U36" s="10" t="s">
-        <v>241</v>
-      </c>
-    </row>
-    <row r="37" spans="1:21" ht="30" x14ac:dyDescent="0.25">
-      <c r="A37" s="4" t="s">
-        <v>17</v>
-      </c>
-      <c r="B37" s="12" t="s">
-        <v>151</v>
-      </c>
-      <c r="C37" s="13" t="s">
-        <v>152</v>
-      </c>
+        <v>159</v>
+      </c>
+    </row>
+    <row r="37" spans="1:21" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A37" s="4"/>
+      <c r="B37" s="12"/>
+      <c r="C37" s="13"/>
       <c r="D37" s="14"/>
       <c r="E37" s="12"/>
       <c r="F37" s="9"/>
-      <c r="G37" s="17" t="s">
-        <v>242</v>
-      </c>
-      <c r="H37" s="18">
-        <v>33</v>
-      </c>
-      <c r="I37" s="5" t="s">
-        <v>20</v>
-      </c>
+      <c r="G37" s="17"/>
+      <c r="H37" s="18"/>
+      <c r="I37" s="5"/>
       <c r="J37" s="27"/>
-      <c r="K37" s="7" t="s">
-        <v>20</v>
-      </c>
-      <c r="L37" s="6" t="s">
-        <v>8</v>
-      </c>
+      <c r="K37" s="7"/>
+      <c r="L37" s="6"/>
       <c r="M37" s="8"/>
-      <c r="N37" s="8" t="s">
-        <v>52</v>
-      </c>
+      <c r="N37" s="8"/>
       <c r="O37" s="9"/>
-      <c r="P37" s="18" t="s">
-        <v>20</v>
-      </c>
-      <c r="Q37" s="10">
-        <v>6</v>
-      </c>
-      <c r="R37" s="11" t="s">
-        <v>157</v>
-      </c>
-      <c r="S37" s="10" t="s">
-        <v>161</v>
-      </c>
-      <c r="T37" s="29" t="s">
-        <v>243</v>
-      </c>
-      <c r="U37" s="10" t="s">
-        <v>163</v>
-      </c>
+      <c r="P37" s="18"/>
+      <c r="Q37" s="10"/>
+      <c r="R37" s="11"/>
+      <c r="S37" s="10"/>
+      <c r="T37" s="29"/>
+      <c r="U37" s="10"/>
     </row>
     <row r="38" spans="1:21" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A38" s="4"/>
@@ -4303,29 +4229,7 @@
       <c r="T69" s="29"/>
       <c r="U69" s="10"/>
     </row>
-    <row r="70" spans="1:21" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A70" s="4"/>
-      <c r="B70" s="12"/>
-      <c r="C70" s="13"/>
-      <c r="D70" s="14"/>
-      <c r="E70" s="12"/>
-      <c r="F70" s="9"/>
-      <c r="G70" s="17"/>
-      <c r="H70" s="18"/>
-      <c r="I70" s="5"/>
-      <c r="J70" s="27"/>
-      <c r="K70" s="7"/>
-      <c r="L70" s="6"/>
-      <c r="M70" s="8"/>
-      <c r="N70" s="8"/>
-      <c r="O70" s="9"/>
-      <c r="P70" s="18"/>
-      <c r="Q70" s="10"/>
-      <c r="R70" s="11"/>
-      <c r="S70" s="10"/>
-      <c r="T70" s="29"/>
-      <c r="U70" s="10"/>
-    </row>
+    <row r="71" spans="1:21" hidden="1" x14ac:dyDescent="0.25"/>
     <row r="72" spans="1:21" hidden="1" x14ac:dyDescent="0.25"/>
     <row r="73" spans="1:21" hidden="1" x14ac:dyDescent="0.25"/>
     <row r="74" spans="1:21" hidden="1" x14ac:dyDescent="0.25"/>
@@ -4338,192 +4242,192 @@
     <row r="81" spans="1:1" hidden="1" x14ac:dyDescent="0.25"/>
     <row r="82" spans="1:1" hidden="1" x14ac:dyDescent="0.25"/>
     <row r="83" spans="1:1" hidden="1" x14ac:dyDescent="0.25"/>
-    <row r="84" spans="1:1" hidden="1" x14ac:dyDescent="0.25"/>
+    <row r="84" spans="1:1" hidden="1" x14ac:dyDescent="0.25">
+      <c r="A84" t="s">
+        <v>92</v>
+      </c>
+    </row>
     <row r="85" spans="1:1" hidden="1" x14ac:dyDescent="0.25">
       <c r="A85" t="s">
-        <v>92</v>
+        <v>93</v>
       </c>
     </row>
     <row r="86" spans="1:1" hidden="1" x14ac:dyDescent="0.25">
       <c r="A86" t="s">
-        <v>93</v>
+        <v>94</v>
       </c>
     </row>
     <row r="87" spans="1:1" hidden="1" x14ac:dyDescent="0.25">
       <c r="A87" t="s">
-        <v>94</v>
+        <v>95</v>
       </c>
     </row>
     <row r="88" spans="1:1" hidden="1" x14ac:dyDescent="0.25">
       <c r="A88" t="s">
-        <v>95</v>
+        <v>96</v>
       </c>
     </row>
     <row r="89" spans="1:1" hidden="1" x14ac:dyDescent="0.25">
       <c r="A89" t="s">
-        <v>96</v>
+        <v>97</v>
       </c>
     </row>
     <row r="90" spans="1:1" hidden="1" x14ac:dyDescent="0.25">
       <c r="A90" t="s">
-        <v>97</v>
+        <v>99</v>
       </c>
     </row>
     <row r="91" spans="1:1" hidden="1" x14ac:dyDescent="0.25">
       <c r="A91" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
     </row>
     <row r="92" spans="1:1" hidden="1" x14ac:dyDescent="0.25">
       <c r="A92" t="s">
-        <v>98</v>
+        <v>100</v>
       </c>
     </row>
     <row r="93" spans="1:1" hidden="1" x14ac:dyDescent="0.25">
       <c r="A93" t="s">
-        <v>100</v>
+        <v>101</v>
       </c>
     </row>
     <row r="94" spans="1:1" hidden="1" x14ac:dyDescent="0.25">
       <c r="A94" t="s">
-        <v>101</v>
+        <v>102</v>
       </c>
     </row>
     <row r="95" spans="1:1" hidden="1" x14ac:dyDescent="0.25">
       <c r="A95" t="s">
-        <v>102</v>
+        <v>103</v>
       </c>
     </row>
     <row r="96" spans="1:1" hidden="1" x14ac:dyDescent="0.25">
       <c r="A96" t="s">
-        <v>103</v>
+        <v>104</v>
       </c>
     </row>
     <row r="97" spans="1:1" hidden="1" x14ac:dyDescent="0.25">
       <c r="A97" t="s">
-        <v>104</v>
+        <v>105</v>
       </c>
     </row>
     <row r="98" spans="1:1" hidden="1" x14ac:dyDescent="0.25">
       <c r="A98" t="s">
-        <v>105</v>
+        <v>106</v>
       </c>
     </row>
     <row r="99" spans="1:1" hidden="1" x14ac:dyDescent="0.25">
       <c r="A99" t="s">
-        <v>106</v>
+        <v>65</v>
       </c>
     </row>
     <row r="100" spans="1:1" hidden="1" x14ac:dyDescent="0.25">
       <c r="A100" t="s">
-        <v>65</v>
+        <v>66</v>
       </c>
     </row>
     <row r="101" spans="1:1" hidden="1" x14ac:dyDescent="0.25">
       <c r="A101" t="s">
-        <v>66</v>
+        <v>67</v>
       </c>
     </row>
     <row r="102" spans="1:1" hidden="1" x14ac:dyDescent="0.25">
       <c r="A102" t="s">
-        <v>67</v>
+        <v>68</v>
       </c>
     </row>
     <row r="103" spans="1:1" hidden="1" x14ac:dyDescent="0.25">
       <c r="A103" t="s">
-        <v>68</v>
+        <v>69</v>
       </c>
     </row>
     <row r="104" spans="1:1" hidden="1" x14ac:dyDescent="0.25">
       <c r="A104" t="s">
-        <v>69</v>
+        <v>70</v>
       </c>
     </row>
     <row r="105" spans="1:1" hidden="1" x14ac:dyDescent="0.25">
       <c r="A105" t="s">
-        <v>70</v>
+        <v>71</v>
       </c>
     </row>
     <row r="106" spans="1:1" hidden="1" x14ac:dyDescent="0.25">
       <c r="A106" t="s">
-        <v>71</v>
+        <v>72</v>
       </c>
     </row>
     <row r="107" spans="1:1" hidden="1" x14ac:dyDescent="0.25">
       <c r="A107" t="s">
-        <v>72</v>
+        <v>73</v>
       </c>
     </row>
     <row r="108" spans="1:1" hidden="1" x14ac:dyDescent="0.25">
       <c r="A108" t="s">
-        <v>73</v>
+        <v>74</v>
       </c>
     </row>
     <row r="109" spans="1:1" hidden="1" x14ac:dyDescent="0.25">
       <c r="A109" t="s">
-        <v>74</v>
+        <v>75</v>
       </c>
     </row>
     <row r="110" spans="1:1" hidden="1" x14ac:dyDescent="0.25">
       <c r="A110" t="s">
-        <v>75</v>
+        <v>76</v>
       </c>
     </row>
     <row r="111" spans="1:1" hidden="1" x14ac:dyDescent="0.25">
       <c r="A111" t="s">
-        <v>76</v>
+        <v>77</v>
       </c>
     </row>
     <row r="112" spans="1:1" hidden="1" x14ac:dyDescent="0.25">
       <c r="A112" t="s">
-        <v>77</v>
+        <v>78</v>
       </c>
     </row>
     <row r="113" spans="1:1" hidden="1" x14ac:dyDescent="0.25">
       <c r="A113" t="s">
-        <v>78</v>
+        <v>79</v>
       </c>
     </row>
     <row r="114" spans="1:1" hidden="1" x14ac:dyDescent="0.25">
       <c r="A114" t="s">
-        <v>79</v>
+        <v>80</v>
       </c>
     </row>
     <row r="115" spans="1:1" hidden="1" x14ac:dyDescent="0.25">
       <c r="A115" t="s">
-        <v>80</v>
+        <v>81</v>
       </c>
     </row>
     <row r="116" spans="1:1" hidden="1" x14ac:dyDescent="0.25">
       <c r="A116" t="s">
-        <v>81</v>
+        <v>82</v>
       </c>
     </row>
     <row r="117" spans="1:1" hidden="1" x14ac:dyDescent="0.25">
       <c r="A117" t="s">
-        <v>82</v>
+        <v>83</v>
       </c>
     </row>
     <row r="118" spans="1:1" hidden="1" x14ac:dyDescent="0.25">
       <c r="A118" t="s">
-        <v>83</v>
+        <v>84</v>
       </c>
     </row>
     <row r="119" spans="1:1" hidden="1" x14ac:dyDescent="0.25">
       <c r="A119" t="s">
-        <v>84</v>
+        <v>116</v>
       </c>
     </row>
     <row r="120" spans="1:1" hidden="1" x14ac:dyDescent="0.25">
       <c r="A120" t="s">
-        <v>116</v>
-      </c>
-    </row>
-    <row r="121" spans="1:1" hidden="1" x14ac:dyDescent="0.25">
-      <c r="A121" t="s">
         <v>115</v>
       </c>
     </row>
+    <row r="121" spans="1:1" hidden="1" x14ac:dyDescent="0.25"/>
     <row r="122" spans="1:1" hidden="1" x14ac:dyDescent="0.25"/>
     <row r="123" spans="1:1" hidden="1" x14ac:dyDescent="0.25"/>
     <row r="124" spans="1:1" hidden="1" x14ac:dyDescent="0.25"/>
@@ -4686,11 +4590,8 @@
     <row r="281" hidden="1" x14ac:dyDescent="0.25"/>
     <row r="282" hidden="1" x14ac:dyDescent="0.25"/>
     <row r="283" hidden="1" x14ac:dyDescent="0.25"/>
-    <row r="284" hidden="1" x14ac:dyDescent="0.25"/>
   </sheetData>
-  <autoFilter ref="A1:U2">
-    <filterColumn colId="12" showButton="0"/>
-  </autoFilter>
+  <autoFilter ref="A2:U36"/>
   <mergeCells count="20">
     <mergeCell ref="I1:I2"/>
     <mergeCell ref="H1:H2"/>
@@ -4715,7 +4616,6 @@
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
-  <legacyDrawing r:id="rId2"/>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{CCE6A557-97BC-4b89-ADB6-D9C93CAAB3DF}">
       <x14:dataValidations xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" count="5">
@@ -4723,31 +4623,31 @@
           <x14:formula1>
             <xm:f>DATOS!$E$14:$E$48</xm:f>
           </x14:formula1>
-          <xm:sqref>N3:N70</xm:sqref>
+          <xm:sqref>N3:N69</xm:sqref>
         </x14:dataValidation>
         <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1">
           <x14:formula1>
             <xm:f>DATOS!$A$1:$A$4</xm:f>
           </x14:formula1>
-          <xm:sqref>A3:A70</xm:sqref>
+          <xm:sqref>A3:A69</xm:sqref>
         </x14:dataValidation>
         <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1">
           <x14:formula1>
             <xm:f>DATOS!$D$1:$D$2</xm:f>
           </x14:formula1>
-          <xm:sqref>K3:K70 P3:P70 I3:I70</xm:sqref>
+          <xm:sqref>P3:P69 K3:K69 I3:I69</xm:sqref>
         </x14:dataValidation>
         <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1">
           <x14:formula1>
             <xm:f>DATOS!$B$1:$B$7</xm:f>
           </x14:formula1>
-          <xm:sqref>L3:L70</xm:sqref>
+          <xm:sqref>L3:L69</xm:sqref>
         </x14:dataValidation>
         <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1">
           <x14:formula1>
             <xm:f>DATOS!$E$1:$E$13</xm:f>
           </x14:formula1>
-          <xm:sqref>M3:M70</xm:sqref>
+          <xm:sqref>M3:M69</xm:sqref>
         </x14:dataValidation>
       </x14:dataValidations>
     </ext>
@@ -4759,8 +4659,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:O133"/>
   <sheetViews>
-    <sheetView topLeftCell="C20" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="E47" sqref="E47"/>
+    <sheetView topLeftCell="C38" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="E46" sqref="E46"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>

<commit_message>
Actualización guion y escaleta CN_06_03_CO
Actualización guion y escaleta CN_06_03_CO
</commit_message>
<xml_diff>
--- a/fuentes/contenidos/grado06/guion03/Escaleta CN_06_03_CO.xlsx
+++ b/fuentes/contenidos/grado06/guion03/Escaleta CN_06_03_CO.xlsx
@@ -5,7 +5,7 @@
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Mpgarcia\Desktop\CienciasNaturales\fuentes\contenidos\grado06\guion03\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\diego\Dropbox\Editorial planeta\1. Autor\Escaletas\CN_06_03_CO\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -13,7 +13,7 @@
   </bookViews>
   <sheets>
     <sheet name="Escaleta" sheetId="2" r:id="rId1"/>
-    <sheet name="VER" sheetId="3" r:id="rId2"/>
+    <sheet name="VER" sheetId="3" state="hidden" r:id="rId2"/>
     <sheet name="DATOS" sheetId="1" state="hidden" r:id="rId3"/>
   </sheets>
   <definedNames>
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="699" uniqueCount="264">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="698" uniqueCount="265">
   <si>
     <t>Asignatura</t>
   </si>
@@ -408,51 +408,15 @@
     <t>m101a</t>
   </si>
   <si>
-    <t>La función de relación</t>
-  </si>
-  <si>
     <t>Selecciona cómo se reproducen estos organismos</t>
   </si>
   <si>
-    <t>Características de los seres vivos</t>
-  </si>
-  <si>
     <t>Refuerza tu aprendizaje: Las funciones de los seres vivos</t>
   </si>
   <si>
-    <t xml:space="preserve">Características de las arqueas </t>
-  </si>
-  <si>
-    <t>Estructura de la bacteria</t>
-  </si>
-  <si>
-    <t>Características de las bacterias</t>
-  </si>
-  <si>
     <t>Importancia biológica de las bacterias</t>
   </si>
   <si>
-    <t>Clasificación de los protistas</t>
-  </si>
-  <si>
-    <t>Características de los protistas</t>
-  </si>
-  <si>
-    <t>Características de los hongos</t>
-  </si>
-  <si>
-    <t>Características de las plantas</t>
-  </si>
-  <si>
-    <t>Identifica y clasifica a los seres vivos</t>
-  </si>
-  <si>
-    <t>La extinción de los dinosaurios</t>
-  </si>
-  <si>
-    <t>Características del reino animal</t>
-  </si>
-  <si>
     <t>Refuerza tu aprendizaje: La clasificación de los seres vivos</t>
   </si>
   <si>
@@ -546,15 +510,9 @@
     <t>Los seres se relacionan</t>
   </si>
   <si>
-    <t>Animación que describe el sistema de orientación usado por los murciélagos, basado en la emisión y recepción de ultrasonidos</t>
-  </si>
-  <si>
     <t>Actividad para identificar el tipo de reproducción de distintos seres vivos</t>
   </si>
   <si>
-    <t>Actividad que permite identificar las principales características de los seres vivos</t>
-  </si>
-  <si>
     <t>Recurso M5A-01</t>
   </si>
   <si>
@@ -576,9 +534,6 @@
     <t>El dominio Bacteria</t>
   </si>
   <si>
-    <t>Interactivo que permite identificar y reconocer las funciones de la estructura celular de una bacteria</t>
-  </si>
-  <si>
     <t>RF</t>
   </si>
   <si>
@@ -618,9 +573,6 @@
     <t>Recurso M2C-02</t>
   </si>
   <si>
-    <t>Actividad de juego del ahorcado que permite reforzar las características principales de los hongos</t>
-  </si>
-  <si>
     <t>Recurso M14A-02</t>
   </si>
   <si>
@@ -630,12 +582,6 @@
     <t>El reino hongos</t>
   </si>
   <si>
-    <t>Actividad que permite reforzar las características principales de las plantas </t>
-  </si>
-  <si>
-    <t>Actividad que permite identificar protistas, hongos y plantas</t>
-  </si>
-  <si>
     <t>Recurso M4A-04</t>
   </si>
   <si>
@@ -645,12 +591,6 @@
     <t>El reino animal</t>
   </si>
   <si>
-    <t>Animación que describe la hipótesis sobre la extinción del 90 % de los seres vivos hace unos 65 millones de años</t>
-  </si>
-  <si>
-    <t>Actividad que permite identificar las características del reino animal</t>
-  </si>
-  <si>
     <t>Recurso M5A-02</t>
   </si>
   <si>
@@ -672,21 +612,12 @@
     <t>Actividad para reconocer los virus y los seres vivos</t>
   </si>
   <si>
-    <t>Recurso M4A-05</t>
-  </si>
-  <si>
     <t>Recurso M101A-04</t>
   </si>
   <si>
     <t>Competencias</t>
   </si>
   <si>
-    <t>Actividad que propone el desarrollo de las destrezas para aprender a describir las características de un ser vivo para que otra persona pueda reconocerlo</t>
-  </si>
-  <si>
-    <t>Actividad que propone realizar el procedimiento de reconocimiento de las funciones vitales de los seres vivos</t>
-  </si>
-  <si>
     <t>Actividad que propone diferenciar los tipos de nutrición que presentan los seres vivos</t>
   </si>
   <si>
@@ -705,9 +636,6 @@
     <t>Competencias: relación de la reproducción con los seres vivos</t>
   </si>
   <si>
-    <t>Actividad que propone realizar el procedimiento de relacionar los diferentes tipos de reproducción que existen con los organismos que la realizan</t>
-  </si>
-  <si>
     <t>Actividad que propone el desarrollo de las destrezas para identificar la función de relación en las plantas y comprender la relación de todos los seres vivos con el medio externo</t>
   </si>
   <si>
@@ -729,9 +657,6 @@
     <t>Ver cambios en cuadro del guion</t>
   </si>
   <si>
-    <t>Ver cambios del texto en la ficha en el cuadro del guion</t>
-  </si>
-  <si>
     <t>Actividad para identificar los elementos básicos que forman parte de un ser vivo</t>
   </si>
   <si>
@@ -816,7 +741,85 @@
     <t>Actividad para identificar las funciones vitales de los seres vivos</t>
   </si>
   <si>
-    <t>Actividad de preguntas que permite afianzar los conocimientos aprendidos acerca de la composición de los seres vivos</t>
+    <t>Recurso M2A-02</t>
+  </si>
+  <si>
+    <t>¿De qué están compuestos los seres vivos?</t>
+  </si>
+  <si>
+    <t>Actividad que permite reconocer la composición de los seres vivos</t>
+  </si>
+  <si>
+    <t>Interactivo que permite identificar las funciones de los seres vivos</t>
+  </si>
+  <si>
+    <t>Recurso F7B-01</t>
+  </si>
+  <si>
+    <t>Las características de los seres vivos</t>
+  </si>
+  <si>
+    <t>Crucigrama que permite identificar las principales características de los seres vivos</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Las características de las arqueas </t>
+  </si>
+  <si>
+    <t>La estructura de la bacteria</t>
+  </si>
+  <si>
+    <t>Interactivo que permite identificar la estructura interna de una bacteria</t>
+  </si>
+  <si>
+    <t>Las características de las bacterias</t>
+  </si>
+  <si>
+    <t>La clasificación de los protistas</t>
+  </si>
+  <si>
+    <t>Las características de los protistas</t>
+  </si>
+  <si>
+    <t>Las características de los hongos</t>
+  </si>
+  <si>
+    <t>Actividad de juego del ahorcado que permite reforzar lo aprendido sobre las características de los hongos</t>
+  </si>
+  <si>
+    <t>Las características de las plantas</t>
+  </si>
+  <si>
+    <t>Actividad de preguntas para reforzar lo aprendido sobre las características de las plantas </t>
+  </si>
+  <si>
+    <t>Actividad que permite identificar y clasificar a los protistas, los hongos y las plantas</t>
+  </si>
+  <si>
+    <t>Identifica y clasifica a los protistas, los hongos y las plantas</t>
+  </si>
+  <si>
+    <t>Interactivo que permite identificar y clasificar a los animales</t>
+  </si>
+  <si>
+    <t>Recurso F6B-01</t>
+  </si>
+  <si>
+    <t>Las características del reino animal</t>
+  </si>
+  <si>
+    <t>Actividad para afianzar los conocimientos sobre las características del reino animal</t>
+  </si>
+  <si>
+    <t>¿Cómo se clasifican los animales?</t>
+  </si>
+  <si>
+    <t>Actividad que propone reconocer las funciones vitales de los seres vivos</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Actividad que propone el desarrollo de las destrezas a fin de aprender a describir las características de un ser vivo para que otra persona pueda reconocerlo </t>
+  </si>
+  <si>
+    <t>Actividad que propone relacionar los diferentes tipos de reproducción que existen con los organismos que la realizan</t>
   </si>
 </sst>
 </file>
@@ -1031,7 +1034,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="66">
+  <cellXfs count="67">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
@@ -1199,6 +1202,9 @@
     </xf>
     <xf numFmtId="0" fontId="2" fillId="4" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="12" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="2">
@@ -1507,9 +1513,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:U283"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="F1" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
+    <sheetView tabSelected="1" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
       <pane ySplit="2" topLeftCell="A3" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="K34" sqref="K34"/>
+      <selection pane="bottomLeft" activeCell="A3" sqref="A3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1520,7 +1526,7 @@
     <col min="4" max="4" width="34.140625" customWidth="1"/>
     <col min="5" max="5" width="34.7109375" customWidth="1"/>
     <col min="6" max="6" width="30.28515625" style="1" customWidth="1"/>
-    <col min="7" max="7" width="31" style="15" customWidth="1"/>
+    <col min="7" max="7" width="35.85546875" style="15" customWidth="1"/>
     <col min="8" max="8" width="12.28515625" style="19" customWidth="1"/>
     <col min="9" max="9" width="11" style="1" customWidth="1"/>
     <col min="10" max="10" width="48.28515625" style="15" customWidth="1"/>
@@ -1631,16 +1637,16 @@
         <v>17</v>
       </c>
       <c r="B3" s="12" t="s">
-        <v>148</v>
+        <v>136</v>
       </c>
       <c r="C3" s="13" t="s">
-        <v>149</v>
+        <v>137</v>
       </c>
       <c r="D3" s="14" t="s">
-        <v>150</v>
+        <v>138</v>
       </c>
       <c r="E3" s="12" t="s">
-        <v>151</v>
+        <v>139</v>
       </c>
       <c r="F3" s="9"/>
       <c r="G3" s="17" t="s">
@@ -1653,7 +1659,7 @@
         <v>19</v>
       </c>
       <c r="J3" s="27" t="s">
-        <v>152</v>
+        <v>140</v>
       </c>
       <c r="K3" s="7" t="s">
         <v>20</v>
@@ -1673,16 +1679,16 @@
         <v>6</v>
       </c>
       <c r="R3" s="11" t="s">
-        <v>153</v>
+        <v>141</v>
       </c>
       <c r="S3" s="30" t="s">
-        <v>154</v>
+        <v>142</v>
       </c>
       <c r="T3" s="29" t="s">
-        <v>155</v>
+        <v>143</v>
       </c>
       <c r="U3" s="10" t="s">
-        <v>156</v>
+        <v>144</v>
       </c>
     </row>
     <row r="4" spans="1:21" ht="30" x14ac:dyDescent="0.25">
@@ -1690,16 +1696,16 @@
         <v>17</v>
       </c>
       <c r="B4" s="12" t="s">
-        <v>148</v>
+        <v>136</v>
       </c>
       <c r="C4" s="13" t="s">
-        <v>149</v>
+        <v>137</v>
       </c>
       <c r="D4" s="14" t="s">
-        <v>150</v>
+        <v>138</v>
       </c>
       <c r="E4" s="12" t="s">
-        <v>151</v>
+        <v>139</v>
       </c>
       <c r="F4" s="9"/>
       <c r="G4" s="17" t="s">
@@ -1712,7 +1718,7 @@
         <v>20</v>
       </c>
       <c r="J4" s="27" t="s">
-        <v>235</v>
+        <v>210</v>
       </c>
       <c r="K4" s="7" t="s">
         <v>20</v>
@@ -1732,16 +1738,16 @@
         <v>6</v>
       </c>
       <c r="R4" s="11" t="s">
-        <v>153</v>
+        <v>141</v>
       </c>
       <c r="S4" s="10" t="s">
-        <v>157</v>
+        <v>145</v>
       </c>
       <c r="T4" s="29" t="s">
-        <v>158</v>
+        <v>146</v>
       </c>
       <c r="U4" s="10" t="s">
-        <v>159</v>
+        <v>147</v>
       </c>
     </row>
     <row r="5" spans="1:21" ht="30" x14ac:dyDescent="0.25">
@@ -1749,16 +1755,16 @@
         <v>17</v>
       </c>
       <c r="B5" s="12" t="s">
+        <v>136</v>
+      </c>
+      <c r="C5" s="13" t="s">
+        <v>137</v>
+      </c>
+      <c r="D5" s="14" t="s">
+        <v>138</v>
+      </c>
+      <c r="E5" s="12" t="s">
         <v>148</v>
-      </c>
-      <c r="C5" s="13" t="s">
-        <v>149</v>
-      </c>
-      <c r="D5" s="14" t="s">
-        <v>150</v>
-      </c>
-      <c r="E5" s="12" t="s">
-        <v>160</v>
       </c>
       <c r="F5" s="9"/>
       <c r="G5" s="17" t="s">
@@ -1771,7 +1777,7 @@
         <v>19</v>
       </c>
       <c r="J5" s="27" t="s">
-        <v>161</v>
+        <v>149</v>
       </c>
       <c r="K5" s="7" t="s">
         <v>19</v>
@@ -1788,40 +1794,40 @@
         <v>19</v>
       </c>
       <c r="Q5" s="10" t="s">
-        <v>166</v>
+        <v>154</v>
       </c>
       <c r="R5" s="11" t="s">
-        <v>167</v>
+        <v>155</v>
       </c>
       <c r="S5" s="10" t="s">
-        <v>149</v>
+        <v>137</v>
       </c>
       <c r="T5" s="29" t="s">
         <v>124</v>
       </c>
       <c r="U5" s="10" t="s">
-        <v>168</v>
-      </c>
-    </row>
-    <row r="6" spans="1:21" ht="45" x14ac:dyDescent="0.25">
+        <v>156</v>
+      </c>
+    </row>
+    <row r="6" spans="1:21" ht="30" x14ac:dyDescent="0.25">
       <c r="A6" s="4" t="s">
         <v>17</v>
       </c>
       <c r="B6" s="12" t="s">
+        <v>136</v>
+      </c>
+      <c r="C6" s="13" t="s">
+        <v>137</v>
+      </c>
+      <c r="D6" s="14" t="s">
+        <v>138</v>
+      </c>
+      <c r="E6" s="12" t="s">
         <v>148</v>
-      </c>
-      <c r="C6" s="13" t="s">
-        <v>149</v>
-      </c>
-      <c r="D6" s="14" t="s">
-        <v>150</v>
-      </c>
-      <c r="E6" s="12" t="s">
-        <v>160</v>
       </c>
       <c r="F6" s="9"/>
       <c r="G6" s="17" t="s">
-        <v>150</v>
+        <v>239</v>
       </c>
       <c r="H6" s="18">
         <v>4</v>
@@ -1830,7 +1836,7 @@
         <v>20</v>
       </c>
       <c r="J6" s="27" t="s">
-        <v>263</v>
+        <v>240</v>
       </c>
       <c r="K6" s="7" t="s">
         <v>20</v>
@@ -1840,26 +1846,26 @@
       </c>
       <c r="M6" s="8"/>
       <c r="N6" s="8" t="s">
-        <v>32</v>
+        <v>28</v>
       </c>
       <c r="O6" s="9"/>
-      <c r="P6" s="33" t="s">
-        <v>20</v>
+      <c r="P6" s="66" t="s">
+        <v>19</v>
       </c>
       <c r="Q6" s="10">
         <v>6</v>
       </c>
       <c r="R6" s="11" t="s">
-        <v>153</v>
+        <v>141</v>
       </c>
       <c r="S6" s="10" t="s">
-        <v>157</v>
+        <v>145</v>
       </c>
       <c r="T6" s="29" t="s">
-        <v>165</v>
+        <v>167</v>
       </c>
       <c r="U6" s="10" t="s">
-        <v>159</v>
+        <v>147</v>
       </c>
     </row>
     <row r="7" spans="1:21" ht="30" x14ac:dyDescent="0.25">
@@ -1867,16 +1873,16 @@
         <v>17</v>
       </c>
       <c r="B7" s="12" t="s">
-        <v>148</v>
+        <v>136</v>
       </c>
       <c r="C7" s="13" t="s">
-        <v>149</v>
+        <v>137</v>
       </c>
       <c r="D7" s="14" t="s">
+        <v>138</v>
+      </c>
+      <c r="E7" s="12" t="s">
         <v>150</v>
-      </c>
-      <c r="E7" s="12" t="s">
-        <v>162</v>
       </c>
       <c r="F7" s="9"/>
       <c r="G7" s="17" t="s">
@@ -1889,7 +1895,7 @@
         <v>20</v>
       </c>
       <c r="J7" s="27" t="s">
-        <v>163</v>
+        <v>151</v>
       </c>
       <c r="K7" s="7" t="s">
         <v>20</v>
@@ -1909,16 +1915,16 @@
         <v>6</v>
       </c>
       <c r="R7" s="11" t="s">
-        <v>153</v>
+        <v>141</v>
       </c>
       <c r="S7" s="10" t="s">
-        <v>157</v>
+        <v>145</v>
       </c>
       <c r="T7" s="29" t="s">
-        <v>164</v>
+        <v>152</v>
       </c>
       <c r="U7" s="10" t="s">
-        <v>159</v>
+        <v>147</v>
       </c>
     </row>
     <row r="8" spans="1:21" ht="15.75" x14ac:dyDescent="0.25">
@@ -1926,16 +1932,16 @@
         <v>17</v>
       </c>
       <c r="B8" s="12" t="s">
-        <v>148</v>
+        <v>136</v>
       </c>
       <c r="C8" s="13" t="s">
-        <v>149</v>
+        <v>137</v>
       </c>
       <c r="D8" s="14" t="s">
-        <v>169</v>
+        <v>157</v>
       </c>
       <c r="E8" s="12" t="s">
-        <v>170</v>
+        <v>158</v>
       </c>
       <c r="F8" s="9"/>
       <c r="G8" s="20"/>
@@ -1959,16 +1965,16 @@
         <v>17</v>
       </c>
       <c r="B9" s="12" t="s">
-        <v>148</v>
+        <v>136</v>
       </c>
       <c r="C9" s="13" t="s">
-        <v>149</v>
+        <v>137</v>
       </c>
       <c r="D9" s="14" t="s">
-        <v>169</v>
+        <v>157</v>
       </c>
       <c r="E9" s="12" t="s">
-        <v>171</v>
+        <v>159</v>
       </c>
       <c r="F9" s="9"/>
       <c r="G9" s="17"/>
@@ -1987,25 +1993,25 @@
       <c r="T9" s="29"/>
       <c r="U9" s="10"/>
     </row>
-    <row r="10" spans="1:21" ht="45" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:21" ht="30" x14ac:dyDescent="0.25">
       <c r="A10" s="4" t="s">
         <v>17</v>
       </c>
       <c r="B10" s="12" t="s">
-        <v>148</v>
+        <v>136</v>
       </c>
       <c r="C10" s="13" t="s">
-        <v>149</v>
+        <v>137</v>
       </c>
       <c r="D10" s="14" t="s">
-        <v>169</v>
+        <v>157</v>
       </c>
       <c r="E10" s="12" t="s">
-        <v>172</v>
+        <v>160</v>
       </c>
       <c r="F10" s="9"/>
       <c r="G10" s="20" t="s">
-        <v>127</v>
+        <v>157</v>
       </c>
       <c r="H10" s="21">
         <v>6</v>
@@ -2014,38 +2020,36 @@
         <v>19</v>
       </c>
       <c r="J10" s="28" t="s">
-        <v>173</v>
+        <v>241</v>
       </c>
       <c r="K10" s="23" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="L10" s="24" t="s">
         <v>5</v>
       </c>
       <c r="M10" s="25" t="s">
-        <v>62</v>
+        <v>55</v>
       </c>
       <c r="N10" s="25"/>
-      <c r="O10" s="32" t="s">
-        <v>234</v>
-      </c>
+      <c r="O10" s="32"/>
       <c r="P10" s="21" t="s">
         <v>19</v>
       </c>
-      <c r="Q10" s="10" t="s">
-        <v>166</v>
+      <c r="Q10" s="10">
+        <v>6</v>
       </c>
       <c r="R10" s="11" t="s">
-        <v>167</v>
+        <v>169</v>
       </c>
       <c r="S10" s="10" t="s">
-        <v>149</v>
+        <v>170</v>
       </c>
       <c r="T10" s="29" t="s">
-        <v>127</v>
+        <v>258</v>
       </c>
       <c r="U10" s="10" t="s">
-        <v>168</v>
+        <v>172</v>
       </c>
     </row>
     <row r="11" spans="1:21" ht="30" x14ac:dyDescent="0.25">
@@ -2053,20 +2057,20 @@
         <v>17</v>
       </c>
       <c r="B11" s="12" t="s">
-        <v>148</v>
+        <v>136</v>
       </c>
       <c r="C11" s="13" t="s">
-        <v>149</v>
+        <v>137</v>
       </c>
       <c r="D11" s="14" t="s">
-        <v>169</v>
+        <v>157</v>
       </c>
       <c r="E11" s="12" t="s">
-        <v>172</v>
+        <v>160</v>
       </c>
       <c r="F11" s="9"/>
       <c r="G11" s="17" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
       <c r="H11" s="18">
         <v>7</v>
@@ -2075,7 +2079,7 @@
         <v>20</v>
       </c>
       <c r="J11" s="27" t="s">
-        <v>174</v>
+        <v>161</v>
       </c>
       <c r="K11" s="7" t="s">
         <v>19</v>
@@ -2092,19 +2096,19 @@
         <v>19</v>
       </c>
       <c r="Q11" s="10" t="s">
-        <v>166</v>
+        <v>154</v>
       </c>
       <c r="R11" s="11" t="s">
-        <v>167</v>
+        <v>155</v>
       </c>
       <c r="S11" s="10" t="s">
-        <v>149</v>
+        <v>137</v>
       </c>
       <c r="T11" s="29" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
       <c r="U11" s="10" t="s">
-        <v>168</v>
+        <v>156</v>
       </c>
     </row>
     <row r="12" spans="1:21" ht="30" x14ac:dyDescent="0.25">
@@ -2112,20 +2116,20 @@
         <v>17</v>
       </c>
       <c r="B12" s="12" t="s">
-        <v>148</v>
+        <v>136</v>
       </c>
       <c r="C12" s="13" t="s">
-        <v>149</v>
+        <v>137</v>
       </c>
       <c r="D12" s="14" t="s">
-        <v>169</v>
+        <v>157</v>
       </c>
       <c r="E12" s="12" t="s">
-        <v>172</v>
+        <v>160</v>
       </c>
       <c r="F12" s="9"/>
       <c r="G12" s="17" t="s">
-        <v>129</v>
+        <v>243</v>
       </c>
       <c r="H12" s="18">
         <v>8</v>
@@ -2134,7 +2138,7 @@
         <v>20</v>
       </c>
       <c r="J12" s="27" t="s">
-        <v>175</v>
+        <v>244</v>
       </c>
       <c r="K12" s="7" t="s">
         <v>20</v>
@@ -2154,16 +2158,16 @@
         <v>6</v>
       </c>
       <c r="R12" s="11" t="s">
-        <v>153</v>
+        <v>141</v>
       </c>
       <c r="S12" s="10" t="s">
-        <v>157</v>
+        <v>145</v>
       </c>
       <c r="T12" s="29" t="s">
-        <v>176</v>
+        <v>162</v>
       </c>
       <c r="U12" s="10" t="s">
-        <v>159</v>
+        <v>147</v>
       </c>
     </row>
     <row r="13" spans="1:21" ht="30" x14ac:dyDescent="0.25">
@@ -2171,20 +2175,20 @@
         <v>17</v>
       </c>
       <c r="B13" s="12" t="s">
-        <v>148</v>
+        <v>136</v>
       </c>
       <c r="C13" s="13" t="s">
-        <v>149</v>
+        <v>137</v>
       </c>
       <c r="D13" s="14" t="s">
-        <v>169</v>
+        <v>157</v>
       </c>
       <c r="E13" s="12" t="s">
-        <v>162</v>
+        <v>150</v>
       </c>
       <c r="F13" s="9"/>
       <c r="G13" s="17" t="s">
-        <v>130</v>
+        <v>128</v>
       </c>
       <c r="H13" s="18">
         <v>9</v>
@@ -2193,7 +2197,7 @@
         <v>20</v>
       </c>
       <c r="J13" s="27" t="s">
-        <v>262</v>
+        <v>237</v>
       </c>
       <c r="K13" s="7" t="s">
         <v>19</v>
@@ -2210,19 +2214,19 @@
         <v>19</v>
       </c>
       <c r="Q13" s="10" t="s">
-        <v>166</v>
+        <v>154</v>
       </c>
       <c r="R13" s="11" t="s">
-        <v>167</v>
+        <v>155</v>
       </c>
       <c r="S13" s="10" t="s">
-        <v>149</v>
+        <v>137</v>
       </c>
       <c r="T13" s="29" t="s">
-        <v>130</v>
+        <v>128</v>
       </c>
       <c r="U13" s="10" t="s">
-        <v>168</v>
+        <v>156</v>
       </c>
     </row>
     <row r="14" spans="1:21" ht="30" x14ac:dyDescent="0.25">
@@ -2230,20 +2234,20 @@
         <v>17</v>
       </c>
       <c r="B14" s="12" t="s">
-        <v>148</v>
+        <v>136</v>
       </c>
       <c r="C14" s="13" t="s">
-        <v>149</v>
+        <v>137</v>
       </c>
       <c r="D14" s="14" t="s">
-        <v>178</v>
+        <v>164</v>
       </c>
       <c r="E14" s="12" t="s">
-        <v>179</v>
+        <v>165</v>
       </c>
       <c r="F14" s="9"/>
       <c r="G14" s="20" t="s">
-        <v>131</v>
+        <v>245</v>
       </c>
       <c r="H14" s="21">
         <v>10</v>
@@ -2252,7 +2256,7 @@
         <v>20</v>
       </c>
       <c r="J14" s="28" t="s">
-        <v>180</v>
+        <v>166</v>
       </c>
       <c r="K14" s="23" t="s">
         <v>20</v>
@@ -2272,16 +2276,16 @@
         <v>6</v>
       </c>
       <c r="R14" s="11" t="s">
-        <v>153</v>
+        <v>141</v>
       </c>
       <c r="S14" s="10" t="s">
-        <v>157</v>
+        <v>145</v>
       </c>
       <c r="T14" s="29" t="s">
-        <v>181</v>
+        <v>238</v>
       </c>
       <c r="U14" s="10" t="s">
-        <v>159</v>
+        <v>147</v>
       </c>
     </row>
     <row r="15" spans="1:21" ht="30" x14ac:dyDescent="0.25">
@@ -2289,20 +2293,20 @@
         <v>17</v>
       </c>
       <c r="B15" s="12" t="s">
-        <v>148</v>
+        <v>136</v>
       </c>
       <c r="C15" s="13" t="s">
-        <v>149</v>
+        <v>137</v>
       </c>
       <c r="D15" s="14" t="s">
-        <v>178</v>
+        <v>164</v>
       </c>
       <c r="E15" s="12" t="s">
-        <v>182</v>
+        <v>168</v>
       </c>
       <c r="F15" s="9"/>
       <c r="G15" s="17" t="s">
-        <v>132</v>
+        <v>246</v>
       </c>
       <c r="H15" s="18">
         <v>11</v>
@@ -2311,7 +2315,7 @@
         <v>19</v>
       </c>
       <c r="J15" s="27" t="s">
-        <v>183</v>
+        <v>247</v>
       </c>
       <c r="K15" s="7" t="s">
         <v>20</v>
@@ -2331,16 +2335,16 @@
         <v>6</v>
       </c>
       <c r="R15" s="11" t="s">
-        <v>184</v>
+        <v>169</v>
       </c>
       <c r="S15" s="10" t="s">
-        <v>185</v>
+        <v>170</v>
       </c>
       <c r="T15" s="29" t="s">
-        <v>186</v>
+        <v>171</v>
       </c>
       <c r="U15" s="10" t="s">
-        <v>187</v>
+        <v>172</v>
       </c>
     </row>
     <row r="16" spans="1:21" ht="30" x14ac:dyDescent="0.25">
@@ -2348,20 +2352,20 @@
         <v>17</v>
       </c>
       <c r="B16" s="12" t="s">
-        <v>148</v>
+        <v>136</v>
       </c>
       <c r="C16" s="13" t="s">
-        <v>149</v>
+        <v>137</v>
       </c>
       <c r="D16" s="14" t="s">
-        <v>178</v>
+        <v>164</v>
       </c>
       <c r="E16" s="12" t="s">
-        <v>182</v>
+        <v>168</v>
       </c>
       <c r="F16" s="9"/>
       <c r="G16" s="17" t="s">
-        <v>133</v>
+        <v>248</v>
       </c>
       <c r="H16" s="18">
         <v>12</v>
@@ -2370,7 +2374,7 @@
         <v>20</v>
       </c>
       <c r="J16" s="27" t="s">
-        <v>188</v>
+        <v>173</v>
       </c>
       <c r="K16" s="7" t="s">
         <v>20</v>
@@ -2390,16 +2394,16 @@
         <v>6</v>
       </c>
       <c r="R16" s="11" t="s">
-        <v>153</v>
+        <v>141</v>
       </c>
       <c r="S16" s="10" t="s">
-        <v>157</v>
+        <v>145</v>
       </c>
       <c r="T16" s="29" t="s">
-        <v>189</v>
+        <v>174</v>
       </c>
       <c r="U16" s="10" t="s">
-        <v>159</v>
+        <v>147</v>
       </c>
     </row>
     <row r="17" spans="1:21" ht="30" x14ac:dyDescent="0.25">
@@ -2407,20 +2411,20 @@
         <v>17</v>
       </c>
       <c r="B17" s="12" t="s">
-        <v>148</v>
+        <v>136</v>
       </c>
       <c r="C17" s="13" t="s">
-        <v>149</v>
+        <v>137</v>
       </c>
       <c r="D17" s="14" t="s">
-        <v>178</v>
+        <v>164</v>
       </c>
       <c r="E17" s="12" t="s">
-        <v>182</v>
+        <v>168</v>
       </c>
       <c r="F17" s="9"/>
       <c r="G17" s="17" t="s">
-        <v>134</v>
+        <v>129</v>
       </c>
       <c r="H17" s="18">
         <v>13</v>
@@ -2429,7 +2433,7 @@
         <v>20</v>
       </c>
       <c r="J17" s="27" t="s">
-        <v>190</v>
+        <v>175</v>
       </c>
       <c r="K17" s="7" t="s">
         <v>20</v>
@@ -2449,16 +2453,16 @@
         <v>6</v>
       </c>
       <c r="R17" s="11" t="s">
-        <v>153</v>
+        <v>141</v>
       </c>
       <c r="S17" s="10" t="s">
-        <v>157</v>
+        <v>145</v>
       </c>
       <c r="T17" s="29" t="s">
-        <v>191</v>
+        <v>176</v>
       </c>
       <c r="U17" s="10" t="s">
-        <v>159</v>
+        <v>147</v>
       </c>
     </row>
     <row r="18" spans="1:21" ht="30" x14ac:dyDescent="0.25">
@@ -2466,22 +2470,22 @@
         <v>17</v>
       </c>
       <c r="B18" s="12" t="s">
-        <v>148</v>
+        <v>136</v>
       </c>
       <c r="C18" s="13" t="s">
-        <v>149</v>
+        <v>137</v>
       </c>
       <c r="D18" s="14" t="s">
-        <v>178</v>
+        <v>164</v>
       </c>
       <c r="E18" s="12" t="s">
-        <v>143</v>
+        <v>131</v>
       </c>
       <c r="F18" s="9" t="s">
-        <v>192</v>
+        <v>177</v>
       </c>
       <c r="G18" s="17" t="s">
-        <v>135</v>
+        <v>249</v>
       </c>
       <c r="H18" s="18">
         <v>14</v>
@@ -2490,7 +2494,7 @@
         <v>19</v>
       </c>
       <c r="J18" s="27" t="s">
-        <v>193</v>
+        <v>178</v>
       </c>
       <c r="K18" s="7" t="s">
         <v>20</v>
@@ -2510,16 +2514,16 @@
         <v>6</v>
       </c>
       <c r="R18" s="11" t="s">
-        <v>184</v>
+        <v>169</v>
       </c>
       <c r="S18" s="10" t="s">
-        <v>185</v>
+        <v>170</v>
       </c>
       <c r="T18" s="29" t="s">
-        <v>194</v>
+        <v>179</v>
       </c>
       <c r="U18" s="10" t="s">
-        <v>187</v>
+        <v>172</v>
       </c>
     </row>
     <row r="19" spans="1:21" ht="30" x14ac:dyDescent="0.25">
@@ -2527,22 +2531,22 @@
         <v>17</v>
       </c>
       <c r="B19" s="12" t="s">
-        <v>148</v>
+        <v>136</v>
       </c>
       <c r="C19" s="13" t="s">
-        <v>149</v>
+        <v>137</v>
       </c>
       <c r="D19" s="14" t="s">
-        <v>178</v>
+        <v>164</v>
       </c>
       <c r="E19" s="12" t="s">
-        <v>143</v>
+        <v>131</v>
       </c>
       <c r="F19" s="9" t="s">
-        <v>192</v>
+        <v>177</v>
       </c>
       <c r="G19" s="17" t="s">
-        <v>136</v>
+        <v>250</v>
       </c>
       <c r="H19" s="18">
         <v>15</v>
@@ -2551,7 +2555,7 @@
         <v>20</v>
       </c>
       <c r="J19" s="27" t="s">
-        <v>195</v>
+        <v>180</v>
       </c>
       <c r="K19" s="7" t="s">
         <v>20</v>
@@ -2571,39 +2575,39 @@
         <v>6</v>
       </c>
       <c r="R19" s="11" t="s">
-        <v>153</v>
+        <v>141</v>
       </c>
       <c r="S19" s="10" t="s">
-        <v>157</v>
+        <v>145</v>
       </c>
       <c r="T19" s="29" t="s">
-        <v>196</v>
+        <v>181</v>
       </c>
       <c r="U19" s="10" t="s">
-        <v>159</v>
-      </c>
-    </row>
-    <row r="20" spans="1:21" ht="30" x14ac:dyDescent="0.25">
+        <v>147</v>
+      </c>
+    </row>
+    <row r="20" spans="1:21" ht="45" x14ac:dyDescent="0.25">
       <c r="A20" s="4" t="s">
         <v>17</v>
       </c>
       <c r="B20" s="12" t="s">
-        <v>148</v>
+        <v>136</v>
       </c>
       <c r="C20" s="13" t="s">
-        <v>149</v>
+        <v>137</v>
       </c>
       <c r="D20" s="14" t="s">
-        <v>178</v>
+        <v>164</v>
       </c>
       <c r="E20" s="12" t="s">
-        <v>143</v>
+        <v>131</v>
       </c>
       <c r="F20" s="9" t="s">
-        <v>200</v>
+        <v>184</v>
       </c>
       <c r="G20" s="17" t="s">
-        <v>137</v>
+        <v>251</v>
       </c>
       <c r="H20" s="18">
         <v>16</v>
@@ -2612,7 +2616,7 @@
         <v>20</v>
       </c>
       <c r="J20" s="27" t="s">
-        <v>197</v>
+        <v>252</v>
       </c>
       <c r="K20" s="7" t="s">
         <v>20</v>
@@ -2632,16 +2636,16 @@
         <v>6</v>
       </c>
       <c r="R20" s="11" t="s">
-        <v>153</v>
+        <v>141</v>
       </c>
       <c r="S20" s="10" t="s">
-        <v>157</v>
+        <v>145</v>
       </c>
       <c r="T20" s="29" t="s">
-        <v>198</v>
+        <v>182</v>
       </c>
       <c r="U20" s="10" t="s">
-        <v>159</v>
+        <v>147</v>
       </c>
     </row>
     <row r="21" spans="1:21" ht="30" x14ac:dyDescent="0.25">
@@ -2649,22 +2653,22 @@
         <v>17</v>
       </c>
       <c r="B21" s="12" t="s">
-        <v>148</v>
+        <v>136</v>
       </c>
       <c r="C21" s="13" t="s">
-        <v>149</v>
+        <v>137</v>
       </c>
       <c r="D21" s="14" t="s">
-        <v>178</v>
+        <v>164</v>
       </c>
       <c r="E21" s="12" t="s">
-        <v>143</v>
+        <v>131</v>
       </c>
       <c r="F21" s="9" t="s">
-        <v>199</v>
+        <v>183</v>
       </c>
       <c r="G21" s="17" t="s">
-        <v>138</v>
+        <v>253</v>
       </c>
       <c r="H21" s="18">
         <v>17</v>
@@ -2673,7 +2677,7 @@
         <v>20</v>
       </c>
       <c r="J21" s="27" t="s">
-        <v>201</v>
+        <v>254</v>
       </c>
       <c r="K21" s="7" t="s">
         <v>20</v>
@@ -2693,16 +2697,16 @@
         <v>6</v>
       </c>
       <c r="R21" s="11" t="s">
+        <v>141</v>
+      </c>
+      <c r="S21" s="10" t="s">
+        <v>145</v>
+      </c>
+      <c r="T21" s="29" t="s">
         <v>153</v>
       </c>
-      <c r="S21" s="10" t="s">
-        <v>157</v>
-      </c>
-      <c r="T21" s="29" t="s">
-        <v>177</v>
-      </c>
       <c r="U21" s="10" t="s">
-        <v>159</v>
+        <v>147</v>
       </c>
     </row>
     <row r="22" spans="1:21" ht="30" x14ac:dyDescent="0.25">
@@ -2710,22 +2714,22 @@
         <v>17</v>
       </c>
       <c r="B22" s="12" t="s">
-        <v>148</v>
+        <v>136</v>
       </c>
       <c r="C22" s="13" t="s">
-        <v>149</v>
+        <v>137</v>
       </c>
       <c r="D22" s="14" t="s">
-        <v>178</v>
+        <v>164</v>
       </c>
       <c r="E22" s="12" t="s">
-        <v>143</v>
+        <v>131</v>
       </c>
       <c r="F22" s="9" t="s">
-        <v>199</v>
+        <v>183</v>
       </c>
       <c r="G22" s="17" t="s">
-        <v>139</v>
+        <v>256</v>
       </c>
       <c r="H22" s="18">
         <v>18</v>
@@ -2734,7 +2738,7 @@
         <v>20</v>
       </c>
       <c r="J22" s="27" t="s">
-        <v>202</v>
+        <v>255</v>
       </c>
       <c r="K22" s="7" t="s">
         <v>20</v>
@@ -2754,39 +2758,39 @@
         <v>6</v>
       </c>
       <c r="R22" s="11" t="s">
-        <v>153</v>
+        <v>141</v>
       </c>
       <c r="S22" s="10" t="s">
-        <v>157</v>
+        <v>145</v>
       </c>
       <c r="T22" s="29" t="s">
-        <v>204</v>
+        <v>186</v>
       </c>
       <c r="U22" s="10" t="s">
-        <v>159</v>
-      </c>
-    </row>
-    <row r="23" spans="1:21" ht="45" x14ac:dyDescent="0.25">
+        <v>147</v>
+      </c>
+    </row>
+    <row r="23" spans="1:21" ht="30" x14ac:dyDescent="0.25">
       <c r="A23" s="4" t="s">
         <v>17</v>
       </c>
       <c r="B23" s="12" t="s">
-        <v>148</v>
+        <v>136</v>
       </c>
       <c r="C23" s="13" t="s">
-        <v>149</v>
+        <v>137</v>
       </c>
       <c r="D23" s="14" t="s">
-        <v>178</v>
+        <v>164</v>
       </c>
       <c r="E23" s="12" t="s">
-        <v>143</v>
+        <v>131</v>
       </c>
       <c r="F23" s="9" t="s">
-        <v>205</v>
+        <v>187</v>
       </c>
       <c r="G23" s="17" t="s">
-        <v>140</v>
+        <v>261</v>
       </c>
       <c r="H23" s="18">
         <v>19</v>
@@ -2795,36 +2799,36 @@
         <v>19</v>
       </c>
       <c r="J23" s="27" t="s">
-        <v>206</v>
+        <v>257</v>
       </c>
       <c r="K23" s="7" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="L23" s="6" t="s">
         <v>5</v>
       </c>
       <c r="M23" s="8" t="s">
-        <v>62</v>
+        <v>57</v>
       </c>
       <c r="N23" s="8"/>
       <c r="O23" s="9"/>
-      <c r="P23" s="18" t="s">
+      <c r="P23" s="21" t="s">
         <v>19</v>
       </c>
-      <c r="Q23" s="10" t="s">
-        <v>166</v>
+      <c r="Q23" s="10">
+        <v>6</v>
       </c>
       <c r="R23" s="11" t="s">
-        <v>167</v>
+        <v>169</v>
       </c>
       <c r="S23" s="10" t="s">
-        <v>149</v>
+        <v>170</v>
       </c>
       <c r="T23" s="29" t="s">
-        <v>140</v>
+        <v>242</v>
       </c>
       <c r="U23" s="10" t="s">
-        <v>168</v>
+        <v>172</v>
       </c>
     </row>
     <row r="24" spans="1:21" ht="30" x14ac:dyDescent="0.25">
@@ -2832,22 +2836,22 @@
         <v>17</v>
       </c>
       <c r="B24" s="12" t="s">
-        <v>148</v>
+        <v>136</v>
       </c>
       <c r="C24" s="13" t="s">
-        <v>149</v>
+        <v>137</v>
       </c>
       <c r="D24" s="14" t="s">
-        <v>178</v>
+        <v>164</v>
       </c>
       <c r="E24" s="12" t="s">
-        <v>143</v>
+        <v>131</v>
       </c>
       <c r="F24" s="9" t="s">
-        <v>205</v>
+        <v>187</v>
       </c>
       <c r="G24" s="17" t="s">
-        <v>141</v>
+        <v>259</v>
       </c>
       <c r="H24" s="18">
         <v>20</v>
@@ -2856,7 +2860,7 @@
         <v>20</v>
       </c>
       <c r="J24" s="27" t="s">
-        <v>207</v>
+        <v>260</v>
       </c>
       <c r="K24" s="7" t="s">
         <v>20</v>
@@ -2876,16 +2880,16 @@
         <v>6</v>
       </c>
       <c r="R24" s="11" t="s">
-        <v>153</v>
+        <v>141</v>
       </c>
       <c r="S24" s="10" t="s">
-        <v>157</v>
+        <v>145</v>
       </c>
       <c r="T24" s="29" t="s">
-        <v>208</v>
+        <v>188</v>
       </c>
       <c r="U24" s="10" t="s">
-        <v>159</v>
+        <v>147</v>
       </c>
     </row>
     <row r="25" spans="1:21" ht="45" x14ac:dyDescent="0.25">
@@ -2893,22 +2897,22 @@
         <v>17</v>
       </c>
       <c r="B25" s="12" t="s">
-        <v>148</v>
+        <v>136</v>
       </c>
       <c r="C25" s="13" t="s">
-        <v>149</v>
+        <v>137</v>
       </c>
       <c r="D25" s="14" t="s">
-        <v>178</v>
+        <v>164</v>
       </c>
       <c r="E25" s="12" t="s">
-        <v>143</v>
+        <v>131</v>
       </c>
       <c r="F25" s="9" t="s">
-        <v>205</v>
+        <v>187</v>
       </c>
       <c r="G25" s="17" t="s">
-        <v>178</v>
+        <v>164</v>
       </c>
       <c r="H25" s="18">
         <v>21</v>
@@ -2917,7 +2921,7 @@
         <v>20</v>
       </c>
       <c r="J25" s="27" t="s">
-        <v>237</v>
+        <v>212</v>
       </c>
       <c r="K25" s="7" t="s">
         <v>20</v>
@@ -2937,16 +2941,16 @@
         <v>6</v>
       </c>
       <c r="R25" s="11" t="s">
-        <v>153</v>
+        <v>141</v>
       </c>
       <c r="S25" s="10" t="s">
-        <v>157</v>
+        <v>145</v>
       </c>
       <c r="T25" s="29" t="s">
-        <v>203</v>
+        <v>163</v>
       </c>
       <c r="U25" s="10" t="s">
-        <v>159</v>
+        <v>147</v>
       </c>
     </row>
     <row r="26" spans="1:21" ht="30" x14ac:dyDescent="0.25">
@@ -2954,20 +2958,20 @@
         <v>17</v>
       </c>
       <c r="B26" s="12" t="s">
-        <v>148</v>
+        <v>136</v>
       </c>
       <c r="C26" s="13" t="s">
-        <v>149</v>
+        <v>137</v>
       </c>
       <c r="D26" s="14" t="s">
-        <v>178</v>
+        <v>164</v>
       </c>
       <c r="E26" s="12" t="s">
-        <v>162</v>
+        <v>150</v>
       </c>
       <c r="F26" s="9"/>
       <c r="G26" s="17" t="s">
-        <v>142</v>
+        <v>130</v>
       </c>
       <c r="H26" s="18">
         <v>22</v>
@@ -2976,7 +2980,7 @@
         <v>20</v>
       </c>
       <c r="J26" s="27" t="s">
-        <v>209</v>
+        <v>189</v>
       </c>
       <c r="K26" s="7" t="s">
         <v>20</v>
@@ -2996,16 +3000,16 @@
         <v>6</v>
       </c>
       <c r="R26" s="11" t="s">
-        <v>153</v>
+        <v>141</v>
       </c>
       <c r="S26" s="10" t="s">
-        <v>157</v>
+        <v>145</v>
       </c>
       <c r="T26" s="29" t="s">
-        <v>211</v>
+        <v>191</v>
       </c>
       <c r="U26" s="10" t="s">
-        <v>159</v>
+        <v>147</v>
       </c>
     </row>
     <row r="27" spans="1:21" ht="30" x14ac:dyDescent="0.25">
@@ -3013,20 +3017,20 @@
         <v>17</v>
       </c>
       <c r="B27" s="12" t="s">
-        <v>148</v>
+        <v>136</v>
       </c>
       <c r="C27" s="13" t="s">
-        <v>149</v>
+        <v>137</v>
       </c>
       <c r="D27" s="14" t="s">
-        <v>178</v>
+        <v>164</v>
       </c>
       <c r="E27" s="12" t="s">
-        <v>162</v>
+        <v>150</v>
       </c>
       <c r="F27" s="9"/>
       <c r="G27" s="17" t="s">
-        <v>236</v>
+        <v>211</v>
       </c>
       <c r="H27" s="18">
         <v>23</v>
@@ -3035,7 +3039,7 @@
         <v>20</v>
       </c>
       <c r="J27" s="27" t="s">
-        <v>210</v>
+        <v>190</v>
       </c>
       <c r="K27" s="7" t="s">
         <v>20</v>
@@ -3055,16 +3059,16 @@
         <v>6</v>
       </c>
       <c r="R27" s="11" t="s">
-        <v>153</v>
+        <v>141</v>
       </c>
       <c r="S27" s="10" t="s">
-        <v>157</v>
+        <v>145</v>
       </c>
       <c r="T27" s="29" t="s">
-        <v>212</v>
+        <v>192</v>
       </c>
       <c r="U27" s="10" t="s">
-        <v>159</v>
+        <v>147</v>
       </c>
     </row>
     <row r="28" spans="1:21" ht="30" x14ac:dyDescent="0.25">
@@ -3072,20 +3076,20 @@
         <v>17</v>
       </c>
       <c r="B28" s="12" t="s">
-        <v>148</v>
+        <v>136</v>
       </c>
       <c r="C28" s="13" t="s">
-        <v>149</v>
+        <v>137</v>
       </c>
       <c r="D28" s="14" t="s">
-        <v>213</v>
+        <v>193</v>
       </c>
       <c r="E28" s="12" t="s">
-        <v>162</v>
+        <v>150</v>
       </c>
       <c r="F28" s="9"/>
       <c r="G28" s="17" t="s">
-        <v>144</v>
+        <v>132</v>
       </c>
       <c r="H28" s="18">
         <v>24</v>
@@ -3094,7 +3098,7 @@
         <v>20</v>
       </c>
       <c r="J28" s="27" t="s">
-        <v>214</v>
+        <v>194</v>
       </c>
       <c r="K28" s="7" t="s">
         <v>20</v>
@@ -3114,16 +3118,16 @@
         <v>6</v>
       </c>
       <c r="R28" s="11" t="s">
-        <v>153</v>
+        <v>141</v>
       </c>
       <c r="S28" s="10" t="s">
-        <v>157</v>
+        <v>145</v>
       </c>
       <c r="T28" s="29" t="s">
-        <v>216</v>
+        <v>195</v>
       </c>
       <c r="U28" s="10" t="s">
-        <v>159</v>
+        <v>147</v>
       </c>
     </row>
     <row r="29" spans="1:21" ht="45" x14ac:dyDescent="0.25">
@@ -3131,18 +3135,18 @@
         <v>17</v>
       </c>
       <c r="B29" s="12" t="s">
-        <v>148</v>
+        <v>136</v>
       </c>
       <c r="C29" s="13" t="s">
-        <v>149</v>
+        <v>137</v>
       </c>
       <c r="D29" s="14" t="s">
-        <v>217</v>
+        <v>196</v>
       </c>
       <c r="E29" s="12"/>
       <c r="F29" s="9"/>
       <c r="G29" s="20" t="s">
-        <v>145</v>
+        <v>133</v>
       </c>
       <c r="H29" s="21">
         <v>25</v>
@@ -3151,7 +3155,7 @@
         <v>20</v>
       </c>
       <c r="J29" s="28" t="s">
-        <v>218</v>
+        <v>263</v>
       </c>
       <c r="K29" s="23" t="s">
         <v>19</v>
@@ -3164,44 +3168,44 @@
         <v>120</v>
       </c>
       <c r="O29" s="9" t="s">
-        <v>233</v>
+        <v>209</v>
       </c>
       <c r="P29" s="21" t="s">
         <v>19</v>
       </c>
       <c r="Q29" s="10" t="s">
-        <v>221</v>
+        <v>198</v>
       </c>
       <c r="R29" s="11" t="s">
-        <v>222</v>
+        <v>199</v>
       </c>
       <c r="S29" s="10" t="s">
-        <v>149</v>
+        <v>137</v>
       </c>
       <c r="T29" s="29" t="s">
-        <v>145</v>
+        <v>133</v>
       </c>
       <c r="U29" s="10" t="s">
-        <v>223</v>
-      </c>
-    </row>
-    <row r="30" spans="1:21" ht="45" x14ac:dyDescent="0.25">
+        <v>200</v>
+      </c>
+    </row>
+    <row r="30" spans="1:21" ht="30" x14ac:dyDescent="0.25">
       <c r="A30" s="4" t="s">
         <v>17</v>
       </c>
       <c r="B30" s="12" t="s">
-        <v>148</v>
+        <v>136</v>
       </c>
       <c r="C30" s="13" t="s">
-        <v>149</v>
+        <v>137</v>
       </c>
       <c r="D30" s="14" t="s">
-        <v>217</v>
+        <v>196</v>
       </c>
       <c r="E30" s="12"/>
       <c r="F30" s="9"/>
       <c r="G30" s="17" t="s">
-        <v>146</v>
+        <v>134</v>
       </c>
       <c r="H30" s="21">
         <v>26</v>
@@ -3210,7 +3214,7 @@
         <v>20</v>
       </c>
       <c r="J30" s="28" t="s">
-        <v>219</v>
+        <v>262</v>
       </c>
       <c r="K30" s="23" t="s">
         <v>19</v>
@@ -3222,24 +3226,26 @@
       <c r="N30" s="25" t="s">
         <v>120</v>
       </c>
-      <c r="O30" s="26"/>
+      <c r="O30" s="9" t="s">
+        <v>209</v>
+      </c>
       <c r="P30" s="21" t="s">
         <v>19</v>
       </c>
       <c r="Q30" s="10" t="s">
-        <v>221</v>
+        <v>198</v>
       </c>
       <c r="R30" s="11" t="s">
-        <v>222</v>
+        <v>199</v>
       </c>
       <c r="S30" s="10" t="s">
-        <v>149</v>
+        <v>137</v>
       </c>
       <c r="T30" s="29" t="s">
-        <v>146</v>
+        <v>134</v>
       </c>
       <c r="U30" s="10" t="s">
-        <v>223</v>
+        <v>200</v>
       </c>
     </row>
     <row r="31" spans="1:21" ht="30" x14ac:dyDescent="0.25">
@@ -3247,18 +3253,18 @@
         <v>17</v>
       </c>
       <c r="B31" s="12" t="s">
-        <v>148</v>
+        <v>136</v>
       </c>
       <c r="C31" s="13" t="s">
-        <v>149</v>
+        <v>137</v>
       </c>
       <c r="D31" s="14" t="s">
-        <v>217</v>
+        <v>196</v>
       </c>
       <c r="E31" s="12"/>
       <c r="F31" s="9"/>
       <c r="G31" s="17" t="s">
-        <v>147</v>
+        <v>135</v>
       </c>
       <c r="H31" s="18">
         <v>27</v>
@@ -3267,7 +3273,7 @@
         <v>20</v>
       </c>
       <c r="J31" s="27" t="s">
-        <v>220</v>
+        <v>197</v>
       </c>
       <c r="K31" s="23" t="s">
         <v>19</v>
@@ -3284,19 +3290,19 @@
         <v>19</v>
       </c>
       <c r="Q31" s="10" t="s">
-        <v>166</v>
+        <v>154</v>
       </c>
       <c r="R31" s="11" t="s">
-        <v>167</v>
+        <v>155</v>
       </c>
       <c r="S31" s="10" t="s">
-        <v>149</v>
+        <v>137</v>
       </c>
       <c r="T31" s="29" t="s">
-        <v>147</v>
+        <v>135</v>
       </c>
       <c r="U31" s="10" t="s">
-        <v>168</v>
+        <v>156</v>
       </c>
     </row>
     <row r="32" spans="1:21" ht="60" x14ac:dyDescent="0.25">
@@ -3304,18 +3310,18 @@
         <v>17</v>
       </c>
       <c r="B32" s="12" t="s">
-        <v>148</v>
+        <v>136</v>
       </c>
       <c r="C32" s="13" t="s">
-        <v>149</v>
+        <v>137</v>
       </c>
       <c r="D32" s="14" t="s">
-        <v>217</v>
+        <v>196</v>
       </c>
       <c r="E32" s="12"/>
       <c r="F32" s="9"/>
       <c r="G32" s="17" t="s">
-        <v>224</v>
+        <v>201</v>
       </c>
       <c r="H32" s="18">
         <v>28</v>
@@ -3324,7 +3330,7 @@
         <v>20</v>
       </c>
       <c r="J32" s="27" t="s">
-        <v>227</v>
+        <v>203</v>
       </c>
       <c r="K32" s="7" t="s">
         <v>19</v>
@@ -3337,25 +3343,25 @@
         <v>120</v>
       </c>
       <c r="O32" s="9" t="s">
-        <v>240</v>
+        <v>215</v>
       </c>
       <c r="P32" s="18" t="s">
         <v>19</v>
       </c>
       <c r="Q32" s="10" t="s">
-        <v>166</v>
+        <v>154</v>
       </c>
       <c r="R32" s="11" t="s">
-        <v>167</v>
+        <v>155</v>
       </c>
       <c r="S32" s="10" t="s">
-        <v>149</v>
+        <v>137</v>
       </c>
       <c r="T32" s="29" t="s">
-        <v>224</v>
+        <v>201</v>
       </c>
       <c r="U32" s="10" t="s">
-        <v>168</v>
+        <v>156</v>
       </c>
     </row>
     <row r="33" spans="1:21" ht="45" x14ac:dyDescent="0.25">
@@ -3363,18 +3369,18 @@
         <v>17</v>
       </c>
       <c r="B33" s="12" t="s">
-        <v>148</v>
+        <v>136</v>
       </c>
       <c r="C33" s="13" t="s">
-        <v>149</v>
+        <v>137</v>
       </c>
       <c r="D33" s="14" t="s">
-        <v>217</v>
+        <v>196</v>
       </c>
       <c r="E33" s="12"/>
       <c r="F33" s="9"/>
       <c r="G33" s="17" t="s">
-        <v>225</v>
+        <v>202</v>
       </c>
       <c r="H33" s="18">
         <v>29</v>
@@ -3383,7 +3389,7 @@
         <v>20</v>
       </c>
       <c r="J33" s="27" t="s">
-        <v>226</v>
+        <v>264</v>
       </c>
       <c r="K33" s="7" t="s">
         <v>19</v>
@@ -3395,24 +3401,26 @@
       <c r="N33" s="25" t="s">
         <v>120</v>
       </c>
-      <c r="O33" s="9"/>
+      <c r="O33" s="9" t="s">
+        <v>209</v>
+      </c>
       <c r="P33" s="18" t="s">
         <v>19</v>
       </c>
       <c r="Q33" s="10" t="s">
-        <v>166</v>
+        <v>154</v>
       </c>
       <c r="R33" s="11" t="s">
-        <v>167</v>
+        <v>155</v>
       </c>
       <c r="S33" s="10" t="s">
-        <v>149</v>
+        <v>137</v>
       </c>
       <c r="T33" s="29" t="s">
-        <v>225</v>
+        <v>202</v>
       </c>
       <c r="U33" s="10" t="s">
-        <v>168</v>
+        <v>156</v>
       </c>
     </row>
     <row r="34" spans="1:21" ht="15.75" x14ac:dyDescent="0.25">
@@ -3420,13 +3428,13 @@
         <v>17</v>
       </c>
       <c r="B34" s="12" t="s">
-        <v>148</v>
+        <v>136</v>
       </c>
       <c r="C34" s="13" t="s">
-        <v>149</v>
+        <v>137</v>
       </c>
       <c r="D34" s="31" t="s">
-        <v>228</v>
+        <v>204</v>
       </c>
       <c r="E34" s="12"/>
       <c r="F34" s="9"/>
@@ -3440,7 +3448,7 @@
         <v>20</v>
       </c>
       <c r="J34" s="27" t="s">
-        <v>230</v>
+        <v>206</v>
       </c>
       <c r="K34" s="7" t="s">
         <v>20</v>
@@ -3465,18 +3473,18 @@
         <v>17</v>
       </c>
       <c r="B35" s="12" t="s">
-        <v>148</v>
+        <v>136</v>
       </c>
       <c r="C35" s="13" t="s">
-        <v>149</v>
+        <v>137</v>
       </c>
       <c r="D35" s="31" t="s">
-        <v>228</v>
+        <v>204</v>
       </c>
       <c r="E35" s="12"/>
       <c r="F35" s="9"/>
       <c r="G35" s="17" t="s">
-        <v>229</v>
+        <v>205</v>
       </c>
       <c r="H35" s="18">
         <v>31</v>
@@ -3485,7 +3493,7 @@
         <v>20</v>
       </c>
       <c r="J35" s="27" t="s">
-        <v>231</v>
+        <v>207</v>
       </c>
       <c r="K35" s="7" t="s">
         <v>20</v>
@@ -3505,16 +3513,16 @@
         <v>6</v>
       </c>
       <c r="R35" s="11" t="s">
-        <v>153</v>
+        <v>141</v>
       </c>
       <c r="S35" s="10" t="s">
-        <v>157</v>
+        <v>145</v>
       </c>
       <c r="T35" s="29" t="s">
-        <v>215</v>
+        <v>185</v>
       </c>
       <c r="U35" s="10" t="s">
-        <v>159</v>
+        <v>147</v>
       </c>
     </row>
     <row r="36" spans="1:21" ht="30" x14ac:dyDescent="0.25">
@@ -3522,18 +3530,18 @@
         <v>17</v>
       </c>
       <c r="B36" s="12" t="s">
-        <v>148</v>
+        <v>136</v>
       </c>
       <c r="C36" s="13" t="s">
-        <v>149</v>
+        <v>137</v>
       </c>
       <c r="D36" s="31" t="s">
-        <v>228</v>
+        <v>204</v>
       </c>
       <c r="E36" s="12"/>
       <c r="F36" s="9"/>
       <c r="G36" s="17" t="s">
-        <v>239</v>
+        <v>214</v>
       </c>
       <c r="H36" s="18">
         <v>32</v>
@@ -3542,7 +3550,7 @@
         <v>20</v>
       </c>
       <c r="J36" s="27" t="s">
-        <v>238</v>
+        <v>213</v>
       </c>
       <c r="K36" s="7" t="s">
         <v>20</v>
@@ -3562,16 +3570,16 @@
         <v>6</v>
       </c>
       <c r="R36" s="11" t="s">
-        <v>153</v>
+        <v>141</v>
       </c>
       <c r="S36" s="10" t="s">
-        <v>157</v>
+        <v>145</v>
       </c>
       <c r="T36" s="29" t="s">
-        <v>232</v>
+        <v>208</v>
       </c>
       <c r="U36" s="10" t="s">
-        <v>159</v>
+        <v>147</v>
       </c>
     </row>
     <row r="37" spans="1:21" ht="15.75" x14ac:dyDescent="0.25">
@@ -4739,7 +4747,7 @@
           <x14:formula1>
             <xm:f>DATOS!$D$1:$D$2</xm:f>
           </x14:formula1>
-          <xm:sqref>P3:P69 K3:K69 I3:I69</xm:sqref>
+          <xm:sqref>I3:I69 K3:K69 P3:P69</xm:sqref>
         </x14:dataValidation>
         <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1">
           <x14:formula1>
@@ -4778,193 +4786,193 @@
   <sheetData>
     <row r="2" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A2" s="34" t="s">
-        <v>241</v>
+        <v>216</v>
       </c>
       <c r="B2" s="34" t="s">
-        <v>242</v>
+        <v>217</v>
       </c>
       <c r="C2" s="34" t="s">
-        <v>245</v>
+        <v>220</v>
       </c>
       <c r="D2" s="34" t="s">
-        <v>243</v>
+        <v>218</v>
       </c>
       <c r="E2" s="34" t="s">
-        <v>244</v>
+        <v>219</v>
       </c>
     </row>
     <row r="3" spans="1:5" ht="45" x14ac:dyDescent="0.25">
       <c r="A3" s="35" t="s">
-        <v>169</v>
+        <v>157</v>
       </c>
       <c r="B3" s="36" t="s">
-        <v>170</v>
+        <v>158</v>
       </c>
       <c r="C3" s="42"/>
       <c r="D3" s="37" t="s">
-        <v>249</v>
+        <v>224</v>
       </c>
       <c r="E3" s="38" t="s">
-        <v>246</v>
+        <v>221</v>
       </c>
     </row>
     <row r="4" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A4" s="35" t="s">
-        <v>169</v>
+        <v>157</v>
       </c>
       <c r="B4" s="36" t="s">
-        <v>170</v>
+        <v>158</v>
       </c>
       <c r="C4" s="42"/>
       <c r="D4" s="37" t="s">
-        <v>247</v>
+        <v>222</v>
       </c>
       <c r="E4" s="38"/>
     </row>
     <row r="5" spans="1:5" ht="45" x14ac:dyDescent="0.25">
       <c r="A5" s="35" t="s">
-        <v>169</v>
+        <v>157</v>
       </c>
       <c r="B5" s="36" t="s">
-        <v>171</v>
+        <v>159</v>
       </c>
       <c r="C5" s="42"/>
       <c r="D5" s="37" t="s">
-        <v>248</v>
+        <v>223</v>
       </c>
       <c r="E5" s="38" t="s">
-        <v>250</v>
+        <v>225</v>
       </c>
     </row>
     <row r="6" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A6" s="35" t="s">
-        <v>178</v>
+        <v>164</v>
       </c>
       <c r="B6" s="36" t="s">
-        <v>179</v>
+        <v>165</v>
       </c>
       <c r="C6" s="42"/>
       <c r="D6" s="37" t="s">
-        <v>251</v>
+        <v>226</v>
       </c>
       <c r="E6" s="38"/>
     </row>
     <row r="7" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A7" s="35" t="s">
-        <v>178</v>
+        <v>164</v>
       </c>
       <c r="B7" s="36" t="s">
-        <v>182</v>
+        <v>168</v>
       </c>
       <c r="C7" s="42"/>
       <c r="D7" s="37" t="s">
-        <v>252</v>
+        <v>227</v>
       </c>
       <c r="E7" s="38"/>
     </row>
     <row r="8" spans="1:5" ht="30" x14ac:dyDescent="0.25">
       <c r="A8" s="35" t="s">
-        <v>178</v>
+        <v>164</v>
       </c>
       <c r="B8" s="36" t="s">
-        <v>182</v>
+        <v>168</v>
       </c>
       <c r="C8" s="42"/>
       <c r="D8" s="37" t="s">
-        <v>253</v>
+        <v>228</v>
       </c>
       <c r="E8" s="38"/>
     </row>
     <row r="9" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A9" s="35" t="s">
-        <v>178</v>
+        <v>164</v>
       </c>
       <c r="B9" s="36" t="s">
-        <v>143</v>
+        <v>131</v>
       </c>
       <c r="C9" s="42" t="s">
-        <v>192</v>
+        <v>177</v>
       </c>
       <c r="D9" s="37" t="s">
-        <v>254</v>
+        <v>229</v>
       </c>
       <c r="E9" s="38"/>
     </row>
     <row r="10" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A10" s="35" t="s">
-        <v>178</v>
+        <v>164</v>
       </c>
       <c r="B10" s="36" t="s">
-        <v>143</v>
+        <v>131</v>
       </c>
       <c r="C10" s="42" t="s">
-        <v>192</v>
+        <v>177</v>
       </c>
       <c r="D10" s="37" t="s">
-        <v>255</v>
+        <v>230</v>
       </c>
       <c r="E10" s="38"/>
     </row>
     <row r="11" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A11" s="35" t="s">
-        <v>178</v>
+        <v>164</v>
       </c>
       <c r="B11" s="36" t="s">
-        <v>143</v>
+        <v>131</v>
       </c>
       <c r="C11" s="42" t="s">
-        <v>200</v>
+        <v>184</v>
       </c>
       <c r="D11" s="37" t="s">
-        <v>256</v>
+        <v>231</v>
       </c>
       <c r="E11" s="38"/>
     </row>
     <row r="12" spans="1:5" ht="30" x14ac:dyDescent="0.25">
       <c r="A12" s="35" t="s">
-        <v>178</v>
+        <v>164</v>
       </c>
       <c r="B12" s="36" t="s">
-        <v>143</v>
+        <v>131</v>
       </c>
       <c r="C12" s="42" t="s">
-        <v>205</v>
+        <v>187</v>
       </c>
       <c r="D12" s="37" t="s">
-        <v>257</v>
+        <v>232</v>
       </c>
       <c r="E12" s="38"/>
     </row>
     <row r="13" spans="1:5" ht="30" x14ac:dyDescent="0.25">
       <c r="A13" s="39" t="s">
-        <v>258</v>
+        <v>233</v>
       </c>
       <c r="B13" s="39"/>
       <c r="C13" s="39"/>
       <c r="D13" s="40" t="s">
-        <v>259</v>
+        <v>234</v>
       </c>
       <c r="E13" s="41"/>
     </row>
     <row r="14" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A14" s="39" t="s">
-        <v>258</v>
+        <v>233</v>
       </c>
       <c r="B14" s="39"/>
       <c r="C14" s="39"/>
       <c r="D14" s="40" t="s">
-        <v>260</v>
+        <v>235</v>
       </c>
       <c r="E14" s="41"/>
     </row>
     <row r="15" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A15" s="39" t="s">
-        <v>258</v>
+        <v>233</v>
       </c>
       <c r="B15" s="39"/>
       <c r="C15" s="39"/>
       <c r="D15" s="40" t="s">
-        <v>261</v>
+        <v>236</v>
       </c>
       <c r="E15" s="41"/>
     </row>

</xml_diff>

<commit_message>
actualización Escaleta CN 06 03 CO
actualización Escaleta CN 06 03 CO
</commit_message>
<xml_diff>
--- a/fuentes/contenidos/grado06/guion03/Escaleta CN_06_03_CO.xlsx
+++ b/fuentes/contenidos/grado06/guion03/Escaleta CN_06_03_CO.xlsx
@@ -591,9 +591,6 @@
     <t>El reino animal</t>
   </si>
   <si>
-    <t>Recurso M5A-02</t>
-  </si>
-  <si>
     <t>Actividad para reconocer y clasificar los seres vivos</t>
   </si>
   <si>
@@ -820,6 +817,9 @@
   </si>
   <si>
     <t>Actividad que propone relacionar los diferentes tipos de reproducción que existen con los organismos que la realizan</t>
+  </si>
+  <si>
+    <t>Recurso M11A-01</t>
   </si>
 </sst>
 </file>
@@ -1134,34 +1134,19 @@
       <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="17" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="3" fillId="12" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="12" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="10" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="10" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="9" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="9" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="11" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="11" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    <xf numFmtId="0" fontId="0" fillId="12" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="12" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="12" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="12" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="12" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -1203,8 +1188,23 @@
     <xf numFmtId="0" fontId="2" fillId="4" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="12" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
+    <xf numFmtId="0" fontId="3" fillId="10" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="10" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="9" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="9" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="11" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="11" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="2">
@@ -1514,8 +1514,8 @@
   <dimension ref="A1:U283"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
-      <pane ySplit="2" topLeftCell="A3" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="A3" sqref="A3"/>
+      <pane ySplit="2" topLeftCell="A9" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="A12" sqref="A12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1543,94 +1543,94 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:21" s="15" customFormat="1" ht="33.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="55" t="s">
+      <c r="A1" s="50" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="53" t="s">
+      <c r="B1" s="48" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="64" t="s">
+      <c r="C1" s="59" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="55" t="s">
+      <c r="D1" s="50" t="s">
         <v>110</v>
       </c>
-      <c r="E1" s="53" t="s">
+      <c r="E1" s="48" t="s">
         <v>111</v>
       </c>
-      <c r="F1" s="51" t="s">
+      <c r="F1" s="44" t="s">
         <v>112</v>
       </c>
-      <c r="G1" s="57" t="s">
+      <c r="G1" s="52" t="s">
         <v>3</v>
       </c>
-      <c r="H1" s="51" t="s">
+      <c r="H1" s="44" t="s">
         <v>113</v>
       </c>
-      <c r="I1" s="51" t="s">
+      <c r="I1" s="44" t="s">
         <v>107</v>
       </c>
-      <c r="J1" s="61" t="s">
+      <c r="J1" s="56" t="s">
         <v>4</v>
       </c>
-      <c r="K1" s="59" t="s">
+      <c r="K1" s="54" t="s">
         <v>108</v>
       </c>
-      <c r="L1" s="57" t="s">
+      <c r="L1" s="52" t="s">
         <v>14</v>
       </c>
-      <c r="M1" s="63" t="s">
+      <c r="M1" s="58" t="s">
         <v>21</v>
       </c>
-      <c r="N1" s="63"/>
-      <c r="O1" s="43" t="s">
+      <c r="N1" s="58"/>
+      <c r="O1" s="46" t="s">
         <v>109</v>
       </c>
-      <c r="P1" s="43" t="s">
+      <c r="P1" s="46" t="s">
         <v>114</v>
       </c>
-      <c r="Q1" s="45" t="s">
+      <c r="Q1" s="61" t="s">
         <v>85</v>
       </c>
-      <c r="R1" s="49" t="s">
+      <c r="R1" s="65" t="s">
         <v>86</v>
       </c>
-      <c r="S1" s="45" t="s">
+      <c r="S1" s="61" t="s">
         <v>87</v>
       </c>
-      <c r="T1" s="47" t="s">
+      <c r="T1" s="63" t="s">
         <v>88</v>
       </c>
-      <c r="U1" s="45" t="s">
+      <c r="U1" s="61" t="s">
         <v>89</v>
       </c>
     </row>
     <row r="2" spans="1:21" s="15" customFormat="1" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A2" s="56"/>
-      <c r="B2" s="54"/>
-      <c r="C2" s="65"/>
-      <c r="D2" s="56"/>
-      <c r="E2" s="54"/>
-      <c r="F2" s="52"/>
-      <c r="G2" s="58"/>
-      <c r="H2" s="52"/>
-      <c r="I2" s="52"/>
-      <c r="J2" s="62"/>
-      <c r="K2" s="60"/>
-      <c r="L2" s="58"/>
+      <c r="A2" s="51"/>
+      <c r="B2" s="49"/>
+      <c r="C2" s="60"/>
+      <c r="D2" s="51"/>
+      <c r="E2" s="49"/>
+      <c r="F2" s="45"/>
+      <c r="G2" s="53"/>
+      <c r="H2" s="45"/>
+      <c r="I2" s="45"/>
+      <c r="J2" s="57"/>
+      <c r="K2" s="55"/>
+      <c r="L2" s="53"/>
       <c r="M2" s="16" t="s">
         <v>90</v>
       </c>
       <c r="N2" s="16" t="s">
         <v>91</v>
       </c>
-      <c r="O2" s="44"/>
-      <c r="P2" s="44"/>
-      <c r="Q2" s="46"/>
-      <c r="R2" s="50"/>
-      <c r="S2" s="46"/>
-      <c r="T2" s="48"/>
-      <c r="U2" s="46"/>
+      <c r="O2" s="47"/>
+      <c r="P2" s="47"/>
+      <c r="Q2" s="62"/>
+      <c r="R2" s="66"/>
+      <c r="S2" s="62"/>
+      <c r="T2" s="64"/>
+      <c r="U2" s="62"/>
     </row>
     <row r="3" spans="1:21" ht="30.75" thickTop="1" x14ac:dyDescent="0.25">
       <c r="A3" s="4" t="s">
@@ -1718,7 +1718,7 @@
         <v>20</v>
       </c>
       <c r="J4" s="27" t="s">
-        <v>210</v>
+        <v>209</v>
       </c>
       <c r="K4" s="7" t="s">
         <v>20</v>
@@ -1827,7 +1827,7 @@
       </c>
       <c r="F6" s="9"/>
       <c r="G6" s="17" t="s">
-        <v>239</v>
+        <v>238</v>
       </c>
       <c r="H6" s="18">
         <v>4</v>
@@ -1836,7 +1836,7 @@
         <v>20</v>
       </c>
       <c r="J6" s="27" t="s">
-        <v>240</v>
+        <v>239</v>
       </c>
       <c r="K6" s="7" t="s">
         <v>20</v>
@@ -1849,7 +1849,7 @@
         <v>28</v>
       </c>
       <c r="O6" s="9"/>
-      <c r="P6" s="66" t="s">
+      <c r="P6" s="43" t="s">
         <v>19</v>
       </c>
       <c r="Q6" s="10">
@@ -2020,7 +2020,7 @@
         <v>19</v>
       </c>
       <c r="J10" s="28" t="s">
-        <v>241</v>
+        <v>240</v>
       </c>
       <c r="K10" s="23" t="s">
         <v>20</v>
@@ -2046,7 +2046,7 @@
         <v>170</v>
       </c>
       <c r="T10" s="29" t="s">
-        <v>258</v>
+        <v>257</v>
       </c>
       <c r="U10" s="10" t="s">
         <v>172</v>
@@ -2129,7 +2129,7 @@
       </c>
       <c r="F12" s="9"/>
       <c r="G12" s="17" t="s">
-        <v>243</v>
+        <v>242</v>
       </c>
       <c r="H12" s="18">
         <v>8</v>
@@ -2138,7 +2138,7 @@
         <v>20</v>
       </c>
       <c r="J12" s="27" t="s">
-        <v>244</v>
+        <v>243</v>
       </c>
       <c r="K12" s="7" t="s">
         <v>20</v>
@@ -2164,7 +2164,7 @@
         <v>145</v>
       </c>
       <c r="T12" s="29" t="s">
-        <v>162</v>
+        <v>264</v>
       </c>
       <c r="U12" s="10" t="s">
         <v>147</v>
@@ -2197,7 +2197,7 @@
         <v>20</v>
       </c>
       <c r="J13" s="27" t="s">
-        <v>237</v>
+        <v>236</v>
       </c>
       <c r="K13" s="7" t="s">
         <v>19</v>
@@ -2247,7 +2247,7 @@
       </c>
       <c r="F14" s="9"/>
       <c r="G14" s="20" t="s">
-        <v>245</v>
+        <v>244</v>
       </c>
       <c r="H14" s="21">
         <v>10</v>
@@ -2282,7 +2282,7 @@
         <v>145</v>
       </c>
       <c r="T14" s="29" t="s">
-        <v>238</v>
+        <v>237</v>
       </c>
       <c r="U14" s="10" t="s">
         <v>147</v>
@@ -2306,7 +2306,7 @@
       </c>
       <c r="F15" s="9"/>
       <c r="G15" s="17" t="s">
-        <v>246</v>
+        <v>245</v>
       </c>
       <c r="H15" s="18">
         <v>11</v>
@@ -2315,7 +2315,7 @@
         <v>19</v>
       </c>
       <c r="J15" s="27" t="s">
-        <v>247</v>
+        <v>246</v>
       </c>
       <c r="K15" s="7" t="s">
         <v>20</v>
@@ -2365,7 +2365,7 @@
       </c>
       <c r="F16" s="9"/>
       <c r="G16" s="17" t="s">
-        <v>248</v>
+        <v>247</v>
       </c>
       <c r="H16" s="18">
         <v>12</v>
@@ -2485,7 +2485,7 @@
         <v>177</v>
       </c>
       <c r="G18" s="17" t="s">
-        <v>249</v>
+        <v>248</v>
       </c>
       <c r="H18" s="18">
         <v>14</v>
@@ -2546,7 +2546,7 @@
         <v>177</v>
       </c>
       <c r="G19" s="17" t="s">
-        <v>250</v>
+        <v>249</v>
       </c>
       <c r="H19" s="18">
         <v>15</v>
@@ -2607,7 +2607,7 @@
         <v>184</v>
       </c>
       <c r="G20" s="17" t="s">
-        <v>251</v>
+        <v>250</v>
       </c>
       <c r="H20" s="18">
         <v>16</v>
@@ -2616,7 +2616,7 @@
         <v>20</v>
       </c>
       <c r="J20" s="27" t="s">
-        <v>252</v>
+        <v>251</v>
       </c>
       <c r="K20" s="7" t="s">
         <v>20</v>
@@ -2668,7 +2668,7 @@
         <v>183</v>
       </c>
       <c r="G21" s="17" t="s">
-        <v>253</v>
+        <v>252</v>
       </c>
       <c r="H21" s="18">
         <v>17</v>
@@ -2677,7 +2677,7 @@
         <v>20</v>
       </c>
       <c r="J21" s="27" t="s">
-        <v>254</v>
+        <v>253</v>
       </c>
       <c r="K21" s="7" t="s">
         <v>20</v>
@@ -2729,7 +2729,7 @@
         <v>183</v>
       </c>
       <c r="G22" s="17" t="s">
-        <v>256</v>
+        <v>255</v>
       </c>
       <c r="H22" s="18">
         <v>18</v>
@@ -2738,7 +2738,7 @@
         <v>20</v>
       </c>
       <c r="J22" s="27" t="s">
-        <v>255</v>
+        <v>254</v>
       </c>
       <c r="K22" s="7" t="s">
         <v>20</v>
@@ -2790,7 +2790,7 @@
         <v>187</v>
       </c>
       <c r="G23" s="17" t="s">
-        <v>261</v>
+        <v>260</v>
       </c>
       <c r="H23" s="18">
         <v>19</v>
@@ -2799,7 +2799,7 @@
         <v>19</v>
       </c>
       <c r="J23" s="27" t="s">
-        <v>257</v>
+        <v>256</v>
       </c>
       <c r="K23" s="7" t="s">
         <v>20</v>
@@ -2825,7 +2825,7 @@
         <v>170</v>
       </c>
       <c r="T23" s="29" t="s">
-        <v>242</v>
+        <v>241</v>
       </c>
       <c r="U23" s="10" t="s">
         <v>172</v>
@@ -2851,7 +2851,7 @@
         <v>187</v>
       </c>
       <c r="G24" s="17" t="s">
-        <v>259</v>
+        <v>258</v>
       </c>
       <c r="H24" s="18">
         <v>20</v>
@@ -2860,7 +2860,7 @@
         <v>20</v>
       </c>
       <c r="J24" s="27" t="s">
-        <v>260</v>
+        <v>259</v>
       </c>
       <c r="K24" s="7" t="s">
         <v>20</v>
@@ -2886,7 +2886,7 @@
         <v>145</v>
       </c>
       <c r="T24" s="29" t="s">
-        <v>188</v>
+        <v>162</v>
       </c>
       <c r="U24" s="10" t="s">
         <v>147</v>
@@ -2921,7 +2921,7 @@
         <v>20</v>
       </c>
       <c r="J25" s="27" t="s">
-        <v>212</v>
+        <v>211</v>
       </c>
       <c r="K25" s="7" t="s">
         <v>20</v>
@@ -2980,7 +2980,7 @@
         <v>20</v>
       </c>
       <c r="J26" s="27" t="s">
-        <v>189</v>
+        <v>188</v>
       </c>
       <c r="K26" s="7" t="s">
         <v>20</v>
@@ -3006,7 +3006,7 @@
         <v>145</v>
       </c>
       <c r="T26" s="29" t="s">
-        <v>191</v>
+        <v>190</v>
       </c>
       <c r="U26" s="10" t="s">
         <v>147</v>
@@ -3030,7 +3030,7 @@
       </c>
       <c r="F27" s="9"/>
       <c r="G27" s="17" t="s">
-        <v>211</v>
+        <v>210</v>
       </c>
       <c r="H27" s="18">
         <v>23</v>
@@ -3039,7 +3039,7 @@
         <v>20</v>
       </c>
       <c r="J27" s="27" t="s">
-        <v>190</v>
+        <v>189</v>
       </c>
       <c r="K27" s="7" t="s">
         <v>20</v>
@@ -3065,7 +3065,7 @@
         <v>145</v>
       </c>
       <c r="T27" s="29" t="s">
-        <v>192</v>
+        <v>191</v>
       </c>
       <c r="U27" s="10" t="s">
         <v>147</v>
@@ -3082,7 +3082,7 @@
         <v>137</v>
       </c>
       <c r="D28" s="14" t="s">
-        <v>193</v>
+        <v>192</v>
       </c>
       <c r="E28" s="12" t="s">
         <v>150</v>
@@ -3098,7 +3098,7 @@
         <v>20</v>
       </c>
       <c r="J28" s="27" t="s">
-        <v>194</v>
+        <v>193</v>
       </c>
       <c r="K28" s="7" t="s">
         <v>20</v>
@@ -3124,7 +3124,7 @@
         <v>145</v>
       </c>
       <c r="T28" s="29" t="s">
-        <v>195</v>
+        <v>194</v>
       </c>
       <c r="U28" s="10" t="s">
         <v>147</v>
@@ -3141,7 +3141,7 @@
         <v>137</v>
       </c>
       <c r="D29" s="14" t="s">
-        <v>196</v>
+        <v>195</v>
       </c>
       <c r="E29" s="12"/>
       <c r="F29" s="9"/>
@@ -3155,7 +3155,7 @@
         <v>20</v>
       </c>
       <c r="J29" s="28" t="s">
-        <v>263</v>
+        <v>262</v>
       </c>
       <c r="K29" s="23" t="s">
         <v>19</v>
@@ -3168,16 +3168,16 @@
         <v>120</v>
       </c>
       <c r="O29" s="9" t="s">
-        <v>209</v>
+        <v>208</v>
       </c>
       <c r="P29" s="21" t="s">
         <v>19</v>
       </c>
       <c r="Q29" s="10" t="s">
+        <v>197</v>
+      </c>
+      <c r="R29" s="11" t="s">
         <v>198</v>
-      </c>
-      <c r="R29" s="11" t="s">
-        <v>199</v>
       </c>
       <c r="S29" s="10" t="s">
         <v>137</v>
@@ -3186,7 +3186,7 @@
         <v>133</v>
       </c>
       <c r="U29" s="10" t="s">
-        <v>200</v>
+        <v>199</v>
       </c>
     </row>
     <row r="30" spans="1:21" ht="30" x14ac:dyDescent="0.25">
@@ -3200,7 +3200,7 @@
         <v>137</v>
       </c>
       <c r="D30" s="14" t="s">
-        <v>196</v>
+        <v>195</v>
       </c>
       <c r="E30" s="12"/>
       <c r="F30" s="9"/>
@@ -3214,7 +3214,7 @@
         <v>20</v>
       </c>
       <c r="J30" s="28" t="s">
-        <v>262</v>
+        <v>261</v>
       </c>
       <c r="K30" s="23" t="s">
         <v>19</v>
@@ -3227,16 +3227,16 @@
         <v>120</v>
       </c>
       <c r="O30" s="9" t="s">
-        <v>209</v>
+        <v>208</v>
       </c>
       <c r="P30" s="21" t="s">
         <v>19</v>
       </c>
       <c r="Q30" s="10" t="s">
+        <v>197</v>
+      </c>
+      <c r="R30" s="11" t="s">
         <v>198</v>
-      </c>
-      <c r="R30" s="11" t="s">
-        <v>199</v>
       </c>
       <c r="S30" s="10" t="s">
         <v>137</v>
@@ -3245,7 +3245,7 @@
         <v>134</v>
       </c>
       <c r="U30" s="10" t="s">
-        <v>200</v>
+        <v>199</v>
       </c>
     </row>
     <row r="31" spans="1:21" ht="30" x14ac:dyDescent="0.25">
@@ -3259,7 +3259,7 @@
         <v>137</v>
       </c>
       <c r="D31" s="14" t="s">
-        <v>196</v>
+        <v>195</v>
       </c>
       <c r="E31" s="12"/>
       <c r="F31" s="9"/>
@@ -3273,7 +3273,7 @@
         <v>20</v>
       </c>
       <c r="J31" s="27" t="s">
-        <v>197</v>
+        <v>196</v>
       </c>
       <c r="K31" s="23" t="s">
         <v>19</v>
@@ -3316,12 +3316,12 @@
         <v>137</v>
       </c>
       <c r="D32" s="14" t="s">
-        <v>196</v>
+        <v>195</v>
       </c>
       <c r="E32" s="12"/>
       <c r="F32" s="9"/>
       <c r="G32" s="17" t="s">
-        <v>201</v>
+        <v>200</v>
       </c>
       <c r="H32" s="18">
         <v>28</v>
@@ -3330,7 +3330,7 @@
         <v>20</v>
       </c>
       <c r="J32" s="27" t="s">
-        <v>203</v>
+        <v>202</v>
       </c>
       <c r="K32" s="7" t="s">
         <v>19</v>
@@ -3343,7 +3343,7 @@
         <v>120</v>
       </c>
       <c r="O32" s="9" t="s">
-        <v>215</v>
+        <v>214</v>
       </c>
       <c r="P32" s="18" t="s">
         <v>19</v>
@@ -3358,7 +3358,7 @@
         <v>137</v>
       </c>
       <c r="T32" s="29" t="s">
-        <v>201</v>
+        <v>200</v>
       </c>
       <c r="U32" s="10" t="s">
         <v>156</v>
@@ -3375,12 +3375,12 @@
         <v>137</v>
       </c>
       <c r="D33" s="14" t="s">
-        <v>196</v>
+        <v>195</v>
       </c>
       <c r="E33" s="12"/>
       <c r="F33" s="9"/>
       <c r="G33" s="17" t="s">
-        <v>202</v>
+        <v>201</v>
       </c>
       <c r="H33" s="18">
         <v>29</v>
@@ -3389,7 +3389,7 @@
         <v>20</v>
       </c>
       <c r="J33" s="27" t="s">
-        <v>264</v>
+        <v>263</v>
       </c>
       <c r="K33" s="7" t="s">
         <v>19</v>
@@ -3402,7 +3402,7 @@
         <v>120</v>
       </c>
       <c r="O33" s="9" t="s">
-        <v>209</v>
+        <v>208</v>
       </c>
       <c r="P33" s="18" t="s">
         <v>19</v>
@@ -3417,7 +3417,7 @@
         <v>137</v>
       </c>
       <c r="T33" s="29" t="s">
-        <v>202</v>
+        <v>201</v>
       </c>
       <c r="U33" s="10" t="s">
         <v>156</v>
@@ -3434,7 +3434,7 @@
         <v>137</v>
       </c>
       <c r="D34" s="31" t="s">
-        <v>204</v>
+        <v>203</v>
       </c>
       <c r="E34" s="12"/>
       <c r="F34" s="9"/>
@@ -3448,7 +3448,7 @@
         <v>20</v>
       </c>
       <c r="J34" s="27" t="s">
-        <v>206</v>
+        <v>205</v>
       </c>
       <c r="K34" s="7" t="s">
         <v>20</v>
@@ -3479,12 +3479,12 @@
         <v>137</v>
       </c>
       <c r="D35" s="31" t="s">
-        <v>204</v>
+        <v>203</v>
       </c>
       <c r="E35" s="12"/>
       <c r="F35" s="9"/>
       <c r="G35" s="17" t="s">
-        <v>205</v>
+        <v>204</v>
       </c>
       <c r="H35" s="18">
         <v>31</v>
@@ -3493,7 +3493,7 @@
         <v>20</v>
       </c>
       <c r="J35" s="27" t="s">
-        <v>207</v>
+        <v>206</v>
       </c>
       <c r="K35" s="7" t="s">
         <v>20</v>
@@ -3536,12 +3536,12 @@
         <v>137</v>
       </c>
       <c r="D36" s="31" t="s">
-        <v>204</v>
+        <v>203</v>
       </c>
       <c r="E36" s="12"/>
       <c r="F36" s="9"/>
       <c r="G36" s="17" t="s">
-        <v>214</v>
+        <v>213</v>
       </c>
       <c r="H36" s="18">
         <v>32</v>
@@ -3550,7 +3550,7 @@
         <v>20</v>
       </c>
       <c r="J36" s="27" t="s">
-        <v>213</v>
+        <v>212</v>
       </c>
       <c r="K36" s="7" t="s">
         <v>20</v>
@@ -3576,7 +3576,7 @@
         <v>145</v>
       </c>
       <c r="T36" s="29" t="s">
-        <v>208</v>
+        <v>207</v>
       </c>
       <c r="U36" s="10" t="s">
         <v>147</v>
@@ -4705,6 +4705,12 @@
   </sheetData>
   <autoFilter ref="A2:U36"/>
   <mergeCells count="20">
+    <mergeCell ref="P1:P2"/>
+    <mergeCell ref="U1:U2"/>
+    <mergeCell ref="T1:T2"/>
+    <mergeCell ref="S1:S2"/>
+    <mergeCell ref="R1:R2"/>
+    <mergeCell ref="Q1:Q2"/>
     <mergeCell ref="I1:I2"/>
     <mergeCell ref="H1:H2"/>
     <mergeCell ref="O1:O2"/>
@@ -4719,12 +4725,6 @@
     <mergeCell ref="D1:D2"/>
     <mergeCell ref="C1:C2"/>
     <mergeCell ref="F1:F2"/>
-    <mergeCell ref="P1:P2"/>
-    <mergeCell ref="U1:U2"/>
-    <mergeCell ref="T1:T2"/>
-    <mergeCell ref="S1:S2"/>
-    <mergeCell ref="R1:R2"/>
-    <mergeCell ref="Q1:Q2"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
@@ -4786,19 +4786,19 @@
   <sheetData>
     <row r="2" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A2" s="34" t="s">
+        <v>215</v>
+      </c>
+      <c r="B2" s="34" t="s">
         <v>216</v>
       </c>
-      <c r="B2" s="34" t="s">
+      <c r="C2" s="34" t="s">
+        <v>219</v>
+      </c>
+      <c r="D2" s="34" t="s">
         <v>217</v>
       </c>
-      <c r="C2" s="34" t="s">
-        <v>220</v>
-      </c>
-      <c r="D2" s="34" t="s">
+      <c r="E2" s="34" t="s">
         <v>218</v>
-      </c>
-      <c r="E2" s="34" t="s">
-        <v>219</v>
       </c>
     </row>
     <row r="3" spans="1:5" ht="45" x14ac:dyDescent="0.25">
@@ -4810,10 +4810,10 @@
       </c>
       <c r="C3" s="42"/>
       <c r="D3" s="37" t="s">
-        <v>224</v>
+        <v>223</v>
       </c>
       <c r="E3" s="38" t="s">
-        <v>221</v>
+        <v>220</v>
       </c>
     </row>
     <row r="4" spans="1:5" x14ac:dyDescent="0.25">
@@ -4825,7 +4825,7 @@
       </c>
       <c r="C4" s="42"/>
       <c r="D4" s="37" t="s">
-        <v>222</v>
+        <v>221</v>
       </c>
       <c r="E4" s="38"/>
     </row>
@@ -4838,10 +4838,10 @@
       </c>
       <c r="C5" s="42"/>
       <c r="D5" s="37" t="s">
-        <v>223</v>
+        <v>222</v>
       </c>
       <c r="E5" s="38" t="s">
-        <v>225</v>
+        <v>224</v>
       </c>
     </row>
     <row r="6" spans="1:5" x14ac:dyDescent="0.25">
@@ -4853,7 +4853,7 @@
       </c>
       <c r="C6" s="42"/>
       <c r="D6" s="37" t="s">
-        <v>226</v>
+        <v>225</v>
       </c>
       <c r="E6" s="38"/>
     </row>
@@ -4866,7 +4866,7 @@
       </c>
       <c r="C7" s="42"/>
       <c r="D7" s="37" t="s">
-        <v>227</v>
+        <v>226</v>
       </c>
       <c r="E7" s="38"/>
     </row>
@@ -4879,7 +4879,7 @@
       </c>
       <c r="C8" s="42"/>
       <c r="D8" s="37" t="s">
-        <v>228</v>
+        <v>227</v>
       </c>
       <c r="E8" s="38"/>
     </row>
@@ -4894,7 +4894,7 @@
         <v>177</v>
       </c>
       <c r="D9" s="37" t="s">
-        <v>229</v>
+        <v>228</v>
       </c>
       <c r="E9" s="38"/>
     </row>
@@ -4909,7 +4909,7 @@
         <v>177</v>
       </c>
       <c r="D10" s="37" t="s">
-        <v>230</v>
+        <v>229</v>
       </c>
       <c r="E10" s="38"/>
     </row>
@@ -4924,7 +4924,7 @@
         <v>184</v>
       </c>
       <c r="D11" s="37" t="s">
-        <v>231</v>
+        <v>230</v>
       </c>
       <c r="E11" s="38"/>
     </row>
@@ -4939,40 +4939,40 @@
         <v>187</v>
       </c>
       <c r="D12" s="37" t="s">
-        <v>232</v>
+        <v>231</v>
       </c>
       <c r="E12" s="38"/>
     </row>
     <row r="13" spans="1:5" ht="30" x14ac:dyDescent="0.25">
       <c r="A13" s="39" t="s">
-        <v>233</v>
+        <v>232</v>
       </c>
       <c r="B13" s="39"/>
       <c r="C13" s="39"/>
       <c r="D13" s="40" t="s">
-        <v>234</v>
+        <v>233</v>
       </c>
       <c r="E13" s="41"/>
     </row>
     <row r="14" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A14" s="39" t="s">
-        <v>233</v>
+        <v>232</v>
       </c>
       <c r="B14" s="39"/>
       <c r="C14" s="39"/>
       <c r="D14" s="40" t="s">
-        <v>235</v>
+        <v>234</v>
       </c>
       <c r="E14" s="41"/>
     </row>
     <row r="15" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A15" s="39" t="s">
-        <v>233</v>
+        <v>232</v>
       </c>
       <c r="B15" s="39"/>
       <c r="C15" s="39"/>
       <c r="D15" s="40" t="s">
-        <v>236</v>
+        <v>235</v>
       </c>
       <c r="E15" s="41"/>
     </row>

</xml_diff>

<commit_message>
actualización escaleta CN 06 03
actualización escaleta CN 06 03
</commit_message>
<xml_diff>
--- a/fuentes/contenidos/grado06/guion03/Escaleta CN_06_03_CO.xlsx
+++ b/fuentes/contenidos/grado06/guion03/Escaleta CN_06_03_CO.xlsx
@@ -1,20 +1,25 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9302"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="5" rupBuild="14420"/>
   <workbookPr defaultThemeVersion="124226"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\diego\Dropbox\Editorial planeta\1. Autor\Escaletas\CN_06_03_CO\"/>
+    </mc:Choice>
+  </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="60" windowWidth="8250" windowHeight="4635"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="8250" windowHeight="4695"/>
   </bookViews>
   <sheets>
     <sheet name="Escaleta" sheetId="2" r:id="rId1"/>
-    <sheet name="VER" sheetId="3" r:id="rId2"/>
-    <sheet name="DATOS" sheetId="1" r:id="rId3"/>
+    <sheet name="VER" sheetId="3" state="hidden" r:id="rId2"/>
+    <sheet name="DATOS" sheetId="1" state="hidden" r:id="rId3"/>
   </sheets>
   <definedNames>
     <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Escaleta!$A$2:$U$36</definedName>
   </definedNames>
-  <calcPr calcId="152511" iterateCount="2" iterateDelta="10"/>
+  <calcPr calcId="152511"/>
 </workbook>
 </file>
 
@@ -409,9 +414,6 @@
     <t>Refuerza tu aprendizaje: Las funciones de los seres vivos</t>
   </si>
   <si>
-    <t>Importancia biológica de las bacterias</t>
-  </si>
-  <si>
     <t>Refuerza tu aprendizaje: La clasificación de los seres vivos</t>
   </si>
   <si>
@@ -559,15 +561,9 @@
     <t>Interactivo que permite identificar y clasificar a los protistas</t>
   </si>
   <si>
-    <t>Recurso F6-01</t>
-  </si>
-  <si>
     <t>Actividad para reforzar el aprendizaje sobre el reino protista</t>
   </si>
   <si>
-    <t>Recurso M2C-02</t>
-  </si>
-  <si>
     <t>Recurso M14A-02</t>
   </si>
   <si>
@@ -658,9 +654,6 @@
     <t>Actividad de preguntas que permite evaluar los conocimientos aprendidos acerca de la clasificación de los seres vivos</t>
   </si>
   <si>
-    <t>Motor que incluye preguntas de respuesta abierta del tema Los seres vivos</t>
-  </si>
-  <si>
     <t>Banco de actividades</t>
   </si>
   <si>
@@ -815,6 +808,18 @@
   </si>
   <si>
     <t>Recurso M11A-01</t>
+  </si>
+  <si>
+    <t>La importancia biológica de las bacterias</t>
+  </si>
+  <si>
+    <t>Recurso F7-01</t>
+  </si>
+  <si>
+    <t>Recurso M2B-01</t>
+  </si>
+  <si>
+    <t>Banco de actividades del tema Los seres vivos</t>
   </si>
 </sst>
 </file>
@@ -1132,34 +1137,16 @@
     <xf numFmtId="0" fontId="0" fillId="12" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="2" fillId="12" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="12" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="3" fillId="12" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="12" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="10" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="10" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="9" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="9" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="11" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="11" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="12" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="12" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -1199,6 +1186,24 @@
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="4" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="10" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="10" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="9" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="9" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="11" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="11" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
@@ -1262,7 +1267,7 @@
     </a:clrScheme>
     <a:fontScheme name="Office">
       <a:majorFont>
-        <a:latin typeface="Cambria"/>
+        <a:latin typeface="Cambria" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -1297,7 +1302,7 @@
         <a:font script="Geor" typeface="Sylfaen"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri"/>
+        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -1508,9 +1513,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:U283"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
-      <pane ySplit="2" topLeftCell="A3" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="K12" sqref="A12:XFD12"/>
+    <sheetView tabSelected="1" topLeftCell="K1" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
+      <pane ySplit="2" topLeftCell="A28" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="P33" sqref="P33"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1528,7 +1533,7 @@
     <col min="11" max="11" width="13.28515625" customWidth="1"/>
     <col min="12" max="12" width="23.85546875" customWidth="1"/>
     <col min="13" max="14" width="9.28515625" customWidth="1"/>
-    <col min="15" max="15" width="13.85546875" style="1" customWidth="1"/>
+    <col min="15" max="15" width="37.85546875" style="1" customWidth="1"/>
     <col min="16" max="16" width="16.5703125" style="19" customWidth="1"/>
     <col min="17" max="17" width="20.42578125" style="1" customWidth="1"/>
     <col min="18" max="18" width="23" bestFit="1" customWidth="1"/>
@@ -1538,110 +1543,110 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:21" s="15" customFormat="1" ht="33.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="56" t="s">
+      <c r="A1" s="50" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="54" t="s">
+      <c r="B1" s="48" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="65" t="s">
+      <c r="C1" s="59" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="56" t="s">
+      <c r="D1" s="50" t="s">
         <v>110</v>
       </c>
-      <c r="E1" s="54" t="s">
+      <c r="E1" s="48" t="s">
         <v>111</v>
       </c>
-      <c r="F1" s="52" t="s">
+      <c r="F1" s="44" t="s">
         <v>112</v>
       </c>
-      <c r="G1" s="58" t="s">
+      <c r="G1" s="52" t="s">
         <v>3</v>
       </c>
-      <c r="H1" s="52" t="s">
+      <c r="H1" s="44" t="s">
         <v>113</v>
       </c>
-      <c r="I1" s="52" t="s">
+      <c r="I1" s="44" t="s">
         <v>107</v>
       </c>
-      <c r="J1" s="62" t="s">
+      <c r="J1" s="56" t="s">
         <v>4</v>
       </c>
-      <c r="K1" s="60" t="s">
+      <c r="K1" s="54" t="s">
         <v>108</v>
       </c>
-      <c r="L1" s="58" t="s">
+      <c r="L1" s="52" t="s">
         <v>14</v>
       </c>
-      <c r="M1" s="64" t="s">
+      <c r="M1" s="58" t="s">
         <v>21</v>
       </c>
-      <c r="N1" s="64"/>
-      <c r="O1" s="44" t="s">
+      <c r="N1" s="58"/>
+      <c r="O1" s="46" t="s">
         <v>109</v>
       </c>
-      <c r="P1" s="44" t="s">
+      <c r="P1" s="46" t="s">
         <v>114</v>
       </c>
-      <c r="Q1" s="46" t="s">
+      <c r="Q1" s="61" t="s">
         <v>85</v>
       </c>
-      <c r="R1" s="50" t="s">
+      <c r="R1" s="65" t="s">
         <v>86</v>
       </c>
-      <c r="S1" s="46" t="s">
+      <c r="S1" s="61" t="s">
         <v>87</v>
       </c>
-      <c r="T1" s="48" t="s">
+      <c r="T1" s="63" t="s">
         <v>88</v>
       </c>
-      <c r="U1" s="46" t="s">
+      <c r="U1" s="61" t="s">
         <v>89</v>
       </c>
     </row>
     <row r="2" spans="1:21" s="15" customFormat="1" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A2" s="57"/>
-      <c r="B2" s="55"/>
-      <c r="C2" s="66"/>
-      <c r="D2" s="57"/>
-      <c r="E2" s="55"/>
-      <c r="F2" s="53"/>
-      <c r="G2" s="59"/>
-      <c r="H2" s="53"/>
-      <c r="I2" s="53"/>
-      <c r="J2" s="63"/>
-      <c r="K2" s="61"/>
-      <c r="L2" s="59"/>
+      <c r="A2" s="51"/>
+      <c r="B2" s="49"/>
+      <c r="C2" s="60"/>
+      <c r="D2" s="51"/>
+      <c r="E2" s="49"/>
+      <c r="F2" s="45"/>
+      <c r="G2" s="53"/>
+      <c r="H2" s="45"/>
+      <c r="I2" s="45"/>
+      <c r="J2" s="57"/>
+      <c r="K2" s="55"/>
+      <c r="L2" s="53"/>
       <c r="M2" s="16" t="s">
         <v>90</v>
       </c>
       <c r="N2" s="16" t="s">
         <v>91</v>
       </c>
-      <c r="O2" s="45"/>
-      <c r="P2" s="45"/>
-      <c r="Q2" s="47"/>
-      <c r="R2" s="51"/>
-      <c r="S2" s="47"/>
-      <c r="T2" s="49"/>
-      <c r="U2" s="47"/>
+      <c r="O2" s="47"/>
+      <c r="P2" s="47"/>
+      <c r="Q2" s="62"/>
+      <c r="R2" s="66"/>
+      <c r="S2" s="62"/>
+      <c r="T2" s="64"/>
+      <c r="U2" s="62"/>
     </row>
     <row r="3" spans="1:21" ht="30.75" thickTop="1" x14ac:dyDescent="0.25">
       <c r="A3" s="4" t="s">
         <v>17</v>
       </c>
       <c r="B3" s="12" t="s">
+        <v>135</v>
+      </c>
+      <c r="C3" s="13" t="s">
         <v>136</v>
       </c>
-      <c r="C3" s="13" t="s">
+      <c r="D3" s="14" t="s">
         <v>137</v>
       </c>
-      <c r="D3" s="14" t="s">
+      <c r="E3" s="12" t="s">
         <v>138</v>
-      </c>
-      <c r="E3" s="12" t="s">
-        <v>139</v>
       </c>
       <c r="F3" s="9"/>
       <c r="G3" s="17" t="s">
@@ -1654,7 +1659,7 @@
         <v>19</v>
       </c>
       <c r="J3" s="27" t="s">
-        <v>140</v>
+        <v>139</v>
       </c>
       <c r="K3" s="7" t="s">
         <v>20</v>
@@ -1674,16 +1679,16 @@
         <v>6</v>
       </c>
       <c r="R3" s="11" t="s">
+        <v>140</v>
+      </c>
+      <c r="S3" s="30" t="s">
         <v>141</v>
       </c>
-      <c r="S3" s="30" t="s">
+      <c r="T3" s="29" t="s">
         <v>142</v>
       </c>
-      <c r="T3" s="29" t="s">
+      <c r="U3" s="10" t="s">
         <v>143</v>
-      </c>
-      <c r="U3" s="10" t="s">
-        <v>144</v>
       </c>
     </row>
     <row r="4" spans="1:21" ht="30" x14ac:dyDescent="0.25">
@@ -1691,16 +1696,16 @@
         <v>17</v>
       </c>
       <c r="B4" s="12" t="s">
+        <v>135</v>
+      </c>
+      <c r="C4" s="13" t="s">
         <v>136</v>
       </c>
-      <c r="C4" s="13" t="s">
+      <c r="D4" s="14" t="s">
         <v>137</v>
       </c>
-      <c r="D4" s="14" t="s">
+      <c r="E4" s="12" t="s">
         <v>138</v>
-      </c>
-      <c r="E4" s="12" t="s">
-        <v>139</v>
       </c>
       <c r="F4" s="9"/>
       <c r="G4" s="17" t="s">
@@ -1713,7 +1718,7 @@
         <v>20</v>
       </c>
       <c r="J4" s="27" t="s">
-        <v>209</v>
+        <v>206</v>
       </c>
       <c r="K4" s="7" t="s">
         <v>20</v>
@@ -1733,16 +1738,16 @@
         <v>6</v>
       </c>
       <c r="R4" s="11" t="s">
-        <v>141</v>
+        <v>140</v>
       </c>
       <c r="S4" s="10" t="s">
+        <v>144</v>
+      </c>
+      <c r="T4" s="29" t="s">
         <v>145</v>
       </c>
-      <c r="T4" s="29" t="s">
+      <c r="U4" s="10" t="s">
         <v>146</v>
-      </c>
-      <c r="U4" s="10" t="s">
-        <v>147</v>
       </c>
     </row>
     <row r="5" spans="1:21" ht="30" x14ac:dyDescent="0.25">
@@ -1750,16 +1755,16 @@
         <v>17</v>
       </c>
       <c r="B5" s="12" t="s">
+        <v>135</v>
+      </c>
+      <c r="C5" s="13" t="s">
         <v>136</v>
       </c>
-      <c r="C5" s="13" t="s">
+      <c r="D5" s="14" t="s">
         <v>137</v>
       </c>
-      <c r="D5" s="14" t="s">
-        <v>138</v>
-      </c>
       <c r="E5" s="12" t="s">
-        <v>148</v>
+        <v>147</v>
       </c>
       <c r="F5" s="9"/>
       <c r="G5" s="17" t="s">
@@ -1772,7 +1777,7 @@
         <v>19</v>
       </c>
       <c r="J5" s="27" t="s">
-        <v>149</v>
+        <v>148</v>
       </c>
       <c r="K5" s="7" t="s">
         <v>19</v>
@@ -1789,19 +1794,19 @@
         <v>19</v>
       </c>
       <c r="Q5" s="10" t="s">
+        <v>153</v>
+      </c>
+      <c r="R5" s="11" t="s">
         <v>154</v>
       </c>
-      <c r="R5" s="11" t="s">
-        <v>155</v>
-      </c>
       <c r="S5" s="10" t="s">
-        <v>137</v>
+        <v>136</v>
       </c>
       <c r="T5" s="29" t="s">
         <v>124</v>
       </c>
       <c r="U5" s="10" t="s">
-        <v>156</v>
+        <v>155</v>
       </c>
     </row>
     <row r="6" spans="1:21" ht="30" x14ac:dyDescent="0.25">
@@ -1809,20 +1814,20 @@
         <v>17</v>
       </c>
       <c r="B6" s="12" t="s">
+        <v>135</v>
+      </c>
+      <c r="C6" s="13" t="s">
         <v>136</v>
       </c>
-      <c r="C6" s="13" t="s">
+      <c r="D6" s="14" t="s">
         <v>137</v>
       </c>
-      <c r="D6" s="14" t="s">
-        <v>138</v>
-      </c>
       <c r="E6" s="12" t="s">
-        <v>148</v>
+        <v>147</v>
       </c>
       <c r="F6" s="9"/>
       <c r="G6" s="17" t="s">
-        <v>238</v>
+        <v>234</v>
       </c>
       <c r="H6" s="18">
         <v>4</v>
@@ -1831,7 +1836,7 @@
         <v>20</v>
       </c>
       <c r="J6" s="27" t="s">
-        <v>239</v>
+        <v>235</v>
       </c>
       <c r="K6" s="7" t="s">
         <v>20</v>
@@ -1851,16 +1856,16 @@
         <v>6</v>
       </c>
       <c r="R6" s="11" t="s">
-        <v>141</v>
+        <v>140</v>
       </c>
       <c r="S6" s="10" t="s">
-        <v>145</v>
+        <v>144</v>
       </c>
       <c r="T6" s="29" t="s">
-        <v>167</v>
+        <v>166</v>
       </c>
       <c r="U6" s="10" t="s">
-        <v>147</v>
+        <v>146</v>
       </c>
     </row>
     <row r="7" spans="1:21" ht="30" x14ac:dyDescent="0.25">
@@ -1868,16 +1873,16 @@
         <v>17</v>
       </c>
       <c r="B7" s="12" t="s">
+        <v>135</v>
+      </c>
+      <c r="C7" s="13" t="s">
         <v>136</v>
       </c>
-      <c r="C7" s="13" t="s">
+      <c r="D7" s="14" t="s">
         <v>137</v>
       </c>
-      <c r="D7" s="14" t="s">
-        <v>138</v>
-      </c>
       <c r="E7" s="12" t="s">
-        <v>150</v>
+        <v>149</v>
       </c>
       <c r="F7" s="9"/>
       <c r="G7" s="17" t="s">
@@ -1890,7 +1895,7 @@
         <v>20</v>
       </c>
       <c r="J7" s="27" t="s">
-        <v>151</v>
+        <v>150</v>
       </c>
       <c r="K7" s="7" t="s">
         <v>20</v>
@@ -1910,16 +1915,16 @@
         <v>6</v>
       </c>
       <c r="R7" s="11" t="s">
-        <v>141</v>
+        <v>140</v>
       </c>
       <c r="S7" s="10" t="s">
-        <v>145</v>
+        <v>144</v>
       </c>
       <c r="T7" s="29" t="s">
-        <v>152</v>
+        <v>151</v>
       </c>
       <c r="U7" s="10" t="s">
-        <v>147</v>
+        <v>146</v>
       </c>
     </row>
     <row r="8" spans="1:21" ht="15.75" x14ac:dyDescent="0.25">
@@ -1927,16 +1932,16 @@
         <v>17</v>
       </c>
       <c r="B8" s="12" t="s">
+        <v>135</v>
+      </c>
+      <c r="C8" s="13" t="s">
         <v>136</v>
       </c>
-      <c r="C8" s="13" t="s">
-        <v>137</v>
-      </c>
       <c r="D8" s="14" t="s">
+        <v>156</v>
+      </c>
+      <c r="E8" s="12" t="s">
         <v>157</v>
-      </c>
-      <c r="E8" s="12" t="s">
-        <v>158</v>
       </c>
       <c r="F8" s="9"/>
       <c r="G8" s="20"/>
@@ -1960,16 +1965,16 @@
         <v>17</v>
       </c>
       <c r="B9" s="12" t="s">
+        <v>135</v>
+      </c>
+      <c r="C9" s="13" t="s">
         <v>136</v>
       </c>
-      <c r="C9" s="13" t="s">
-        <v>137</v>
-      </c>
       <c r="D9" s="14" t="s">
-        <v>157</v>
+        <v>156</v>
       </c>
       <c r="E9" s="12" t="s">
-        <v>159</v>
+        <v>158</v>
       </c>
       <c r="F9" s="9"/>
       <c r="G9" s="17"/>
@@ -1993,20 +1998,20 @@
         <v>17</v>
       </c>
       <c r="B10" s="12" t="s">
+        <v>135</v>
+      </c>
+      <c r="C10" s="13" t="s">
         <v>136</v>
       </c>
-      <c r="C10" s="13" t="s">
-        <v>137</v>
-      </c>
       <c r="D10" s="14" t="s">
-        <v>157</v>
+        <v>156</v>
       </c>
       <c r="E10" s="12" t="s">
-        <v>160</v>
+        <v>159</v>
       </c>
       <c r="F10" s="9"/>
       <c r="G10" s="20" t="s">
-        <v>157</v>
+        <v>156</v>
       </c>
       <c r="H10" s="21">
         <v>6</v>
@@ -2015,7 +2020,7 @@
         <v>19</v>
       </c>
       <c r="J10" s="28" t="s">
-        <v>240</v>
+        <v>236</v>
       </c>
       <c r="K10" s="23" t="s">
         <v>20</v>
@@ -2035,16 +2040,16 @@
         <v>6</v>
       </c>
       <c r="R10" s="11" t="s">
+        <v>168</v>
+      </c>
+      <c r="S10" s="10" t="s">
         <v>169</v>
       </c>
-      <c r="S10" s="10" t="s">
-        <v>170</v>
-      </c>
       <c r="T10" s="29" t="s">
-        <v>257</v>
+        <v>253</v>
       </c>
       <c r="U10" s="10" t="s">
-        <v>172</v>
+        <v>171</v>
       </c>
     </row>
     <row r="11" spans="1:21" ht="30" x14ac:dyDescent="0.25">
@@ -2052,16 +2057,16 @@
         <v>17</v>
       </c>
       <c r="B11" s="12" t="s">
+        <v>135</v>
+      </c>
+      <c r="C11" s="13" t="s">
         <v>136</v>
       </c>
-      <c r="C11" s="13" t="s">
-        <v>137</v>
-      </c>
       <c r="D11" s="14" t="s">
-        <v>157</v>
+        <v>156</v>
       </c>
       <c r="E11" s="12" t="s">
-        <v>160</v>
+        <v>159</v>
       </c>
       <c r="F11" s="9"/>
       <c r="G11" s="17" t="s">
@@ -2074,7 +2079,7 @@
         <v>20</v>
       </c>
       <c r="J11" s="27" t="s">
-        <v>161</v>
+        <v>160</v>
       </c>
       <c r="K11" s="7" t="s">
         <v>19</v>
@@ -2083,7 +2088,7 @@
         <v>8</v>
       </c>
       <c r="M11" s="8"/>
-      <c r="N11" s="8" t="s">
+      <c r="N11" s="25" t="s">
         <v>33</v>
       </c>
       <c r="O11" s="9"/>
@@ -2091,19 +2096,19 @@
         <v>19</v>
       </c>
       <c r="Q11" s="10" t="s">
+        <v>153</v>
+      </c>
+      <c r="R11" s="11" t="s">
         <v>154</v>
       </c>
-      <c r="R11" s="11" t="s">
-        <v>155</v>
-      </c>
       <c r="S11" s="10" t="s">
-        <v>137</v>
+        <v>136</v>
       </c>
       <c r="T11" s="29" t="s">
         <v>127</v>
       </c>
       <c r="U11" s="10" t="s">
-        <v>156</v>
+        <v>155</v>
       </c>
     </row>
     <row r="12" spans="1:21" ht="30" x14ac:dyDescent="0.25">
@@ -2111,20 +2116,20 @@
         <v>17</v>
       </c>
       <c r="B12" s="12" t="s">
+        <v>135</v>
+      </c>
+      <c r="C12" s="13" t="s">
         <v>136</v>
       </c>
-      <c r="C12" s="13" t="s">
-        <v>137</v>
-      </c>
       <c r="D12" s="14" t="s">
-        <v>157</v>
+        <v>156</v>
       </c>
       <c r="E12" s="12" t="s">
-        <v>160</v>
+        <v>159</v>
       </c>
       <c r="F12" s="9"/>
       <c r="G12" s="17" t="s">
-        <v>242</v>
+        <v>238</v>
       </c>
       <c r="H12" s="18">
         <v>8</v>
@@ -2133,7 +2138,7 @@
         <v>20</v>
       </c>
       <c r="J12" s="27" t="s">
-        <v>243</v>
+        <v>239</v>
       </c>
       <c r="K12" s="7" t="s">
         <v>20</v>
@@ -2153,16 +2158,16 @@
         <v>6</v>
       </c>
       <c r="R12" s="11" t="s">
-        <v>141</v>
+        <v>140</v>
       </c>
       <c r="S12" s="10" t="s">
-        <v>145</v>
+        <v>144</v>
       </c>
       <c r="T12" s="29" t="s">
-        <v>264</v>
+        <v>260</v>
       </c>
       <c r="U12" s="10" t="s">
-        <v>147</v>
+        <v>146</v>
       </c>
     </row>
     <row r="13" spans="1:21" ht="30" x14ac:dyDescent="0.25">
@@ -2170,16 +2175,16 @@
         <v>17</v>
       </c>
       <c r="B13" s="12" t="s">
+        <v>135</v>
+      </c>
+      <c r="C13" s="13" t="s">
         <v>136</v>
       </c>
-      <c r="C13" s="13" t="s">
-        <v>137</v>
-      </c>
       <c r="D13" s="14" t="s">
-        <v>157</v>
+        <v>156</v>
       </c>
       <c r="E13" s="12" t="s">
-        <v>150</v>
+        <v>149</v>
       </c>
       <c r="F13" s="9"/>
       <c r="G13" s="17" t="s">
@@ -2192,7 +2197,7 @@
         <v>20</v>
       </c>
       <c r="J13" s="27" t="s">
-        <v>236</v>
+        <v>232</v>
       </c>
       <c r="K13" s="7" t="s">
         <v>19</v>
@@ -2209,19 +2214,19 @@
         <v>19</v>
       </c>
       <c r="Q13" s="10" t="s">
+        <v>153</v>
+      </c>
+      <c r="R13" s="11" t="s">
         <v>154</v>
       </c>
-      <c r="R13" s="11" t="s">
-        <v>155</v>
-      </c>
       <c r="S13" s="10" t="s">
-        <v>137</v>
+        <v>136</v>
       </c>
       <c r="T13" s="29" t="s">
         <v>128</v>
       </c>
       <c r="U13" s="10" t="s">
-        <v>156</v>
+        <v>155</v>
       </c>
     </row>
     <row r="14" spans="1:21" ht="30" x14ac:dyDescent="0.25">
@@ -2229,20 +2234,20 @@
         <v>17</v>
       </c>
       <c r="B14" s="12" t="s">
+        <v>135</v>
+      </c>
+      <c r="C14" s="13" t="s">
         <v>136</v>
       </c>
-      <c r="C14" s="13" t="s">
-        <v>137</v>
-      </c>
       <c r="D14" s="14" t="s">
+        <v>163</v>
+      </c>
+      <c r="E14" s="12" t="s">
         <v>164</v>
-      </c>
-      <c r="E14" s="12" t="s">
-        <v>165</v>
       </c>
       <c r="F14" s="9"/>
       <c r="G14" s="20" t="s">
-        <v>244</v>
+        <v>240</v>
       </c>
       <c r="H14" s="21">
         <v>10</v>
@@ -2251,7 +2256,7 @@
         <v>20</v>
       </c>
       <c r="J14" s="28" t="s">
-        <v>166</v>
+        <v>165</v>
       </c>
       <c r="K14" s="23" t="s">
         <v>20</v>
@@ -2271,16 +2276,16 @@
         <v>6</v>
       </c>
       <c r="R14" s="11" t="s">
-        <v>141</v>
+        <v>140</v>
       </c>
       <c r="S14" s="10" t="s">
-        <v>145</v>
+        <v>144</v>
       </c>
       <c r="T14" s="29" t="s">
-        <v>237</v>
+        <v>233</v>
       </c>
       <c r="U14" s="10" t="s">
-        <v>147</v>
+        <v>146</v>
       </c>
     </row>
     <row r="15" spans="1:21" ht="30" x14ac:dyDescent="0.25">
@@ -2288,20 +2293,20 @@
         <v>17</v>
       </c>
       <c r="B15" s="12" t="s">
+        <v>135</v>
+      </c>
+      <c r="C15" s="13" t="s">
         <v>136</v>
       </c>
-      <c r="C15" s="13" t="s">
-        <v>137</v>
-      </c>
       <c r="D15" s="14" t="s">
-        <v>164</v>
+        <v>163</v>
       </c>
       <c r="E15" s="12" t="s">
-        <v>168</v>
+        <v>167</v>
       </c>
       <c r="F15" s="9"/>
       <c r="G15" s="17" t="s">
-        <v>245</v>
+        <v>241</v>
       </c>
       <c r="H15" s="18">
         <v>11</v>
@@ -2310,7 +2315,7 @@
         <v>19</v>
       </c>
       <c r="J15" s="27" t="s">
-        <v>246</v>
+        <v>242</v>
       </c>
       <c r="K15" s="7" t="s">
         <v>20</v>
@@ -2330,16 +2335,16 @@
         <v>6</v>
       </c>
       <c r="R15" s="11" t="s">
+        <v>168</v>
+      </c>
+      <c r="S15" s="10" t="s">
         <v>169</v>
       </c>
-      <c r="S15" s="10" t="s">
+      <c r="T15" s="29" t="s">
         <v>170</v>
       </c>
-      <c r="T15" s="29" t="s">
+      <c r="U15" s="10" t="s">
         <v>171</v>
-      </c>
-      <c r="U15" s="10" t="s">
-        <v>172</v>
       </c>
     </row>
     <row r="16" spans="1:21" ht="30" x14ac:dyDescent="0.25">
@@ -2347,20 +2352,20 @@
         <v>17</v>
       </c>
       <c r="B16" s="12" t="s">
+        <v>135</v>
+      </c>
+      <c r="C16" s="13" t="s">
         <v>136</v>
       </c>
-      <c r="C16" s="13" t="s">
-        <v>137</v>
-      </c>
       <c r="D16" s="14" t="s">
-        <v>164</v>
+        <v>163</v>
       </c>
       <c r="E16" s="12" t="s">
-        <v>168</v>
+        <v>167</v>
       </c>
       <c r="F16" s="9"/>
       <c r="G16" s="17" t="s">
-        <v>247</v>
+        <v>243</v>
       </c>
       <c r="H16" s="18">
         <v>12</v>
@@ -2369,7 +2374,7 @@
         <v>20</v>
       </c>
       <c r="J16" s="27" t="s">
-        <v>173</v>
+        <v>172</v>
       </c>
       <c r="K16" s="7" t="s">
         <v>20</v>
@@ -2389,16 +2394,16 @@
         <v>6</v>
       </c>
       <c r="R16" s="11" t="s">
-        <v>141</v>
+        <v>140</v>
       </c>
       <c r="S16" s="10" t="s">
-        <v>145</v>
+        <v>144</v>
       </c>
       <c r="T16" s="29" t="s">
-        <v>174</v>
+        <v>173</v>
       </c>
       <c r="U16" s="10" t="s">
-        <v>147</v>
+        <v>146</v>
       </c>
     </row>
     <row r="17" spans="1:21" ht="30" x14ac:dyDescent="0.25">
@@ -2406,20 +2411,20 @@
         <v>17</v>
       </c>
       <c r="B17" s="12" t="s">
+        <v>135</v>
+      </c>
+      <c r="C17" s="13" t="s">
         <v>136</v>
       </c>
-      <c r="C17" s="13" t="s">
-        <v>137</v>
-      </c>
       <c r="D17" s="14" t="s">
-        <v>164</v>
+        <v>163</v>
       </c>
       <c r="E17" s="12" t="s">
-        <v>168</v>
+        <v>167</v>
       </c>
       <c r="F17" s="9"/>
       <c r="G17" s="17" t="s">
-        <v>129</v>
+        <v>261</v>
       </c>
       <c r="H17" s="18">
         <v>13</v>
@@ -2428,7 +2433,7 @@
         <v>20</v>
       </c>
       <c r="J17" s="27" t="s">
-        <v>175</v>
+        <v>174</v>
       </c>
       <c r="K17" s="7" t="s">
         <v>20</v>
@@ -2448,16 +2453,16 @@
         <v>6</v>
       </c>
       <c r="R17" s="11" t="s">
-        <v>141</v>
+        <v>140</v>
       </c>
       <c r="S17" s="10" t="s">
-        <v>145</v>
+        <v>144</v>
       </c>
       <c r="T17" s="29" t="s">
-        <v>176</v>
+        <v>175</v>
       </c>
       <c r="U17" s="10" t="s">
-        <v>147</v>
+        <v>146</v>
       </c>
     </row>
     <row r="18" spans="1:21" ht="30" x14ac:dyDescent="0.25">
@@ -2465,22 +2470,22 @@
         <v>17</v>
       </c>
       <c r="B18" s="12" t="s">
+        <v>135</v>
+      </c>
+      <c r="C18" s="13" t="s">
         <v>136</v>
       </c>
-      <c r="C18" s="13" t="s">
-        <v>137</v>
-      </c>
       <c r="D18" s="14" t="s">
-        <v>164</v>
+        <v>163</v>
       </c>
       <c r="E18" s="12" t="s">
-        <v>131</v>
+        <v>130</v>
       </c>
       <c r="F18" s="9" t="s">
-        <v>177</v>
+        <v>176</v>
       </c>
       <c r="G18" s="17" t="s">
-        <v>248</v>
+        <v>244</v>
       </c>
       <c r="H18" s="18">
         <v>14</v>
@@ -2489,7 +2494,7 @@
         <v>19</v>
       </c>
       <c r="J18" s="27" t="s">
-        <v>178</v>
+        <v>177</v>
       </c>
       <c r="K18" s="7" t="s">
         <v>20</v>
@@ -2498,7 +2503,7 @@
         <v>5</v>
       </c>
       <c r="M18" s="8" t="s">
-        <v>54</v>
+        <v>56</v>
       </c>
       <c r="N18" s="8"/>
       <c r="O18" s="9"/>
@@ -2509,16 +2514,16 @@
         <v>6</v>
       </c>
       <c r="R18" s="11" t="s">
+        <v>168</v>
+      </c>
+      <c r="S18" s="10" t="s">
         <v>169</v>
       </c>
-      <c r="S18" s="10" t="s">
-        <v>170</v>
-      </c>
       <c r="T18" s="29" t="s">
-        <v>179</v>
+        <v>262</v>
       </c>
       <c r="U18" s="10" t="s">
-        <v>172</v>
+        <v>171</v>
       </c>
     </row>
     <row r="19" spans="1:21" ht="30" x14ac:dyDescent="0.25">
@@ -2526,22 +2531,22 @@
         <v>17</v>
       </c>
       <c r="B19" s="12" t="s">
+        <v>135</v>
+      </c>
+      <c r="C19" s="13" t="s">
         <v>136</v>
       </c>
-      <c r="C19" s="13" t="s">
-        <v>137</v>
-      </c>
       <c r="D19" s="14" t="s">
-        <v>164</v>
+        <v>163</v>
       </c>
       <c r="E19" s="12" t="s">
-        <v>131</v>
+        <v>130</v>
       </c>
       <c r="F19" s="9" t="s">
-        <v>177</v>
+        <v>176</v>
       </c>
       <c r="G19" s="17" t="s">
-        <v>249</v>
+        <v>245</v>
       </c>
       <c r="H19" s="18">
         <v>15</v>
@@ -2550,7 +2555,7 @@
         <v>20</v>
       </c>
       <c r="J19" s="27" t="s">
-        <v>180</v>
+        <v>178</v>
       </c>
       <c r="K19" s="7" t="s">
         <v>20</v>
@@ -2560,7 +2565,7 @@
       </c>
       <c r="M19" s="8"/>
       <c r="N19" s="8" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="O19" s="9"/>
       <c r="P19" s="18" t="s">
@@ -2570,16 +2575,16 @@
         <v>6</v>
       </c>
       <c r="R19" s="11" t="s">
-        <v>141</v>
+        <v>140</v>
       </c>
       <c r="S19" s="10" t="s">
-        <v>145</v>
+        <v>144</v>
       </c>
       <c r="T19" s="29" t="s">
-        <v>181</v>
+        <v>263</v>
       </c>
       <c r="U19" s="10" t="s">
-        <v>147</v>
+        <v>146</v>
       </c>
     </row>
     <row r="20" spans="1:21" ht="45" x14ac:dyDescent="0.25">
@@ -2587,22 +2592,22 @@
         <v>17</v>
       </c>
       <c r="B20" s="12" t="s">
+        <v>135</v>
+      </c>
+      <c r="C20" s="13" t="s">
         <v>136</v>
       </c>
-      <c r="C20" s="13" t="s">
-        <v>137</v>
-      </c>
       <c r="D20" s="14" t="s">
-        <v>164</v>
+        <v>163</v>
       </c>
       <c r="E20" s="12" t="s">
-        <v>131</v>
+        <v>130</v>
       </c>
       <c r="F20" s="9" t="s">
-        <v>184</v>
+        <v>181</v>
       </c>
       <c r="G20" s="17" t="s">
-        <v>250</v>
+        <v>246</v>
       </c>
       <c r="H20" s="18">
         <v>16</v>
@@ -2611,7 +2616,7 @@
         <v>20</v>
       </c>
       <c r="J20" s="27" t="s">
-        <v>251</v>
+        <v>247</v>
       </c>
       <c r="K20" s="7" t="s">
         <v>20</v>
@@ -2631,16 +2636,16 @@
         <v>6</v>
       </c>
       <c r="R20" s="11" t="s">
-        <v>141</v>
+        <v>140</v>
       </c>
       <c r="S20" s="10" t="s">
-        <v>145</v>
+        <v>144</v>
       </c>
       <c r="T20" s="29" t="s">
-        <v>182</v>
+        <v>179</v>
       </c>
       <c r="U20" s="10" t="s">
-        <v>147</v>
+        <v>146</v>
       </c>
     </row>
     <row r="21" spans="1:21" ht="30" x14ac:dyDescent="0.25">
@@ -2648,22 +2653,22 @@
         <v>17</v>
       </c>
       <c r="B21" s="12" t="s">
+        <v>135</v>
+      </c>
+      <c r="C21" s="13" t="s">
         <v>136</v>
       </c>
-      <c r="C21" s="13" t="s">
-        <v>137</v>
-      </c>
       <c r="D21" s="14" t="s">
-        <v>164</v>
+        <v>163</v>
       </c>
       <c r="E21" s="12" t="s">
-        <v>131</v>
+        <v>130</v>
       </c>
       <c r="F21" s="9" t="s">
-        <v>183</v>
+        <v>180</v>
       </c>
       <c r="G21" s="17" t="s">
-        <v>252</v>
+        <v>248</v>
       </c>
       <c r="H21" s="18">
         <v>17</v>
@@ -2672,7 +2677,7 @@
         <v>20</v>
       </c>
       <c r="J21" s="27" t="s">
-        <v>253</v>
+        <v>249</v>
       </c>
       <c r="K21" s="7" t="s">
         <v>20</v>
@@ -2692,16 +2697,16 @@
         <v>6</v>
       </c>
       <c r="R21" s="11" t="s">
-        <v>141</v>
+        <v>140</v>
       </c>
       <c r="S21" s="10" t="s">
-        <v>145</v>
+        <v>144</v>
       </c>
       <c r="T21" s="29" t="s">
-        <v>153</v>
+        <v>152</v>
       </c>
       <c r="U21" s="10" t="s">
-        <v>147</v>
+        <v>146</v>
       </c>
     </row>
     <row r="22" spans="1:21" ht="30" x14ac:dyDescent="0.25">
@@ -2709,22 +2714,22 @@
         <v>17</v>
       </c>
       <c r="B22" s="12" t="s">
+        <v>135</v>
+      </c>
+      <c r="C22" s="13" t="s">
         <v>136</v>
       </c>
-      <c r="C22" s="13" t="s">
-        <v>137</v>
-      </c>
       <c r="D22" s="14" t="s">
-        <v>164</v>
+        <v>163</v>
       </c>
       <c r="E22" s="12" t="s">
-        <v>131</v>
+        <v>130</v>
       </c>
       <c r="F22" s="9" t="s">
-        <v>183</v>
+        <v>180</v>
       </c>
       <c r="G22" s="17" t="s">
-        <v>255</v>
+        <v>251</v>
       </c>
       <c r="H22" s="18">
         <v>18</v>
@@ -2733,7 +2738,7 @@
         <v>20</v>
       </c>
       <c r="J22" s="27" t="s">
-        <v>254</v>
+        <v>250</v>
       </c>
       <c r="K22" s="7" t="s">
         <v>20</v>
@@ -2753,16 +2758,16 @@
         <v>6</v>
       </c>
       <c r="R22" s="11" t="s">
-        <v>141</v>
+        <v>140</v>
       </c>
       <c r="S22" s="10" t="s">
-        <v>145</v>
+        <v>144</v>
       </c>
       <c r="T22" s="29" t="s">
-        <v>186</v>
+        <v>183</v>
       </c>
       <c r="U22" s="10" t="s">
-        <v>147</v>
+        <v>146</v>
       </c>
     </row>
     <row r="23" spans="1:21" ht="30" x14ac:dyDescent="0.25">
@@ -2770,22 +2775,22 @@
         <v>17</v>
       </c>
       <c r="B23" s="12" t="s">
+        <v>135</v>
+      </c>
+      <c r="C23" s="13" t="s">
         <v>136</v>
       </c>
-      <c r="C23" s="13" t="s">
-        <v>137</v>
-      </c>
       <c r="D23" s="14" t="s">
-        <v>164</v>
+        <v>163</v>
       </c>
       <c r="E23" s="12" t="s">
-        <v>131</v>
+        <v>130</v>
       </c>
       <c r="F23" s="9" t="s">
-        <v>187</v>
+        <v>184</v>
       </c>
       <c r="G23" s="17" t="s">
-        <v>260</v>
+        <v>256</v>
       </c>
       <c r="H23" s="18">
         <v>19</v>
@@ -2794,7 +2799,7 @@
         <v>19</v>
       </c>
       <c r="J23" s="27" t="s">
-        <v>256</v>
+        <v>252</v>
       </c>
       <c r="K23" s="7" t="s">
         <v>20</v>
@@ -2814,16 +2819,16 @@
         <v>6</v>
       </c>
       <c r="R23" s="11" t="s">
+        <v>168</v>
+      </c>
+      <c r="S23" s="10" t="s">
         <v>169</v>
       </c>
-      <c r="S23" s="10" t="s">
-        <v>170</v>
-      </c>
       <c r="T23" s="29" t="s">
-        <v>241</v>
+        <v>237</v>
       </c>
       <c r="U23" s="10" t="s">
-        <v>172</v>
+        <v>171</v>
       </c>
     </row>
     <row r="24" spans="1:21" ht="30" x14ac:dyDescent="0.25">
@@ -2831,22 +2836,22 @@
         <v>17</v>
       </c>
       <c r="B24" s="12" t="s">
+        <v>135</v>
+      </c>
+      <c r="C24" s="13" t="s">
         <v>136</v>
       </c>
-      <c r="C24" s="13" t="s">
-        <v>137</v>
-      </c>
       <c r="D24" s="14" t="s">
-        <v>164</v>
+        <v>163</v>
       </c>
       <c r="E24" s="12" t="s">
-        <v>131</v>
+        <v>130</v>
       </c>
       <c r="F24" s="9" t="s">
-        <v>187</v>
+        <v>184</v>
       </c>
       <c r="G24" s="17" t="s">
-        <v>258</v>
+        <v>254</v>
       </c>
       <c r="H24" s="18">
         <v>20</v>
@@ -2855,7 +2860,7 @@
         <v>20</v>
       </c>
       <c r="J24" s="27" t="s">
-        <v>259</v>
+        <v>255</v>
       </c>
       <c r="K24" s="7" t="s">
         <v>20</v>
@@ -2875,16 +2880,16 @@
         <v>6</v>
       </c>
       <c r="R24" s="11" t="s">
-        <v>141</v>
+        <v>140</v>
       </c>
       <c r="S24" s="10" t="s">
-        <v>145</v>
+        <v>144</v>
       </c>
       <c r="T24" s="29" t="s">
-        <v>162</v>
+        <v>161</v>
       </c>
       <c r="U24" s="10" t="s">
-        <v>147</v>
+        <v>146</v>
       </c>
     </row>
     <row r="25" spans="1:21" ht="45" x14ac:dyDescent="0.25">
@@ -2892,22 +2897,22 @@
         <v>17</v>
       </c>
       <c r="B25" s="12" t="s">
+        <v>135</v>
+      </c>
+      <c r="C25" s="13" t="s">
         <v>136</v>
       </c>
-      <c r="C25" s="13" t="s">
-        <v>137</v>
-      </c>
       <c r="D25" s="14" t="s">
-        <v>164</v>
+        <v>163</v>
       </c>
       <c r="E25" s="12" t="s">
-        <v>131</v>
+        <v>130</v>
       </c>
       <c r="F25" s="9" t="s">
-        <v>187</v>
+        <v>184</v>
       </c>
       <c r="G25" s="17" t="s">
-        <v>164</v>
+        <v>163</v>
       </c>
       <c r="H25" s="18">
         <v>21</v>
@@ -2916,7 +2921,7 @@
         <v>20</v>
       </c>
       <c r="J25" s="27" t="s">
-        <v>211</v>
+        <v>208</v>
       </c>
       <c r="K25" s="7" t="s">
         <v>20</v>
@@ -2936,16 +2941,16 @@
         <v>6</v>
       </c>
       <c r="R25" s="11" t="s">
-        <v>141</v>
+        <v>140</v>
       </c>
       <c r="S25" s="10" t="s">
-        <v>145</v>
+        <v>144</v>
       </c>
       <c r="T25" s="29" t="s">
-        <v>163</v>
+        <v>162</v>
       </c>
       <c r="U25" s="10" t="s">
-        <v>147</v>
+        <v>146</v>
       </c>
     </row>
     <row r="26" spans="1:21" ht="30" x14ac:dyDescent="0.25">
@@ -2953,20 +2958,20 @@
         <v>17</v>
       </c>
       <c r="B26" s="12" t="s">
+        <v>135</v>
+      </c>
+      <c r="C26" s="13" t="s">
         <v>136</v>
       </c>
-      <c r="C26" s="13" t="s">
-        <v>137</v>
-      </c>
       <c r="D26" s="14" t="s">
-        <v>164</v>
+        <v>163</v>
       </c>
       <c r="E26" s="12" t="s">
-        <v>150</v>
+        <v>149</v>
       </c>
       <c r="F26" s="9"/>
       <c r="G26" s="17" t="s">
-        <v>130</v>
+        <v>129</v>
       </c>
       <c r="H26" s="18">
         <v>22</v>
@@ -2975,7 +2980,7 @@
         <v>20</v>
       </c>
       <c r="J26" s="27" t="s">
-        <v>188</v>
+        <v>185</v>
       </c>
       <c r="K26" s="7" t="s">
         <v>20</v>
@@ -2995,16 +3000,16 @@
         <v>6</v>
       </c>
       <c r="R26" s="11" t="s">
-        <v>141</v>
+        <v>140</v>
       </c>
       <c r="S26" s="10" t="s">
-        <v>145</v>
+        <v>144</v>
       </c>
       <c r="T26" s="29" t="s">
-        <v>190</v>
+        <v>187</v>
       </c>
       <c r="U26" s="10" t="s">
-        <v>147</v>
+        <v>146</v>
       </c>
     </row>
     <row r="27" spans="1:21" ht="30" x14ac:dyDescent="0.25">
@@ -3012,20 +3017,20 @@
         <v>17</v>
       </c>
       <c r="B27" s="12" t="s">
+        <v>135</v>
+      </c>
+      <c r="C27" s="13" t="s">
         <v>136</v>
       </c>
-      <c r="C27" s="13" t="s">
-        <v>137</v>
-      </c>
       <c r="D27" s="14" t="s">
-        <v>164</v>
+        <v>163</v>
       </c>
       <c r="E27" s="12" t="s">
-        <v>150</v>
+        <v>149</v>
       </c>
       <c r="F27" s="9"/>
       <c r="G27" s="17" t="s">
-        <v>210</v>
+        <v>207</v>
       </c>
       <c r="H27" s="18">
         <v>23</v>
@@ -3034,7 +3039,7 @@
         <v>20</v>
       </c>
       <c r="J27" s="27" t="s">
-        <v>189</v>
+        <v>186</v>
       </c>
       <c r="K27" s="7" t="s">
         <v>20</v>
@@ -3054,16 +3059,16 @@
         <v>6</v>
       </c>
       <c r="R27" s="11" t="s">
-        <v>141</v>
+        <v>140</v>
       </c>
       <c r="S27" s="10" t="s">
-        <v>145</v>
+        <v>144</v>
       </c>
       <c r="T27" s="29" t="s">
-        <v>191</v>
+        <v>188</v>
       </c>
       <c r="U27" s="10" t="s">
-        <v>147</v>
+        <v>146</v>
       </c>
     </row>
     <row r="28" spans="1:21" ht="30" x14ac:dyDescent="0.25">
@@ -3071,20 +3076,20 @@
         <v>17</v>
       </c>
       <c r="B28" s="12" t="s">
+        <v>135</v>
+      </c>
+      <c r="C28" s="13" t="s">
         <v>136</v>
       </c>
-      <c r="C28" s="13" t="s">
-        <v>137</v>
-      </c>
       <c r="D28" s="14" t="s">
-        <v>192</v>
+        <v>189</v>
       </c>
       <c r="E28" s="12" t="s">
-        <v>150</v>
+        <v>149</v>
       </c>
       <c r="F28" s="9"/>
       <c r="G28" s="17" t="s">
-        <v>132</v>
+        <v>131</v>
       </c>
       <c r="H28" s="18">
         <v>24</v>
@@ -3093,7 +3098,7 @@
         <v>20</v>
       </c>
       <c r="J28" s="27" t="s">
-        <v>193</v>
+        <v>190</v>
       </c>
       <c r="K28" s="7" t="s">
         <v>20</v>
@@ -3113,16 +3118,16 @@
         <v>6</v>
       </c>
       <c r="R28" s="11" t="s">
-        <v>141</v>
+        <v>140</v>
       </c>
       <c r="S28" s="10" t="s">
-        <v>145</v>
+        <v>144</v>
       </c>
       <c r="T28" s="29" t="s">
-        <v>194</v>
+        <v>191</v>
       </c>
       <c r="U28" s="10" t="s">
-        <v>147</v>
+        <v>146</v>
       </c>
     </row>
     <row r="29" spans="1:21" ht="45" x14ac:dyDescent="0.25">
@@ -3130,18 +3135,18 @@
         <v>17</v>
       </c>
       <c r="B29" s="12" t="s">
+        <v>135</v>
+      </c>
+      <c r="C29" s="13" t="s">
         <v>136</v>
       </c>
-      <c r="C29" s="13" t="s">
-        <v>137</v>
-      </c>
       <c r="D29" s="14" t="s">
-        <v>195</v>
+        <v>192</v>
       </c>
       <c r="E29" s="12"/>
       <c r="F29" s="9"/>
       <c r="G29" s="20" t="s">
-        <v>133</v>
+        <v>132</v>
       </c>
       <c r="H29" s="21">
         <v>25</v>
@@ -3150,7 +3155,7 @@
         <v>20</v>
       </c>
       <c r="J29" s="28" t="s">
-        <v>262</v>
+        <v>258</v>
       </c>
       <c r="K29" s="23" t="s">
         <v>19</v>
@@ -3163,25 +3168,25 @@
         <v>120</v>
       </c>
       <c r="O29" s="9" t="s">
-        <v>208</v>
+        <v>205</v>
       </c>
       <c r="P29" s="21" t="s">
         <v>19</v>
       </c>
       <c r="Q29" s="10" t="s">
-        <v>197</v>
+        <v>194</v>
       </c>
       <c r="R29" s="11" t="s">
-        <v>198</v>
+        <v>195</v>
       </c>
       <c r="S29" s="10" t="s">
-        <v>137</v>
+        <v>136</v>
       </c>
       <c r="T29" s="29" t="s">
-        <v>133</v>
+        <v>132</v>
       </c>
       <c r="U29" s="10" t="s">
-        <v>199</v>
+        <v>196</v>
       </c>
     </row>
     <row r="30" spans="1:21" ht="30" x14ac:dyDescent="0.25">
@@ -3189,18 +3194,18 @@
         <v>17</v>
       </c>
       <c r="B30" s="12" t="s">
+        <v>135</v>
+      </c>
+      <c r="C30" s="13" t="s">
         <v>136</v>
       </c>
-      <c r="C30" s="13" t="s">
-        <v>137</v>
-      </c>
       <c r="D30" s="14" t="s">
-        <v>195</v>
+        <v>192</v>
       </c>
       <c r="E30" s="12"/>
       <c r="F30" s="9"/>
       <c r="G30" s="17" t="s">
-        <v>134</v>
+        <v>133</v>
       </c>
       <c r="H30" s="21">
         <v>26</v>
@@ -3209,7 +3214,7 @@
         <v>20</v>
       </c>
       <c r="J30" s="28" t="s">
-        <v>261</v>
+        <v>257</v>
       </c>
       <c r="K30" s="23" t="s">
         <v>19</v>
@@ -3222,25 +3227,25 @@
         <v>120</v>
       </c>
       <c r="O30" s="9" t="s">
-        <v>208</v>
+        <v>205</v>
       </c>
       <c r="P30" s="21" t="s">
         <v>19</v>
       </c>
       <c r="Q30" s="10" t="s">
-        <v>197</v>
+        <v>194</v>
       </c>
       <c r="R30" s="11" t="s">
-        <v>198</v>
+        <v>195</v>
       </c>
       <c r="S30" s="10" t="s">
-        <v>137</v>
+        <v>136</v>
       </c>
       <c r="T30" s="29" t="s">
-        <v>134</v>
+        <v>133</v>
       </c>
       <c r="U30" s="10" t="s">
-        <v>199</v>
+        <v>196</v>
       </c>
     </row>
     <row r="31" spans="1:21" ht="30" x14ac:dyDescent="0.25">
@@ -3248,18 +3253,18 @@
         <v>17</v>
       </c>
       <c r="B31" s="12" t="s">
+        <v>135</v>
+      </c>
+      <c r="C31" s="13" t="s">
         <v>136</v>
       </c>
-      <c r="C31" s="13" t="s">
-        <v>137</v>
-      </c>
       <c r="D31" s="14" t="s">
-        <v>195</v>
+        <v>192</v>
       </c>
       <c r="E31" s="12"/>
       <c r="F31" s="9"/>
       <c r="G31" s="17" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
       <c r="H31" s="18">
         <v>27</v>
@@ -3268,7 +3273,7 @@
         <v>20</v>
       </c>
       <c r="J31" s="27" t="s">
-        <v>196</v>
+        <v>193</v>
       </c>
       <c r="K31" s="23" t="s">
         <v>19</v>
@@ -3285,19 +3290,19 @@
         <v>19</v>
       </c>
       <c r="Q31" s="10" t="s">
+        <v>153</v>
+      </c>
+      <c r="R31" s="11" t="s">
         <v>154</v>
       </c>
-      <c r="R31" s="11" t="s">
+      <c r="S31" s="10" t="s">
+        <v>136</v>
+      </c>
+      <c r="T31" s="29" t="s">
+        <v>134</v>
+      </c>
+      <c r="U31" s="10" t="s">
         <v>155</v>
-      </c>
-      <c r="S31" s="10" t="s">
-        <v>137</v>
-      </c>
-      <c r="T31" s="29" t="s">
-        <v>135</v>
-      </c>
-      <c r="U31" s="10" t="s">
-        <v>156</v>
       </c>
     </row>
     <row r="32" spans="1:21" ht="60" x14ac:dyDescent="0.25">
@@ -3305,18 +3310,18 @@
         <v>17</v>
       </c>
       <c r="B32" s="12" t="s">
+        <v>135</v>
+      </c>
+      <c r="C32" s="13" t="s">
         <v>136</v>
       </c>
-      <c r="C32" s="13" t="s">
-        <v>137</v>
-      </c>
       <c r="D32" s="14" t="s">
-        <v>195</v>
+        <v>192</v>
       </c>
       <c r="E32" s="12"/>
       <c r="F32" s="9"/>
       <c r="G32" s="17" t="s">
-        <v>200</v>
+        <v>197</v>
       </c>
       <c r="H32" s="18">
         <v>28</v>
@@ -3325,7 +3330,7 @@
         <v>20</v>
       </c>
       <c r="J32" s="27" t="s">
-        <v>202</v>
+        <v>199</v>
       </c>
       <c r="K32" s="7" t="s">
         <v>19</v>
@@ -3338,25 +3343,25 @@
         <v>120</v>
       </c>
       <c r="O32" s="9" t="s">
-        <v>214</v>
+        <v>210</v>
       </c>
       <c r="P32" s="18" t="s">
         <v>19</v>
       </c>
       <c r="Q32" s="10" t="s">
+        <v>153</v>
+      </c>
+      <c r="R32" s="11" t="s">
         <v>154</v>
       </c>
-      <c r="R32" s="11" t="s">
+      <c r="S32" s="10" t="s">
+        <v>136</v>
+      </c>
+      <c r="T32" s="29" t="s">
+        <v>197</v>
+      </c>
+      <c r="U32" s="10" t="s">
         <v>155</v>
-      </c>
-      <c r="S32" s="10" t="s">
-        <v>137</v>
-      </c>
-      <c r="T32" s="29" t="s">
-        <v>200</v>
-      </c>
-      <c r="U32" s="10" t="s">
-        <v>156</v>
       </c>
     </row>
     <row r="33" spans="1:21" ht="45" x14ac:dyDescent="0.25">
@@ -3364,18 +3369,18 @@
         <v>17</v>
       </c>
       <c r="B33" s="12" t="s">
+        <v>135</v>
+      </c>
+      <c r="C33" s="13" t="s">
         <v>136</v>
       </c>
-      <c r="C33" s="13" t="s">
-        <v>137</v>
-      </c>
       <c r="D33" s="14" t="s">
-        <v>195</v>
+        <v>192</v>
       </c>
       <c r="E33" s="12"/>
       <c r="F33" s="9"/>
       <c r="G33" s="17" t="s">
-        <v>201</v>
+        <v>198</v>
       </c>
       <c r="H33" s="18">
         <v>29</v>
@@ -3384,7 +3389,7 @@
         <v>20</v>
       </c>
       <c r="J33" s="27" t="s">
-        <v>263</v>
+        <v>259</v>
       </c>
       <c r="K33" s="7" t="s">
         <v>19</v>
@@ -3397,25 +3402,25 @@
         <v>120</v>
       </c>
       <c r="O33" s="9" t="s">
-        <v>208</v>
-      </c>
-      <c r="P33" s="18" t="s">
-        <v>19</v>
+        <v>205</v>
+      </c>
+      <c r="P33" s="33" t="s">
+        <v>20</v>
       </c>
       <c r="Q33" s="10" t="s">
+        <v>153</v>
+      </c>
+      <c r="R33" s="11" t="s">
         <v>154</v>
       </c>
-      <c r="R33" s="11" t="s">
+      <c r="S33" s="10" t="s">
+        <v>136</v>
+      </c>
+      <c r="T33" s="29" t="s">
+        <v>198</v>
+      </c>
+      <c r="U33" s="10" t="s">
         <v>155</v>
-      </c>
-      <c r="S33" s="10" t="s">
-        <v>137</v>
-      </c>
-      <c r="T33" s="29" t="s">
-        <v>201</v>
-      </c>
-      <c r="U33" s="10" t="s">
-        <v>156</v>
       </c>
     </row>
     <row r="34" spans="1:21" ht="15.75" x14ac:dyDescent="0.25">
@@ -3423,13 +3428,13 @@
         <v>17</v>
       </c>
       <c r="B34" s="12" t="s">
+        <v>135</v>
+      </c>
+      <c r="C34" s="13" t="s">
         <v>136</v>
       </c>
-      <c r="C34" s="13" t="s">
-        <v>137</v>
-      </c>
       <c r="D34" s="31" t="s">
-        <v>203</v>
+        <v>200</v>
       </c>
       <c r="E34" s="12"/>
       <c r="F34" s="9"/>
@@ -3443,7 +3448,7 @@
         <v>20</v>
       </c>
       <c r="J34" s="27" t="s">
-        <v>205</v>
+        <v>202</v>
       </c>
       <c r="K34" s="7" t="s">
         <v>20</v>
@@ -3468,18 +3473,18 @@
         <v>17</v>
       </c>
       <c r="B35" s="12" t="s">
+        <v>135</v>
+      </c>
+      <c r="C35" s="13" t="s">
         <v>136</v>
       </c>
-      <c r="C35" s="13" t="s">
-        <v>137</v>
-      </c>
       <c r="D35" s="31" t="s">
-        <v>203</v>
+        <v>200</v>
       </c>
       <c r="E35" s="12"/>
       <c r="F35" s="9"/>
       <c r="G35" s="17" t="s">
-        <v>204</v>
+        <v>201</v>
       </c>
       <c r="H35" s="18">
         <v>31</v>
@@ -3488,7 +3493,7 @@
         <v>20</v>
       </c>
       <c r="J35" s="27" t="s">
-        <v>206</v>
+        <v>203</v>
       </c>
       <c r="K35" s="7" t="s">
         <v>20</v>
@@ -3508,35 +3513,35 @@
         <v>6</v>
       </c>
       <c r="R35" s="11" t="s">
-        <v>141</v>
+        <v>140</v>
       </c>
       <c r="S35" s="10" t="s">
-        <v>145</v>
+        <v>144</v>
       </c>
       <c r="T35" s="29" t="s">
-        <v>185</v>
+        <v>182</v>
       </c>
       <c r="U35" s="10" t="s">
-        <v>147</v>
-      </c>
-    </row>
-    <row r="36" spans="1:21" ht="30" x14ac:dyDescent="0.25">
+        <v>146</v>
+      </c>
+    </row>
+    <row r="36" spans="1:21" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A36" s="4" t="s">
         <v>17</v>
       </c>
       <c r="B36" s="12" t="s">
+        <v>135</v>
+      </c>
+      <c r="C36" s="13" t="s">
         <v>136</v>
       </c>
-      <c r="C36" s="13" t="s">
-        <v>137</v>
-      </c>
       <c r="D36" s="31" t="s">
-        <v>203</v>
+        <v>200</v>
       </c>
       <c r="E36" s="12"/>
       <c r="F36" s="9"/>
       <c r="G36" s="17" t="s">
-        <v>213</v>
+        <v>209</v>
       </c>
       <c r="H36" s="18">
         <v>32</v>
@@ -3545,7 +3550,7 @@
         <v>20</v>
       </c>
       <c r="J36" s="27" t="s">
-        <v>212</v>
+        <v>264</v>
       </c>
       <c r="K36" s="7" t="s">
         <v>20</v>
@@ -3565,16 +3570,16 @@
         <v>6</v>
       </c>
       <c r="R36" s="11" t="s">
-        <v>141</v>
+        <v>140</v>
       </c>
       <c r="S36" s="10" t="s">
-        <v>145</v>
+        <v>144</v>
       </c>
       <c r="T36" s="29" t="s">
-        <v>207</v>
+        <v>204</v>
       </c>
       <c r="U36" s="10" t="s">
-        <v>147</v>
+        <v>146</v>
       </c>
     </row>
     <row r="37" spans="1:21" ht="15.75" x14ac:dyDescent="0.25">
@@ -4698,7 +4703,14 @@
     <row r="282" hidden="1" x14ac:dyDescent="0.25"/>
     <row r="283" hidden="1" x14ac:dyDescent="0.25"/>
   </sheetData>
+  <autoFilter ref="A2:U36"/>
   <mergeCells count="20">
+    <mergeCell ref="P1:P2"/>
+    <mergeCell ref="U1:U2"/>
+    <mergeCell ref="T1:T2"/>
+    <mergeCell ref="S1:S2"/>
+    <mergeCell ref="R1:R2"/>
+    <mergeCell ref="Q1:Q2"/>
     <mergeCell ref="I1:I2"/>
     <mergeCell ref="H1:H2"/>
     <mergeCell ref="O1:O2"/>
@@ -4713,12 +4725,6 @@
     <mergeCell ref="D1:D2"/>
     <mergeCell ref="C1:C2"/>
     <mergeCell ref="F1:F2"/>
-    <mergeCell ref="P1:P2"/>
-    <mergeCell ref="U1:U2"/>
-    <mergeCell ref="T1:T2"/>
-    <mergeCell ref="S1:S2"/>
-    <mergeCell ref="R1:R2"/>
-    <mergeCell ref="Q1:Q2"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
@@ -4780,193 +4786,193 @@
   <sheetData>
     <row r="2" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A2" s="34" t="s">
+        <v>211</v>
+      </c>
+      <c r="B2" s="34" t="s">
+        <v>212</v>
+      </c>
+      <c r="C2" s="34" t="s">
         <v>215</v>
       </c>
-      <c r="B2" s="34" t="s">
-        <v>216</v>
-      </c>
-      <c r="C2" s="34" t="s">
-        <v>219</v>
-      </c>
       <c r="D2" s="34" t="s">
-        <v>217</v>
+        <v>213</v>
       </c>
       <c r="E2" s="34" t="s">
-        <v>218</v>
+        <v>214</v>
       </c>
     </row>
     <row r="3" spans="1:5" ht="45" x14ac:dyDescent="0.25">
       <c r="A3" s="35" t="s">
+        <v>156</v>
+      </c>
+      <c r="B3" s="36" t="s">
         <v>157</v>
-      </c>
-      <c r="B3" s="36" t="s">
-        <v>158</v>
       </c>
       <c r="C3" s="42"/>
       <c r="D3" s="37" t="s">
-        <v>223</v>
+        <v>219</v>
       </c>
       <c r="E3" s="38" t="s">
-        <v>220</v>
+        <v>216</v>
       </c>
     </row>
     <row r="4" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A4" s="35" t="s">
+        <v>156</v>
+      </c>
+      <c r="B4" s="36" t="s">
         <v>157</v>
-      </c>
-      <c r="B4" s="36" t="s">
-        <v>158</v>
       </c>
       <c r="C4" s="42"/>
       <c r="D4" s="37" t="s">
-        <v>221</v>
+        <v>217</v>
       </c>
       <c r="E4" s="38"/>
     </row>
     <row r="5" spans="1:5" ht="45" x14ac:dyDescent="0.25">
       <c r="A5" s="35" t="s">
-        <v>157</v>
+        <v>156</v>
       </c>
       <c r="B5" s="36" t="s">
-        <v>159</v>
+        <v>158</v>
       </c>
       <c r="C5" s="42"/>
       <c r="D5" s="37" t="s">
-        <v>222</v>
+        <v>218</v>
       </c>
       <c r="E5" s="38" t="s">
-        <v>224</v>
+        <v>220</v>
       </c>
     </row>
     <row r="6" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A6" s="35" t="s">
+        <v>163</v>
+      </c>
+      <c r="B6" s="36" t="s">
         <v>164</v>
-      </c>
-      <c r="B6" s="36" t="s">
-        <v>165</v>
       </c>
       <c r="C6" s="42"/>
       <c r="D6" s="37" t="s">
-        <v>225</v>
+        <v>221</v>
       </c>
       <c r="E6" s="38"/>
     </row>
     <row r="7" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A7" s="35" t="s">
-        <v>164</v>
+        <v>163</v>
       </c>
       <c r="B7" s="36" t="s">
-        <v>168</v>
+        <v>167</v>
       </c>
       <c r="C7" s="42"/>
       <c r="D7" s="37" t="s">
-        <v>226</v>
+        <v>222</v>
       </c>
       <c r="E7" s="38"/>
     </row>
     <row r="8" spans="1:5" ht="30" x14ac:dyDescent="0.25">
       <c r="A8" s="35" t="s">
-        <v>164</v>
+        <v>163</v>
       </c>
       <c r="B8" s="36" t="s">
-        <v>168</v>
+        <v>167</v>
       </c>
       <c r="C8" s="42"/>
       <c r="D8" s="37" t="s">
-        <v>227</v>
+        <v>223</v>
       </c>
       <c r="E8" s="38"/>
     </row>
     <row r="9" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A9" s="35" t="s">
-        <v>164</v>
+        <v>163</v>
       </c>
       <c r="B9" s="36" t="s">
-        <v>131</v>
+        <v>130</v>
       </c>
       <c r="C9" s="42" t="s">
-        <v>177</v>
+        <v>176</v>
       </c>
       <c r="D9" s="37" t="s">
-        <v>228</v>
+        <v>224</v>
       </c>
       <c r="E9" s="38"/>
     </row>
     <row r="10" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A10" s="35" t="s">
-        <v>164</v>
+        <v>163</v>
       </c>
       <c r="B10" s="36" t="s">
-        <v>131</v>
+        <v>130</v>
       </c>
       <c r="C10" s="42" t="s">
-        <v>177</v>
+        <v>176</v>
       </c>
       <c r="D10" s="37" t="s">
-        <v>229</v>
+        <v>225</v>
       </c>
       <c r="E10" s="38"/>
     </row>
     <row r="11" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A11" s="35" t="s">
-        <v>164</v>
+        <v>163</v>
       </c>
       <c r="B11" s="36" t="s">
-        <v>131</v>
+        <v>130</v>
       </c>
       <c r="C11" s="42" t="s">
-        <v>184</v>
+        <v>181</v>
       </c>
       <c r="D11" s="37" t="s">
-        <v>230</v>
+        <v>226</v>
       </c>
       <c r="E11" s="38"/>
     </row>
     <row r="12" spans="1:5" ht="30" x14ac:dyDescent="0.25">
       <c r="A12" s="35" t="s">
-        <v>164</v>
+        <v>163</v>
       </c>
       <c r="B12" s="36" t="s">
-        <v>131</v>
+        <v>130</v>
       </c>
       <c r="C12" s="42" t="s">
-        <v>187</v>
+        <v>184</v>
       </c>
       <c r="D12" s="37" t="s">
-        <v>231</v>
+        <v>227</v>
       </c>
       <c r="E12" s="38"/>
     </row>
     <row r="13" spans="1:5" ht="30" x14ac:dyDescent="0.25">
       <c r="A13" s="39" t="s">
-        <v>232</v>
+        <v>228</v>
       </c>
       <c r="B13" s="39"/>
       <c r="C13" s="39"/>
       <c r="D13" s="40" t="s">
-        <v>233</v>
+        <v>229</v>
       </c>
       <c r="E13" s="41"/>
     </row>
     <row r="14" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A14" s="39" t="s">
-        <v>232</v>
+        <v>228</v>
       </c>
       <c r="B14" s="39"/>
       <c r="C14" s="39"/>
       <c r="D14" s="40" t="s">
-        <v>234</v>
+        <v>230</v>
       </c>
       <c r="E14" s="41"/>
     </row>
     <row r="15" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A15" s="39" t="s">
-        <v>232</v>
+        <v>228</v>
       </c>
       <c r="B15" s="39"/>
       <c r="C15" s="39"/>
       <c r="D15" s="40" t="s">
-        <v>235</v>
+        <v>231</v>
       </c>
       <c r="E15" s="41"/>
     </row>

</xml_diff>